<commit_message>
Atualizações do 3 torneio(correção artilharia)
</commit_message>
<xml_diff>
--- a/Dados/Dados_Torneio.xlsx
+++ b/Dados/Dados_Torneio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Site\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6418A5-04F0-4E1A-9CDC-A877A824D571}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B618EE-739E-43AA-9B6F-6821741DA667}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1430,19 +1430,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1460,22 +1463,19 @@
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2058,8 +2058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2273,91 +2273,91 @@
     </row>
     <row r="14" spans="1:9" ht="24" customHeight="1">
       <c r="A14" s="17" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C14" s="17">
-        <v>2</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>34</v>
+        <v>3</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>312</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="24" customHeight="1">
       <c r="A15" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>69</v>
+        <v>25</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>319</v>
       </c>
       <c r="C15" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="24" customHeight="1">
       <c r="A16" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C16" s="17">
         <v>2</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="24" customHeight="1">
       <c r="A17" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>315</v>
+        <v>21</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="C17" s="17">
         <v>2</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>311</v>
+      <c r="D17" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="24" customHeight="1">
       <c r="A18" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" s="17">
-        <v>3</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>312</v>
+        <v>2</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="24" customHeight="1">
       <c r="A19" s="17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C19" s="17">
-        <v>3</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>118</v>
+        <v>2</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>311</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -4763,8 +4763,8 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <sortState ref="B3:D48">
-    <sortCondition descending="1" ref="C3:C48"/>
+  <sortState ref="A3:D46">
+    <sortCondition descending="1" ref="C3:C46"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
@@ -7409,10 +7409,10 @@
       <c r="E1" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="55"/>
+      <c r="G1" s="45"/>
       <c r="H1" s="35" t="s">
         <v>311</v>
       </c>
@@ -7433,10 +7433,10 @@
       <c r="E2" s="36">
         <v>8</v>
       </c>
-      <c r="F2" s="56">
+      <c r="F2" s="46">
         <v>16</v>
       </c>
-      <c r="G2" s="56"/>
+      <c r="G2" s="46"/>
       <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1">
@@ -7465,10 +7465,10 @@
       <c r="E4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="57"/>
+      <c r="G4" s="47"/>
       <c r="H4" s="33" t="s">
         <v>81</v>
       </c>
@@ -7489,10 +7489,10 @@
       <c r="E5" s="23">
         <v>17</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="48">
         <v>14</v>
       </c>
-      <c r="G5" s="58"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:8" ht="24" customHeight="1">
@@ -7521,10 +7521,10 @@
       <c r="E7" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="59"/>
+      <c r="G7" s="49"/>
       <c r="H7" s="40" t="s">
         <v>314</v>
       </c>
@@ -7545,10 +7545,10 @@
       <c r="E8" s="41">
         <v>24</v>
       </c>
-      <c r="F8" s="54">
+      <c r="F8" s="44">
         <v>9</v>
       </c>
-      <c r="G8" s="54"/>
+      <c r="G8" s="44"/>
       <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" ht="24" customHeight="1">
@@ -7577,10 +7577,10 @@
       <c r="E10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="49" t="s">
+      <c r="F10" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="49"/>
+      <c r="G10" s="50"/>
       <c r="H10" s="5" t="s">
         <v>36</v>
       </c>
@@ -7601,10 +7601,10 @@
       <c r="E11" s="24">
         <v>17</v>
       </c>
-      <c r="F11" s="50">
+      <c r="F11" s="51">
         <v>23</v>
       </c>
-      <c r="G11" s="50"/>
+      <c r="G11" s="51"/>
       <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" ht="24" customHeight="1">
@@ -7633,10 +7633,10 @@
       <c r="E13" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="51" t="s">
+      <c r="F13" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="51"/>
+      <c r="G13" s="52"/>
       <c r="H13" s="37" t="s">
         <v>313</v>
       </c>
@@ -7657,10 +7657,10 @@
       <c r="E14" s="38">
         <v>12</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="53">
         <v>13</v>
       </c>
-      <c r="G14" s="52"/>
+      <c r="G14" s="53"/>
       <c r="H14" s="39"/>
     </row>
     <row r="15" spans="1:8" ht="24" customHeight="1">
@@ -7689,10 +7689,10 @@
       <c r="E16" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="53" t="s">
+      <c r="F16" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="53"/>
+      <c r="G16" s="54"/>
       <c r="H16" s="6" t="s">
         <v>103</v>
       </c>
@@ -7713,10 +7713,10 @@
       <c r="E17" s="25">
         <v>6</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="55">
         <v>8</v>
       </c>
-      <c r="G17" s="44"/>
+      <c r="G17" s="55"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="24" customHeight="1">
@@ -7745,10 +7745,10 @@
       <c r="E19" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="45" t="s">
+      <c r="F19" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="45"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="26" t="s">
         <v>104</v>
       </c>
@@ -7769,10 +7769,10 @@
       <c r="E20" s="27">
         <v>8</v>
       </c>
-      <c r="F20" s="46">
+      <c r="F20" s="57">
         <v>11</v>
       </c>
-      <c r="G20" s="46"/>
+      <c r="G20" s="57"/>
       <c r="H20" s="32"/>
     </row>
     <row r="21" spans="1:8" ht="24" customHeight="1">
@@ -7801,10 +7801,10 @@
       <c r="E22" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="47" t="s">
+      <c r="F22" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="47"/>
+      <c r="G22" s="58"/>
       <c r="H22" s="28" t="s">
         <v>35</v>
       </c>
@@ -7825,10 +7825,10 @@
       <c r="E23" s="29">
         <v>15</v>
       </c>
-      <c r="F23" s="48">
+      <c r="F23" s="59">
         <v>11</v>
       </c>
-      <c r="G23" s="48"/>
+      <c r="G23" s="59"/>
       <c r="H23" s="32"/>
     </row>
     <row r="30" spans="1:8">
@@ -7839,22 +7839,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Correção de KDA dos clubes(Arsenal e Man. City) e placar de um jogo da fase grupos e atualização da pontuação dos torneios
</commit_message>
<xml_diff>
--- a/Dados/Dados_Torneio.xlsx
+++ b/Dados/Dados_Torneio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Site\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B618EE-739E-43AA-9B6F-6821741DA667}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05FA549-41C8-4F80-A633-160A4B9D4E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Artilharia" sheetId="1" r:id="rId1"/>
@@ -1016,10 +1016,10 @@
     <t>Man. City</t>
   </si>
   <si>
-    <t xml:space="preserve">3 x 0 </t>
-  </si>
-  <si>
     <t>1 x 1(6x5)</t>
+  </si>
+  <si>
+    <t>4 x 0</t>
   </si>
 </sst>
 </file>
@@ -1430,22 +1430,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1463,19 +1460,22 @@
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2058,8 +2058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView showWhiteSpace="0" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2236,7 +2236,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>43</v>
+        <v>313</v>
       </c>
       <c r="F11" s="1"/>
       <c r="I11" s="2"/>
@@ -5023,8 +5023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F94794-2326-4125-84B0-613C359A2BCD}">
   <dimension ref="L1:T75"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView topLeftCell="K28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5956,7 +5956,7 @@
   <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7125,7 +7125,7 @@
         <v>311</v>
       </c>
       <c r="P35" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Q35" s="10" t="s">
         <v>103</v>
@@ -7270,7 +7270,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G39" s="11">
         <v>0</v>
@@ -7282,7 +7282,7 @@
         <v>326</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M39" s="10" t="s">
         <v>36</v>
@@ -7343,7 +7343,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H41" s="12">
         <v>1</v>
@@ -7382,8 +7382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042CEF4B-51C6-46DD-9493-7BEA1AB5B2B1}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="69" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7409,10 +7409,10 @@
       <c r="E1" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="45"/>
+      <c r="G1" s="55"/>
       <c r="H1" s="35" t="s">
         <v>311</v>
       </c>
@@ -7433,10 +7433,10 @@
       <c r="E2" s="36">
         <v>8</v>
       </c>
-      <c r="F2" s="46">
+      <c r="F2" s="56">
         <v>16</v>
       </c>
-      <c r="G2" s="46"/>
+      <c r="G2" s="56"/>
       <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1">
@@ -7465,10 +7465,10 @@
       <c r="E4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="47" t="s">
+      <c r="F4" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="47"/>
+      <c r="G4" s="57"/>
       <c r="H4" s="33" t="s">
         <v>81</v>
       </c>
@@ -7489,10 +7489,10 @@
       <c r="E5" s="23">
         <v>17</v>
       </c>
-      <c r="F5" s="48">
+      <c r="F5" s="58">
         <v>14</v>
       </c>
-      <c r="G5" s="48"/>
+      <c r="G5" s="58"/>
       <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:8" ht="24" customHeight="1">
@@ -7521,10 +7521,10 @@
       <c r="E7" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="49"/>
+      <c r="G7" s="59"/>
       <c r="H7" s="40" t="s">
         <v>314</v>
       </c>
@@ -7543,12 +7543,12 @@
         <v>1</v>
       </c>
       <c r="E8" s="41">
-        <v>24</v>
-      </c>
-      <c r="F8" s="44">
+        <v>25</v>
+      </c>
+      <c r="F8" s="54">
         <v>9</v>
       </c>
-      <c r="G8" s="44"/>
+      <c r="G8" s="54"/>
       <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" ht="24" customHeight="1">
@@ -7577,10 +7577,10 @@
       <c r="E10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="50" t="s">
+      <c r="F10" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="50"/>
+      <c r="G10" s="49"/>
       <c r="H10" s="5" t="s">
         <v>36</v>
       </c>
@@ -7601,10 +7601,10 @@
       <c r="E11" s="24">
         <v>17</v>
       </c>
-      <c r="F11" s="51">
-        <v>23</v>
-      </c>
-      <c r="G11" s="51"/>
+      <c r="F11" s="50">
+        <v>24</v>
+      </c>
+      <c r="G11" s="50"/>
       <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" ht="24" customHeight="1">
@@ -7633,10 +7633,10 @@
       <c r="E13" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="52" t="s">
+      <c r="F13" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="52"/>
+      <c r="G13" s="51"/>
       <c r="H13" s="37" t="s">
         <v>313</v>
       </c>
@@ -7657,10 +7657,10 @@
       <c r="E14" s="38">
         <v>12</v>
       </c>
-      <c r="F14" s="53">
+      <c r="F14" s="52">
         <v>13</v>
       </c>
-      <c r="G14" s="53"/>
+      <c r="G14" s="52"/>
       <c r="H14" s="39"/>
     </row>
     <row r="15" spans="1:8" ht="24" customHeight="1">
@@ -7689,10 +7689,10 @@
       <c r="E16" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="54" t="s">
+      <c r="F16" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="54"/>
+      <c r="G16" s="53"/>
       <c r="H16" s="6" t="s">
         <v>103</v>
       </c>
@@ -7713,10 +7713,10 @@
       <c r="E17" s="25">
         <v>6</v>
       </c>
-      <c r="F17" s="55">
+      <c r="F17" s="44">
         <v>8</v>
       </c>
-      <c r="G17" s="55"/>
+      <c r="G17" s="44"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="24" customHeight="1">
@@ -7745,10 +7745,10 @@
       <c r="E19" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="56" t="s">
+      <c r="F19" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="56"/>
+      <c r="G19" s="45"/>
       <c r="H19" s="26" t="s">
         <v>104</v>
       </c>
@@ -7769,10 +7769,10 @@
       <c r="E20" s="27">
         <v>8</v>
       </c>
-      <c r="F20" s="57">
+      <c r="F20" s="46">
         <v>11</v>
       </c>
-      <c r="G20" s="57"/>
+      <c r="G20" s="46"/>
       <c r="H20" s="32"/>
     </row>
     <row r="21" spans="1:8" ht="24" customHeight="1">
@@ -7801,10 +7801,10 @@
       <c r="E22" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="58" t="s">
+      <c r="F22" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="58"/>
+      <c r="G22" s="47"/>
       <c r="H22" s="28" t="s">
         <v>35</v>
       </c>
@@ -7825,10 +7825,10 @@
       <c r="E23" s="29">
         <v>15</v>
       </c>
-      <c r="F23" s="59">
+      <c r="F23" s="48">
         <v>11</v>
       </c>
-      <c r="G23" s="59"/>
+      <c r="G23" s="48"/>
       <c r="H23" s="32"/>
     </row>
     <row r="30" spans="1:8">
@@ -7839,22 +7839,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F16:G16"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Correção de KDA em geral e adição de botão para download do banco de dados(.xlxs)
</commit_message>
<xml_diff>
--- a/Dados/Dados_Torneio.xlsx
+++ b/Dados/Dados_Torneio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Site\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05FA549-41C8-4F80-A633-160A4B9D4E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FE59D3-A327-4EA4-9D9A-67ADC01BA8D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1430,19 +1430,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1460,22 +1463,19 @@
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5955,8 +5955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D960C3E-E2A1-4F5E-9B7E-CC59E9774824}">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7380,10 +7380,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042CEF4B-51C6-46DD-9493-7BEA1AB5B2B1}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="69" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7409,10 +7409,10 @@
       <c r="E1" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="55"/>
+      <c r="G1" s="45"/>
       <c r="H1" s="35" t="s">
         <v>311</v>
       </c>
@@ -7433,10 +7433,10 @@
       <c r="E2" s="36">
         <v>8</v>
       </c>
-      <c r="F2" s="56">
+      <c r="F2" s="46">
         <v>16</v>
       </c>
-      <c r="G2" s="56"/>
+      <c r="G2" s="46"/>
       <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1">
@@ -7465,10 +7465,10 @@
       <c r="E4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="57"/>
+      <c r="G4" s="47"/>
       <c r="H4" s="33" t="s">
         <v>81</v>
       </c>
@@ -7478,21 +7478,21 @@
         <v>14</v>
       </c>
       <c r="B5" s="23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="23">
         <v>5</v>
       </c>
       <c r="D5" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="23">
         <v>17</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="48">
         <v>14</v>
       </c>
-      <c r="G5" s="58"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:8" ht="24" customHeight="1">
@@ -7521,10 +7521,10 @@
       <c r="E7" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="59"/>
+      <c r="G7" s="49"/>
       <c r="H7" s="40" t="s">
         <v>314</v>
       </c>
@@ -7534,7 +7534,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="41">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C8" s="41">
         <v>3</v>
@@ -7545,10 +7545,10 @@
       <c r="E8" s="41">
         <v>25</v>
       </c>
-      <c r="F8" s="54">
+      <c r="F8" s="44">
         <v>9</v>
       </c>
-      <c r="G8" s="54"/>
+      <c r="G8" s="44"/>
       <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" ht="24" customHeight="1">
@@ -7577,10 +7577,10 @@
       <c r="E10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="49" t="s">
+      <c r="F10" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="49"/>
+      <c r="G10" s="50"/>
       <c r="H10" s="5" t="s">
         <v>36</v>
       </c>
@@ -7596,15 +7596,15 @@
         <v>3</v>
       </c>
       <c r="D11" s="24">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E11" s="24">
         <v>17</v>
       </c>
-      <c r="F11" s="50">
+      <c r="F11" s="51">
         <v>24</v>
       </c>
-      <c r="G11" s="50"/>
+      <c r="G11" s="51"/>
       <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" ht="24" customHeight="1">
@@ -7633,10 +7633,10 @@
       <c r="E13" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="51" t="s">
+      <c r="F13" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="51"/>
+      <c r="G13" s="52"/>
       <c r="H13" s="37" t="s">
         <v>313</v>
       </c>
@@ -7657,10 +7657,10 @@
       <c r="E14" s="38">
         <v>12</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="53">
         <v>13</v>
       </c>
-      <c r="G14" s="52"/>
+      <c r="G14" s="53"/>
       <c r="H14" s="39"/>
     </row>
     <row r="15" spans="1:8" ht="24" customHeight="1">
@@ -7689,10 +7689,10 @@
       <c r="E16" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="53" t="s">
+      <c r="F16" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="53"/>
+      <c r="G16" s="54"/>
       <c r="H16" s="6" t="s">
         <v>103</v>
       </c>
@@ -7713,10 +7713,10 @@
       <c r="E17" s="25">
         <v>6</v>
       </c>
-      <c r="F17" s="44">
-        <v>8</v>
-      </c>
-      <c r="G17" s="44"/>
+      <c r="F17" s="55">
+        <v>9</v>
+      </c>
+      <c r="G17" s="55"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="24" customHeight="1">
@@ -7745,10 +7745,10 @@
       <c r="E19" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="45" t="s">
+      <c r="F19" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="45"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="26" t="s">
         <v>104</v>
       </c>
@@ -7769,10 +7769,10 @@
       <c r="E20" s="27">
         <v>8</v>
       </c>
-      <c r="F20" s="46">
+      <c r="F20" s="57">
         <v>11</v>
       </c>
-      <c r="G20" s="46"/>
+      <c r="G20" s="57"/>
       <c r="H20" s="32"/>
     </row>
     <row r="21" spans="1:8" ht="24" customHeight="1">
@@ -7801,61 +7801,68 @@
       <c r="E22" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="47" t="s">
+      <c r="F22" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="47"/>
+      <c r="G22" s="58"/>
       <c r="H22" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="24" customHeight="1">
       <c r="A23" s="29">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B23" s="29">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" s="29">
         <v>3</v>
       </c>
       <c r="D23" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E23" s="29">
         <v>15</v>
       </c>
-      <c r="F23" s="48">
-        <v>11</v>
-      </c>
-      <c r="G23" s="48"/>
+      <c r="F23" s="59">
+        <v>12</v>
+      </c>
+      <c r="G23" s="59"/>
       <c r="H23" s="32"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="G27" s="2"/>
     </row>
     <row r="30" spans="1:8">
       <c r="G30" s="2"/>
     </row>
-    <row r="37" spans="8:8">
+    <row r="37" spans="7:8">
       <c r="H37" s="2"/>
+    </row>
+    <row r="45" spans="7:8">
+      <c r="G45" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalização do Arsenal. Integração do Madrid.
</commit_message>
<xml_diff>
--- a/Dados/Dados_Torneio.xlsx
+++ b/Dados/Dados_Torneio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Site\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91C1440-2E47-4EB5-A75D-6A244327B942}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC306D97-E3B2-495B-9E13-C3E85AA5B0DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1487,19 +1487,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1517,22 +1520,19 @@
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -8108,7 +8108,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="69" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="A19" sqref="A19:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8134,10 +8134,10 @@
       <c r="E1" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="55"/>
+      <c r="G1" s="45"/>
       <c r="H1" s="35" t="s">
         <v>311</v>
       </c>
@@ -8158,10 +8158,10 @@
       <c r="E2" s="36">
         <v>17</v>
       </c>
-      <c r="F2" s="56">
+      <c r="F2" s="46">
         <v>22</v>
       </c>
-      <c r="G2" s="56"/>
+      <c r="G2" s="46"/>
       <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1">
@@ -8190,10 +8190,10 @@
       <c r="E4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="57"/>
+      <c r="G4" s="47"/>
       <c r="H4" s="33" t="s">
         <v>81</v>
       </c>
@@ -8214,10 +8214,10 @@
       <c r="E5" s="23">
         <v>22</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="48">
         <v>15</v>
       </c>
-      <c r="G5" s="58"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:8" ht="24" customHeight="1">
@@ -8246,10 +8246,10 @@
       <c r="E7" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="59"/>
+      <c r="G7" s="49"/>
       <c r="H7" s="40" t="s">
         <v>314</v>
       </c>
@@ -8270,10 +8270,10 @@
       <c r="E8" s="41">
         <v>36</v>
       </c>
-      <c r="F8" s="54">
+      <c r="F8" s="44">
         <v>17</v>
       </c>
-      <c r="G8" s="54"/>
+      <c r="G8" s="44"/>
       <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" ht="24" customHeight="1">
@@ -8302,10 +8302,10 @@
       <c r="E10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="49" t="s">
+      <c r="F10" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="49"/>
+      <c r="G10" s="50"/>
       <c r="H10" s="5" t="s">
         <v>36</v>
       </c>
@@ -8326,10 +8326,10 @@
       <c r="E11" s="24">
         <v>18</v>
       </c>
-      <c r="F11" s="50">
+      <c r="F11" s="51">
         <v>30</v>
       </c>
-      <c r="G11" s="50"/>
+      <c r="G11" s="51"/>
       <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" ht="24" customHeight="1">
@@ -8358,10 +8358,10 @@
       <c r="E13" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="51" t="s">
+      <c r="F13" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="51"/>
+      <c r="G13" s="52"/>
       <c r="H13" s="37" t="s">
         <v>313</v>
       </c>
@@ -8382,10 +8382,10 @@
       <c r="E14" s="38">
         <v>16</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="53">
         <v>20</v>
       </c>
-      <c r="G14" s="52"/>
+      <c r="G14" s="53"/>
       <c r="H14" s="39"/>
     </row>
     <row r="15" spans="1:8" ht="24" customHeight="1">
@@ -8414,10 +8414,10 @@
       <c r="E16" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="53" t="s">
+      <c r="F16" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="53"/>
+      <c r="G16" s="54"/>
       <c r="H16" s="6" t="s">
         <v>103</v>
       </c>
@@ -8438,10 +8438,10 @@
       <c r="E17" s="25">
         <v>6</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="55">
         <v>9</v>
       </c>
-      <c r="G17" s="44"/>
+      <c r="G17" s="55"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="24" customHeight="1">
@@ -8470,34 +8470,34 @@
       <c r="E19" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="45" t="s">
+      <c r="F19" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="45"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="26" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="24" customHeight="1">
       <c r="A20" s="27">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B20" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C20" s="27">
         <v>0</v>
       </c>
       <c r="D20" s="27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E20" s="27">
-        <v>8</v>
-      </c>
-      <c r="F20" s="46">
-        <v>11</v>
-      </c>
-      <c r="G20" s="46"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="57">
+        <v>0</v>
+      </c>
+      <c r="G20" s="57"/>
       <c r="H20" s="32"/>
     </row>
     <row r="21" spans="1:8" ht="24" customHeight="1">
@@ -8526,10 +8526,10 @@
       <c r="E22" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="47" t="s">
+      <c r="F22" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="47"/>
+      <c r="G22" s="58"/>
       <c r="H22" s="28" t="s">
         <v>35</v>
       </c>
@@ -8550,10 +8550,10 @@
       <c r="E23" s="29">
         <v>22</v>
       </c>
-      <c r="F23" s="48">
+      <c r="F23" s="59">
         <v>16</v>
       </c>
-      <c r="G23" s="48"/>
+      <c r="G23" s="59"/>
       <c r="H23" s="32"/>
     </row>
     <row r="27" spans="1:8">
@@ -8570,22 +8570,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizando tabela do torneio 5
</commit_message>
<xml_diff>
--- a/Dados/Dados_Torneio.xlsx
+++ b/Dados/Dados_Torneio.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmarinho\Desktop\Site\Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allys\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60650F8-496D-4AA7-B8D0-527C5D3BFB1F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Artilharia" sheetId="1" r:id="rId1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="348">
   <si>
     <t>Melhores Jogadores</t>
   </si>
@@ -296,6 +297,9 @@
   </si>
   <si>
     <t xml:space="preserve">1 x 2 </t>
+  </si>
+  <si>
+    <t>1 x1</t>
   </si>
   <si>
     <t xml:space="preserve">Ajax </t>
@@ -1078,7 +1082,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="27">
     <font>
       <sz val="11"/>
@@ -2108,11 +2112,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1009"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D56"/>
+    <sheetView showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2178,13 +2182,13 @@
         <v>10</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C4" s="17">
         <v>8</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -2199,7 +2203,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -2208,13 +2212,13 @@
         <v>12</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C6" s="17">
         <v>6</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -2229,7 +2233,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -2304,7 +2308,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -2319,7 +2323,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -2334,7 +2338,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -2373,13 +2377,13 @@
         <v>23</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C17" s="17">
         <v>3</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F17" s="1"/>
       <c r="I17" s="2"/>
@@ -2410,7 +2414,7 @@
         <v>3</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -2455,7 +2459,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -2494,7 +2498,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C25" s="17">
         <v>2</v>
@@ -2509,7 +2513,7 @@
         <v>32</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C26" s="17">
         <v>2</v>
@@ -2521,40 +2525,40 @@
     </row>
     <row r="27" spans="1:9" ht="24" customHeight="1">
       <c r="A27" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C27" s="17">
         <v>2</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="24" customHeight="1">
       <c r="A28" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C28" s="17">
         <v>1</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="24" customHeight="1">
       <c r="A29" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C29" s="17">
         <v>1</v>
@@ -2566,66 +2570,66 @@
     </row>
     <row r="30" spans="1:9" ht="24" customHeight="1">
       <c r="A30" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C30" s="17">
         <v>1</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="24" customHeight="1">
       <c r="A31" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C31" s="17">
         <v>1</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="24.75" customHeight="1">
       <c r="A32" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C32" s="17">
         <v>1</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:4" ht="24.75" customHeight="1">
       <c r="A33" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C33" s="17">
         <v>1</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="24.75" customHeight="1">
       <c r="A34" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>47</v>
@@ -2634,12 +2638,12 @@
         <v>1</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="24.75" customHeight="1">
       <c r="A35" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>50</v>
@@ -2648,12 +2652,12 @@
         <v>1</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.75" customHeight="1">
       <c r="A36" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>52</v>
@@ -2662,12 +2666,12 @@
         <v>1</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="24.75" customHeight="1">
       <c r="A37" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>53</v>
@@ -2676,12 +2680,12 @@
         <v>1</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="24.75" customHeight="1">
       <c r="A38" s="17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>60</v>
@@ -2695,7 +2699,7 @@
     </row>
     <row r="39" spans="1:4" ht="24.75" customHeight="1">
       <c r="A39" s="17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B39" s="19" t="s">
         <v>55</v>
@@ -2709,7 +2713,7 @@
     </row>
     <row r="40" spans="1:4" ht="24.75" customHeight="1">
       <c r="A40" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B40" s="19" t="s">
         <v>57</v>
@@ -2718,29 +2722,29 @@
         <v>1</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="24.75" customHeight="1">
       <c r="A41" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C41" s="17">
         <v>1</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="24.75" customHeight="1">
       <c r="A42" s="17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C42" s="17">
         <v>1</v>
@@ -2751,21 +2755,21 @@
     </row>
     <row r="43" spans="1:4" ht="24.75" customHeight="1">
       <c r="A43" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C43" s="17">
         <v>1</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="24.75" customHeight="1">
       <c r="A44" s="17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>64</v>
@@ -2774,43 +2778,43 @@
         <v>1</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="24.75" customHeight="1">
       <c r="A45" s="17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C45" s="17">
         <v>1</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="24.75" customHeight="1">
       <c r="A46" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C46" s="17">
         <v>1</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="24.75" customHeight="1">
       <c r="A47" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C47" s="17">
         <v>1</v>
@@ -2821,10 +2825,10 @@
     </row>
     <row r="48" spans="1:4" ht="24.75" customHeight="1">
       <c r="A48" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C48" s="17">
         <v>1</v>
@@ -2835,24 +2839,24 @@
     </row>
     <row r="49" spans="1:11" ht="24.75" customHeight="1">
       <c r="A49" s="17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C49" s="17">
         <v>1</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="24.75" customHeight="1">
       <c r="A50" s="17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C50" s="17">
         <v>1</v>
@@ -2863,10 +2867,10 @@
     </row>
     <row r="51" spans="1:11" ht="24.75" customHeight="1">
       <c r="A51" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C51" s="17">
         <v>1</v>
@@ -2877,10 +2881,10 @@
     </row>
     <row r="52" spans="1:11" ht="24.75" customHeight="1">
       <c r="A52" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C52" s="17">
         <v>1</v>
@@ -2891,24 +2895,24 @@
     </row>
     <row r="53" spans="1:11" ht="24.75" customHeight="1">
       <c r="A53" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C53" s="17">
         <v>1</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="24.75" customHeight="1">
       <c r="A54" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C54" s="17">
         <v>1</v>
@@ -2919,10 +2923,10 @@
     </row>
     <row r="55" spans="1:11" ht="24.75" customHeight="1">
       <c r="A55" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C55" s="17">
         <v>1</v>
@@ -2933,10 +2937,10 @@
     </row>
     <row r="56" spans="1:11" ht="24.75" customHeight="1">
       <c r="A56" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C56" s="17">
         <v>1</v>
@@ -2947,12 +2951,12 @@
     </row>
     <row r="57" spans="1:11" ht="24.75" customHeight="1">
       <c r="A57" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="24.75" customHeight="1">
       <c r="A58" s="17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
@@ -2961,7 +2965,7 @@
     </row>
     <row r="59" spans="1:11" ht="24.75" customHeight="1">
       <c r="A59" s="17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
@@ -2969,7 +2973,7 @@
     </row>
     <row r="60" spans="1:11" ht="24.75" customHeight="1">
       <c r="A60" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
@@ -2977,7 +2981,7 @@
     </row>
     <row r="61" spans="1:11" ht="24.75" customHeight="1">
       <c r="A61" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
@@ -2985,7 +2989,7 @@
     </row>
     <row r="62" spans="1:11" ht="24.75" customHeight="1">
       <c r="A62" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
@@ -2993,7 +2997,7 @@
     </row>
     <row r="63" spans="1:11" ht="24.75" customHeight="1">
       <c r="A63" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
@@ -3001,7 +3005,7 @@
     </row>
     <row r="64" spans="1:11" ht="24.75" customHeight="1">
       <c r="A64" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B64" s="17"/>
       <c r="C64" s="17"/>
@@ -3009,7 +3013,7 @@
     </row>
     <row r="65" spans="1:4" ht="24.75" customHeight="1">
       <c r="A65" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
@@ -3017,7 +3021,7 @@
     </row>
     <row r="66" spans="1:4" ht="24.75" customHeight="1">
       <c r="A66" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B66" s="17"/>
       <c r="C66" s="17"/>
@@ -3025,7 +3029,7 @@
     </row>
     <row r="67" spans="1:4" ht="24.75" customHeight="1">
       <c r="A67" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B67" s="17"/>
       <c r="C67" s="17"/>
@@ -3033,7 +3037,7 @@
     </row>
     <row r="68" spans="1:4" ht="24.75" customHeight="1">
       <c r="A68" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>
@@ -3041,7 +3045,7 @@
     </row>
     <row r="69" spans="1:4" ht="24.75" customHeight="1">
       <c r="A69" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B69" s="17"/>
       <c r="C69" s="17"/>
@@ -3049,7 +3053,7 @@
     </row>
     <row r="70" spans="1:4" ht="24.75" customHeight="1">
       <c r="A70" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B70" s="17"/>
       <c r="C70" s="17"/>
@@ -3057,7 +3061,7 @@
     </row>
     <row r="71" spans="1:4" ht="24.75" customHeight="1">
       <c r="A71" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B71" s="17"/>
       <c r="C71" s="17"/>
@@ -3065,7 +3069,7 @@
     </row>
     <row r="72" spans="1:4" ht="24.75" customHeight="1">
       <c r="A72" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B72" s="17"/>
       <c r="C72" s="17"/>
@@ -3073,7 +3077,7 @@
     </row>
     <row r="73" spans="1:4" ht="24.75" customHeight="1">
       <c r="A73" s="17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B73" s="17"/>
       <c r="C73" s="17"/>
@@ -3081,7 +3085,7 @@
     </row>
     <row r="74" spans="1:4" ht="24.75" customHeight="1">
       <c r="A74" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B74" s="17"/>
       <c r="C74" s="17"/>
@@ -3089,7 +3093,7 @@
     </row>
     <row r="75" spans="1:4" ht="24.75" customHeight="1">
       <c r="A75" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B75" s="17"/>
       <c r="C75" s="17"/>
@@ -3097,7 +3101,7 @@
     </row>
     <row r="76" spans="1:4" ht="24.75" customHeight="1">
       <c r="A76" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
@@ -3105,7 +3109,7 @@
     </row>
     <row r="77" spans="1:4" ht="24.75" customHeight="1">
       <c r="A77" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B77" s="17"/>
       <c r="C77" s="17"/>
@@ -3113,7 +3117,7 @@
     </row>
     <row r="78" spans="1:4" ht="24.75" customHeight="1">
       <c r="A78" s="17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B78" s="17"/>
       <c r="C78" s="17"/>
@@ -3121,7 +3125,7 @@
     </row>
     <row r="79" spans="1:4" ht="24.75" customHeight="1">
       <c r="A79" s="17" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B79" s="17"/>
       <c r="C79" s="17"/>
@@ -3129,7 +3133,7 @@
     </row>
     <row r="80" spans="1:4" ht="24.75" customHeight="1">
       <c r="A80" s="17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B80" s="17"/>
       <c r="C80" s="17"/>
@@ -3137,7 +3141,7 @@
     </row>
     <row r="81" spans="1:4" ht="24.75" customHeight="1">
       <c r="A81" s="17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B81" s="17"/>
       <c r="C81" s="17"/>
@@ -3145,7 +3149,7 @@
     </row>
     <row r="82" spans="1:4" ht="24.75" customHeight="1">
       <c r="A82" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B82" s="17"/>
       <c r="C82" s="17"/>
@@ -3153,7 +3157,7 @@
     </row>
     <row r="83" spans="1:4" ht="24.75" customHeight="1">
       <c r="A83" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B83" s="17"/>
       <c r="C83" s="17"/>
@@ -3161,7 +3165,7 @@
     </row>
     <row r="84" spans="1:4" ht="24.75" customHeight="1">
       <c r="A84" s="17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
@@ -3169,7 +3173,7 @@
     </row>
     <row r="85" spans="1:4" ht="24.75" customHeight="1">
       <c r="A85" s="17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B85" s="17"/>
       <c r="C85" s="17"/>
@@ -3177,7 +3181,7 @@
     </row>
     <row r="86" spans="1:4" ht="24.75" customHeight="1">
       <c r="A86" s="17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B86" s="17"/>
       <c r="C86" s="17"/>
@@ -3185,7 +3189,7 @@
     </row>
     <row r="87" spans="1:4" ht="24.75" customHeight="1">
       <c r="A87" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B87" s="17"/>
       <c r="C87" s="17"/>
@@ -3193,7 +3197,7 @@
     </row>
     <row r="88" spans="1:4" ht="24.75" customHeight="1">
       <c r="A88" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B88" s="17"/>
       <c r="C88" s="17"/>
@@ -3201,7 +3205,7 @@
     </row>
     <row r="89" spans="1:4" ht="24.75" customHeight="1">
       <c r="A89" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B89" s="17"/>
       <c r="C89" s="17"/>
@@ -3209,7 +3213,7 @@
     </row>
     <row r="90" spans="1:4" ht="24.75" customHeight="1">
       <c r="A90" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B90" s="17"/>
       <c r="C90" s="17"/>
@@ -3217,7 +3221,7 @@
     </row>
     <row r="91" spans="1:4" ht="24.75" customHeight="1">
       <c r="A91" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B91" s="17"/>
       <c r="C91" s="17"/>
@@ -3225,7 +3229,7 @@
     </row>
     <row r="92" spans="1:4" ht="24.75" customHeight="1">
       <c r="A92" s="17" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B92" s="17"/>
       <c r="C92" s="17"/>
@@ -3233,7 +3237,7 @@
     </row>
     <row r="93" spans="1:4" ht="24.75" customHeight="1">
       <c r="A93" s="17" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B93" s="17"/>
       <c r="C93" s="17"/>
@@ -3241,7 +3245,7 @@
     </row>
     <row r="94" spans="1:4" ht="24.75" customHeight="1">
       <c r="A94" s="17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B94" s="17"/>
       <c r="C94" s="17"/>
@@ -3249,7 +3253,7 @@
     </row>
     <row r="95" spans="1:4" ht="24.75" customHeight="1">
       <c r="A95" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B95" s="17"/>
       <c r="C95" s="17"/>
@@ -3257,7 +3261,7 @@
     </row>
     <row r="96" spans="1:4" ht="24.75" customHeight="1">
       <c r="A96" s="17" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B96" s="17"/>
       <c r="C96" s="17"/>
@@ -3265,7 +3269,7 @@
     </row>
     <row r="97" spans="1:4" ht="24.75" customHeight="1">
       <c r="A97" s="17" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B97" s="17"/>
       <c r="C97" s="17"/>
@@ -3273,7 +3277,7 @@
     </row>
     <row r="98" spans="1:4" ht="24.75" customHeight="1">
       <c r="A98" s="17" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B98" s="17"/>
       <c r="C98" s="17"/>
@@ -3281,7 +3285,7 @@
     </row>
     <row r="99" spans="1:4" ht="24.75" customHeight="1">
       <c r="A99" s="17" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B99" s="17"/>
       <c r="C99" s="17"/>
@@ -3289,7 +3293,7 @@
     </row>
     <row r="100" spans="1:4" ht="24.75" customHeight="1">
       <c r="A100" s="17" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B100" s="17"/>
       <c r="C100" s="17"/>
@@ -3297,7 +3301,7 @@
     </row>
     <row r="101" spans="1:4" ht="24.75" customHeight="1">
       <c r="A101" s="17" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B101" s="17"/>
       <c r="C101" s="17"/>
@@ -3305,7 +3309,7 @@
     </row>
     <row r="102" spans="1:4" ht="24.75" customHeight="1">
       <c r="A102" s="17" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B102" s="17"/>
       <c r="C102" s="17"/>
@@ -3313,7 +3317,7 @@
     </row>
     <row r="103" spans="1:4" ht="24.75" customHeight="1">
       <c r="A103" s="17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B103" s="17"/>
       <c r="C103" s="17"/>
@@ -3321,7 +3325,7 @@
     </row>
     <row r="104" spans="1:4" ht="24.75" customHeight="1">
       <c r="A104" s="17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B104" s="17"/>
       <c r="C104" s="17"/>
@@ -3329,7 +3333,7 @@
     </row>
     <row r="105" spans="1:4" ht="24.75" customHeight="1">
       <c r="A105" s="17" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B105" s="17"/>
       <c r="C105" s="17"/>
@@ -3337,7 +3341,7 @@
     </row>
     <row r="106" spans="1:4" ht="24.75" customHeight="1">
       <c r="A106" s="17" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B106" s="17"/>
       <c r="C106" s="17"/>
@@ -3345,7 +3349,7 @@
     </row>
     <row r="107" spans="1:4" ht="24.75" customHeight="1">
       <c r="A107" s="17" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B107" s="17"/>
       <c r="C107" s="17"/>
@@ -3353,7 +3357,7 @@
     </row>
     <row r="108" spans="1:4" ht="24.75" customHeight="1">
       <c r="A108" s="17" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B108" s="17"/>
       <c r="C108" s="17"/>
@@ -3361,7 +3365,7 @@
     </row>
     <row r="109" spans="1:4" ht="24.75" customHeight="1">
       <c r="A109" s="17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B109" s="17"/>
       <c r="C109" s="17"/>
@@ -3369,7 +3373,7 @@
     </row>
     <row r="110" spans="1:4" ht="24.75" customHeight="1">
       <c r="A110" s="17" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B110" s="17"/>
       <c r="C110" s="17"/>
@@ -3377,7 +3381,7 @@
     </row>
     <row r="111" spans="1:4" ht="24.75" customHeight="1">
       <c r="A111" s="17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B111" s="17"/>
       <c r="C111" s="17"/>
@@ -3385,7 +3389,7 @@
     </row>
     <row r="112" spans="1:4" ht="24.75" customHeight="1">
       <c r="A112" s="17" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B112" s="17"/>
       <c r="C112" s="17"/>
@@ -3393,7 +3397,7 @@
     </row>
     <row r="113" spans="1:4" ht="24.75" customHeight="1">
       <c r="A113" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B113" s="17"/>
       <c r="C113" s="17"/>
@@ -3401,7 +3405,7 @@
     </row>
     <row r="114" spans="1:4" ht="24.75" customHeight="1">
       <c r="A114" s="17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B114" s="17"/>
       <c r="C114" s="17"/>
@@ -3409,7 +3413,7 @@
     </row>
     <row r="115" spans="1:4" ht="24.75" customHeight="1">
       <c r="A115" s="17" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B115" s="17"/>
       <c r="C115" s="17"/>
@@ -3417,7 +3421,7 @@
     </row>
     <row r="116" spans="1:4" ht="24.75" customHeight="1">
       <c r="A116" s="17" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B116" s="17"/>
       <c r="C116" s="17"/>
@@ -3425,7 +3429,7 @@
     </row>
     <row r="117" spans="1:4" ht="24.75" customHeight="1">
       <c r="A117" s="17" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B117" s="17"/>
       <c r="C117" s="17"/>
@@ -3433,7 +3437,7 @@
     </row>
     <row r="118" spans="1:4" ht="24.75" customHeight="1">
       <c r="A118" s="17" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B118" s="17"/>
       <c r="C118" s="17"/>
@@ -3441,7 +3445,7 @@
     </row>
     <row r="119" spans="1:4" ht="24.75" customHeight="1">
       <c r="A119" s="17" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B119" s="17"/>
       <c r="C119" s="17"/>
@@ -3449,7 +3453,7 @@
     </row>
     <row r="120" spans="1:4" ht="24.75" customHeight="1">
       <c r="A120" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B120" s="17"/>
       <c r="C120" s="17"/>
@@ -3457,7 +3461,7 @@
     </row>
     <row r="121" spans="1:4" ht="24.75" customHeight="1">
       <c r="A121" s="17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B121" s="17"/>
       <c r="C121" s="17"/>
@@ -3465,7 +3469,7 @@
     </row>
     <row r="122" spans="1:4" ht="24.75" customHeight="1">
       <c r="A122" s="17" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B122" s="17"/>
       <c r="C122" s="17"/>
@@ -3473,7 +3477,7 @@
     </row>
     <row r="123" spans="1:4" ht="24.75" customHeight="1">
       <c r="A123" s="17" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B123" s="17"/>
       <c r="C123" s="17"/>
@@ -3481,7 +3485,7 @@
     </row>
     <row r="124" spans="1:4" ht="24.75" customHeight="1">
       <c r="A124" s="17" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B124" s="17"/>
       <c r="C124" s="17"/>
@@ -3489,7 +3493,7 @@
     </row>
     <row r="125" spans="1:4" ht="24.75" customHeight="1">
       <c r="A125" s="17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B125" s="17"/>
       <c r="C125" s="17"/>
@@ -3497,7 +3501,7 @@
     </row>
     <row r="126" spans="1:4" ht="24.75" customHeight="1">
       <c r="A126" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B126" s="17"/>
       <c r="C126" s="17"/>
@@ -3505,7 +3509,7 @@
     </row>
     <row r="127" spans="1:4" ht="24.75" customHeight="1">
       <c r="A127" s="17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B127" s="17"/>
       <c r="C127" s="17"/>
@@ -3513,7 +3517,7 @@
     </row>
     <row r="128" spans="1:4" ht="24.75" customHeight="1">
       <c r="A128" s="17" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B128" s="17"/>
       <c r="C128" s="17"/>
@@ -3521,7 +3525,7 @@
     </row>
     <row r="129" spans="1:4" ht="24.75" customHeight="1">
       <c r="A129" s="17" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B129" s="17"/>
       <c r="C129" s="17"/>
@@ -3529,7 +3533,7 @@
     </row>
     <row r="130" spans="1:4" ht="24.75" customHeight="1">
       <c r="A130" s="17" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B130" s="17"/>
       <c r="C130" s="17"/>
@@ -3537,7 +3541,7 @@
     </row>
     <row r="131" spans="1:4" ht="24.75" customHeight="1">
       <c r="A131" s="17" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B131" s="17"/>
       <c r="C131" s="17"/>
@@ -3545,7 +3549,7 @@
     </row>
     <row r="132" spans="1:4" ht="24.75" customHeight="1">
       <c r="A132" s="17" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B132" s="17"/>
       <c r="C132" s="17"/>
@@ -3553,7 +3557,7 @@
     </row>
     <row r="133" spans="1:4" ht="24.75" customHeight="1">
       <c r="A133" s="17" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B133" s="17"/>
       <c r="C133" s="17"/>
@@ -3561,7 +3565,7 @@
     </row>
     <row r="134" spans="1:4" ht="24.75" customHeight="1">
       <c r="A134" s="17" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B134" s="17"/>
       <c r="C134" s="17"/>
@@ -3569,7 +3573,7 @@
     </row>
     <row r="135" spans="1:4" ht="24.75" customHeight="1">
       <c r="A135" s="17" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B135" s="17"/>
       <c r="C135" s="17"/>
@@ -3577,7 +3581,7 @@
     </row>
     <row r="136" spans="1:4" ht="24.75" customHeight="1">
       <c r="A136" s="17" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B136" s="17"/>
       <c r="C136" s="17"/>
@@ -3585,7 +3589,7 @@
     </row>
     <row r="137" spans="1:4" ht="24.75" customHeight="1">
       <c r="A137" s="17" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B137" s="17"/>
       <c r="C137" s="17"/>
@@ -3593,7 +3597,7 @@
     </row>
     <row r="138" spans="1:4" ht="24.75" customHeight="1">
       <c r="A138" s="17" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B138" s="17"/>
       <c r="C138" s="17"/>
@@ -3601,7 +3605,7 @@
     </row>
     <row r="139" spans="1:4" ht="24.75" customHeight="1">
       <c r="A139" s="17" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B139" s="17"/>
       <c r="C139" s="17"/>
@@ -3609,7 +3613,7 @@
     </row>
     <row r="140" spans="1:4" ht="24.75" customHeight="1">
       <c r="A140" s="17" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B140" s="17"/>
       <c r="C140" s="17"/>
@@ -3617,7 +3621,7 @@
     </row>
     <row r="141" spans="1:4" ht="24.75" customHeight="1">
       <c r="A141" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B141" s="17"/>
       <c r="C141" s="17"/>
@@ -3625,7 +3629,7 @@
     </row>
     <row r="142" spans="1:4" ht="24.75" customHeight="1">
       <c r="A142" s="17" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B142" s="17"/>
       <c r="C142" s="17"/>
@@ -3633,7 +3637,7 @@
     </row>
     <row r="143" spans="1:4" ht="24.75" customHeight="1">
       <c r="A143" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B143" s="17"/>
       <c r="C143" s="17"/>
@@ -3641,7 +3645,7 @@
     </row>
     <row r="144" spans="1:4" ht="24.75" customHeight="1">
       <c r="A144" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B144" s="17"/>
       <c r="C144" s="17"/>
@@ -3649,7 +3653,7 @@
     </row>
     <row r="145" spans="1:4" ht="24.75" customHeight="1">
       <c r="A145" s="17" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B145" s="17"/>
       <c r="C145" s="17"/>
@@ -3657,7 +3661,7 @@
     </row>
     <row r="146" spans="1:4" ht="24.75" customHeight="1">
       <c r="A146" s="17" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B146" s="17"/>
       <c r="C146" s="17"/>
@@ -3665,7 +3669,7 @@
     </row>
     <row r="147" spans="1:4" ht="24.75" customHeight="1">
       <c r="A147" s="17" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B147" s="17"/>
       <c r="C147" s="17"/>
@@ -3673,7 +3677,7 @@
     </row>
     <row r="148" spans="1:4" ht="24.75" customHeight="1">
       <c r="A148" s="17" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B148" s="17"/>
       <c r="C148" s="17"/>
@@ -3681,7 +3685,7 @@
     </row>
     <row r="149" spans="1:4" ht="24.75" customHeight="1">
       <c r="A149" s="17" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B149" s="17"/>
       <c r="C149" s="17"/>
@@ -3689,7 +3693,7 @@
     </row>
     <row r="150" spans="1:4" ht="24.75" customHeight="1">
       <c r="A150" s="17" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B150" s="17"/>
       <c r="C150" s="17"/>
@@ -3697,7 +3701,7 @@
     </row>
     <row r="151" spans="1:4" ht="24.75" customHeight="1">
       <c r="A151" s="17" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B151" s="17"/>
       <c r="C151" s="17"/>
@@ -3705,7 +3709,7 @@
     </row>
     <row r="152" spans="1:4" ht="24.75" customHeight="1">
       <c r="A152" s="17" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B152" s="17"/>
       <c r="C152" s="17"/>
@@ -3713,7 +3717,7 @@
     </row>
     <row r="153" spans="1:4" ht="24.75" customHeight="1">
       <c r="A153" s="17" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B153" s="17"/>
       <c r="C153" s="17"/>
@@ -3721,7 +3725,7 @@
     </row>
     <row r="154" spans="1:4" ht="24.75" customHeight="1">
       <c r="A154" s="17" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B154" s="17"/>
       <c r="C154" s="17"/>
@@ -3729,7 +3733,7 @@
     </row>
     <row r="155" spans="1:4" ht="24.75" customHeight="1">
       <c r="A155" s="17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B155" s="17"/>
       <c r="C155" s="17"/>
@@ -3737,7 +3741,7 @@
     </row>
     <row r="156" spans="1:4" ht="24.75" customHeight="1">
       <c r="A156" s="17" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B156" s="17"/>
       <c r="C156" s="17"/>
@@ -3745,7 +3749,7 @@
     </row>
     <row r="157" spans="1:4" ht="24.75" customHeight="1">
       <c r="A157" s="17" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B157" s="17"/>
       <c r="C157" s="17"/>
@@ -3753,7 +3757,7 @@
     </row>
     <row r="158" spans="1:4" ht="24.75" customHeight="1">
       <c r="A158" s="17" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B158" s="17"/>
       <c r="C158" s="17"/>
@@ -3761,7 +3765,7 @@
     </row>
     <row r="159" spans="1:4" ht="24.75" customHeight="1">
       <c r="A159" s="17" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B159" s="17"/>
       <c r="C159" s="17"/>
@@ -3769,7 +3773,7 @@
     </row>
     <row r="160" spans="1:4" ht="24.75" customHeight="1">
       <c r="A160" s="17" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B160" s="17"/>
       <c r="C160" s="17"/>
@@ -3777,7 +3781,7 @@
     </row>
     <row r="161" spans="1:4" ht="24.75" customHeight="1">
       <c r="A161" s="17" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B161" s="17"/>
       <c r="C161" s="17"/>
@@ -3785,7 +3789,7 @@
     </row>
     <row r="162" spans="1:4" ht="24.75" customHeight="1">
       <c r="A162" s="17" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B162" s="17"/>
       <c r="C162" s="17"/>
@@ -3793,7 +3797,7 @@
     </row>
     <row r="163" spans="1:4" ht="24.75" customHeight="1">
       <c r="A163" s="17" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B163" s="17"/>
       <c r="C163" s="17"/>
@@ -3801,7 +3805,7 @@
     </row>
     <row r="164" spans="1:4" ht="24.75" customHeight="1">
       <c r="A164" s="17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B164" s="17"/>
       <c r="C164" s="17"/>
@@ -3809,7 +3813,7 @@
     </row>
     <row r="165" spans="1:4" ht="24.75" customHeight="1">
       <c r="A165" s="17" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B165" s="17"/>
       <c r="C165" s="17"/>
@@ -3817,7 +3821,7 @@
     </row>
     <row r="166" spans="1:4" ht="24.75" customHeight="1">
       <c r="A166" s="17" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B166" s="17"/>
       <c r="C166" s="17"/>
@@ -3825,7 +3829,7 @@
     </row>
     <row r="167" spans="1:4" ht="24.75" customHeight="1">
       <c r="A167" s="17" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B167" s="17"/>
       <c r="C167" s="17"/>
@@ -3833,7 +3837,7 @@
     </row>
     <row r="168" spans="1:4" ht="24.75" customHeight="1">
       <c r="A168" s="17" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B168" s="17"/>
       <c r="C168" s="17"/>
@@ -3841,7 +3845,7 @@
     </row>
     <row r="169" spans="1:4" ht="24.75" customHeight="1">
       <c r="A169" s="17" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B169" s="17"/>
       <c r="C169" s="17"/>
@@ -3849,7 +3853,7 @@
     </row>
     <row r="170" spans="1:4" ht="24.75" customHeight="1">
       <c r="A170" s="17" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B170" s="17"/>
       <c r="C170" s="17"/>
@@ -3857,7 +3861,7 @@
     </row>
     <row r="171" spans="1:4" ht="24.75" customHeight="1">
       <c r="A171" s="17" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B171" s="17"/>
       <c r="C171" s="17"/>
@@ -3865,7 +3869,7 @@
     </row>
     <row r="172" spans="1:4" ht="24.75" customHeight="1">
       <c r="A172" s="17" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B172" s="17"/>
       <c r="C172" s="17"/>
@@ -3873,7 +3877,7 @@
     </row>
     <row r="173" spans="1:4" ht="24.75" customHeight="1">
       <c r="A173" s="17" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B173" s="17"/>
       <c r="C173" s="17"/>
@@ -3881,7 +3885,7 @@
     </row>
     <row r="174" spans="1:4" ht="24.75" customHeight="1">
       <c r="A174" s="17" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B174" s="17"/>
       <c r="C174" s="17"/>
@@ -3889,7 +3893,7 @@
     </row>
     <row r="175" spans="1:4" ht="24.75" customHeight="1">
       <c r="A175" s="17" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B175" s="17"/>
       <c r="C175" s="17"/>
@@ -3897,7 +3901,7 @@
     </row>
     <row r="176" spans="1:4" ht="24.75" customHeight="1">
       <c r="A176" s="17" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B176" s="17"/>
       <c r="C176" s="17"/>
@@ -3905,7 +3909,7 @@
     </row>
     <row r="177" spans="1:4" ht="24.75" customHeight="1">
       <c r="A177" s="17" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B177" s="17"/>
       <c r="C177" s="17"/>
@@ -3913,7 +3917,7 @@
     </row>
     <row r="178" spans="1:4" ht="24.75" customHeight="1">
       <c r="A178" s="17" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B178" s="17"/>
       <c r="C178" s="17"/>
@@ -3921,7 +3925,7 @@
     </row>
     <row r="179" spans="1:4" ht="24.75" customHeight="1">
       <c r="A179" s="17" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B179" s="17"/>
       <c r="C179" s="17"/>
@@ -3929,7 +3933,7 @@
     </row>
     <row r="180" spans="1:4" ht="24.75" customHeight="1">
       <c r="A180" s="17" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B180" s="17"/>
       <c r="C180" s="17"/>
@@ -3937,7 +3941,7 @@
     </row>
     <row r="181" spans="1:4" ht="24.75" customHeight="1">
       <c r="A181" s="17" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B181" s="17"/>
       <c r="C181" s="17"/>
@@ -3945,7 +3949,7 @@
     </row>
     <row r="182" spans="1:4" ht="24.75" customHeight="1">
       <c r="A182" s="17" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B182" s="17"/>
       <c r="C182" s="17"/>
@@ -3953,7 +3957,7 @@
     </row>
     <row r="183" spans="1:4" ht="24.75" customHeight="1">
       <c r="A183" s="17" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B183" s="17"/>
       <c r="C183" s="17"/>
@@ -3961,7 +3965,7 @@
     </row>
     <row r="184" spans="1:4" ht="24.75" customHeight="1">
       <c r="A184" s="17" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B184" s="17"/>
       <c r="C184" s="17"/>
@@ -3969,7 +3973,7 @@
     </row>
     <row r="185" spans="1:4" ht="24.75" customHeight="1">
       <c r="A185" s="17" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B185" s="17"/>
       <c r="C185" s="17"/>
@@ -3977,7 +3981,7 @@
     </row>
     <row r="186" spans="1:4" ht="24.75" customHeight="1">
       <c r="A186" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B186" s="17"/>
       <c r="C186" s="17"/>
@@ -3985,7 +3989,7 @@
     </row>
     <row r="187" spans="1:4" ht="24.75" customHeight="1">
       <c r="A187" s="17" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B187" s="17"/>
       <c r="C187" s="17"/>
@@ -3993,7 +3997,7 @@
     </row>
     <row r="188" spans="1:4" ht="24.75" customHeight="1">
       <c r="A188" s="17" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B188" s="17"/>
       <c r="C188" s="17"/>
@@ -4001,7 +4005,7 @@
     </row>
     <row r="189" spans="1:4" ht="24.75" customHeight="1">
       <c r="A189" s="17" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B189" s="17"/>
       <c r="C189" s="17"/>
@@ -4009,7 +4013,7 @@
     </row>
     <row r="190" spans="1:4" ht="24.75" customHeight="1">
       <c r="A190" s="17" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B190" s="17"/>
       <c r="C190" s="17"/>
@@ -4017,7 +4021,7 @@
     </row>
     <row r="191" spans="1:4" ht="24.75" customHeight="1">
       <c r="A191" s="17" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B191" s="17"/>
       <c r="C191" s="17"/>
@@ -4025,7 +4029,7 @@
     </row>
     <row r="192" spans="1:4" ht="24.75" customHeight="1">
       <c r="A192" s="17" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B192" s="17"/>
       <c r="C192" s="17"/>
@@ -4033,7 +4037,7 @@
     </row>
     <row r="193" spans="1:4" ht="24.75" customHeight="1">
       <c r="A193" s="17" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B193" s="17"/>
       <c r="C193" s="17"/>
@@ -4041,7 +4045,7 @@
     </row>
     <row r="194" spans="1:4" ht="24.75" customHeight="1">
       <c r="A194" s="17" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B194" s="17"/>
       <c r="C194" s="17"/>
@@ -4049,7 +4053,7 @@
     </row>
     <row r="195" spans="1:4" ht="24.75" customHeight="1">
       <c r="A195" s="17" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B195" s="17"/>
       <c r="C195" s="17"/>
@@ -4057,7 +4061,7 @@
     </row>
     <row r="196" spans="1:4" ht="24.75" customHeight="1">
       <c r="A196" s="17" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B196" s="17"/>
       <c r="C196" s="17"/>
@@ -4065,7 +4069,7 @@
     </row>
     <row r="197" spans="1:4" ht="24.75" customHeight="1">
       <c r="A197" s="17" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B197" s="17"/>
       <c r="C197" s="17"/>
@@ -4073,7 +4077,7 @@
     </row>
     <row r="198" spans="1:4" ht="24.75" customHeight="1">
       <c r="A198" s="17" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B198" s="17"/>
       <c r="C198" s="17"/>
@@ -4081,7 +4085,7 @@
     </row>
     <row r="199" spans="1:4" ht="24.75" customHeight="1">
       <c r="A199" s="17" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B199" s="17"/>
       <c r="C199" s="17"/>
@@ -4089,7 +4093,7 @@
     </row>
     <row r="200" spans="1:4" ht="24.75" customHeight="1">
       <c r="A200" s="17" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B200" s="17"/>
       <c r="C200" s="17"/>
@@ -4097,7 +4101,7 @@
     </row>
     <row r="201" spans="1:4" ht="24.75" customHeight="1">
       <c r="A201" s="17" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B201" s="17"/>
       <c r="C201" s="17"/>
@@ -4105,7 +4109,7 @@
     </row>
     <row r="202" spans="1:4" ht="24.75" customHeight="1">
       <c r="A202" s="17" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B202" s="17"/>
       <c r="C202" s="17"/>
@@ -4113,7 +4117,7 @@
     </row>
     <row r="203" spans="1:4" ht="24.75" customHeight="1">
       <c r="A203" s="17" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B203" s="17"/>
       <c r="C203" s="17"/>
@@ -4121,7 +4125,7 @@
     </row>
     <row r="204" spans="1:4" ht="24.75" customHeight="1">
       <c r="A204" s="17" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B204" s="17"/>
       <c r="C204" s="17"/>
@@ -4129,7 +4133,7 @@
     </row>
     <row r="205" spans="1:4" ht="24.75" customHeight="1">
       <c r="A205" s="17" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B205" s="17"/>
       <c r="C205" s="17"/>
@@ -4137,7 +4141,7 @@
     </row>
     <row r="206" spans="1:4" ht="24.75" customHeight="1">
       <c r="A206" s="17" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B206" s="17"/>
       <c r="C206" s="17"/>
@@ -4145,7 +4149,7 @@
     </row>
     <row r="207" spans="1:4" ht="24.75" customHeight="1">
       <c r="A207" s="17" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B207" s="17"/>
       <c r="C207" s="17"/>
@@ -4153,7 +4157,7 @@
     </row>
     <row r="208" spans="1:4" ht="24.75" customHeight="1">
       <c r="A208" s="17" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B208" s="17"/>
       <c r="C208" s="17"/>
@@ -4961,7 +4965,7 @@
     <row r="1008" ht="15.75" customHeight="1"/>
     <row r="1009" ht="15.75" customHeight="1"/>
   </sheetData>
-  <sortState ref="A3:D1012">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D1012">
     <sortCondition descending="1" ref="C3:C1012"/>
   </sortState>
   <mergeCells count="1">
@@ -4995,10 +4999,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" sqref="D3:D42">
+    <dataValidation type="list" allowBlank="1" sqref="D3:D42" xr:uid="{CEF6A7C0-1AC2-4F68-8866-4B12B6E80CD5}">
       <formula1>"Internazionale,Arsenal,Barcelona,Manchester City,Juventus,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D58:D208 D43:D56">
+    <dataValidation type="list" allowBlank="1" sqref="D58:D208 D43:D56" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Ajax,Arsenal,Barcelona,Liverpool,Milan,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5008,11 +5012,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5365B4F2-D15B-4A5D-9EFD-6769AA916B3D}">
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5067,7 +5071,7 @@
         <v>61</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>11</v>
@@ -5215,7 +5219,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="B3:B26">
+    <dataValidation type="list" allowBlank="1" sqref="B3:B26" xr:uid="{4BB2EE2B-7E6E-46C4-ADDA-EC1BF214C8F9}">
       <formula1>"Internazionale,Arsenal,Barcelona,Manchester City,Juventus,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5224,11 +5228,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F94794-2326-4125-84B0-613C359A2BCD}">
   <dimension ref="L1:T85"/>
   <sheetViews>
-    <sheetView topLeftCell="K55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:O57"/>
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5272,7 +5276,7 @@
         <v>6</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="12:15" ht="24" customHeight="1">
@@ -5322,13 +5326,13 @@
         <v>13</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N7" s="18">
         <v>4</v>
       </c>
       <c r="O7" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="12:15" ht="24" customHeight="1">
@@ -5336,13 +5340,13 @@
         <v>14</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="N8" s="17">
         <v>4</v>
       </c>
       <c r="O8" s="17" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="12:15" ht="24" customHeight="1">
@@ -5350,13 +5354,13 @@
         <v>15</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N9" s="17">
         <v>3</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="12:15" ht="24" customHeight="1">
@@ -5364,7 +5368,7 @@
         <v>16</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N10" s="17">
         <v>3</v>
@@ -5378,13 +5382,13 @@
         <v>17</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N11" s="17">
         <v>3</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" spans="12:15" ht="24" customHeight="1">
@@ -5412,7 +5416,7 @@
         <v>3</v>
       </c>
       <c r="O13" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="12:15" ht="24" customHeight="1">
@@ -5434,13 +5438,13 @@
         <v>21</v>
       </c>
       <c r="M15" s="19" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="N15" s="17">
         <v>3</v>
       </c>
       <c r="O15" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="12:15" ht="24" customHeight="1">
@@ -5468,7 +5472,7 @@
         <v>2</v>
       </c>
       <c r="O17" s="17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="12:20" ht="24" customHeight="1">
@@ -5482,7 +5486,7 @@
         <v>2</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="12:20" ht="24" customHeight="1">
@@ -5496,7 +5500,7 @@
         <v>2</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="12:20" ht="24" customHeight="1">
@@ -5518,13 +5522,13 @@
         <v>27</v>
       </c>
       <c r="M21" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N21" s="17">
         <v>2</v>
       </c>
       <c r="O21" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="T21" s="2"/>
     </row>
@@ -5533,7 +5537,7 @@
         <v>28</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="N22" s="17">
         <v>2</v>
@@ -5548,13 +5552,13 @@
         <v>29</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="N23" s="17">
         <v>2</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="12:20" ht="24" customHeight="1">
@@ -5562,7 +5566,7 @@
         <v>30</v>
       </c>
       <c r="M24" s="17" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N24" s="17">
         <v>2</v>
@@ -5576,7 +5580,7 @@
         <v>31</v>
       </c>
       <c r="M25" s="19" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="N25" s="17">
         <v>2</v>
@@ -5596,12 +5600,12 @@
         <v>2</v>
       </c>
       <c r="O26" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="12:20" ht="24" customHeight="1">
       <c r="L27" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M27" s="17" t="s">
         <v>64</v>
@@ -5610,12 +5614,12 @@
         <v>2</v>
       </c>
       <c r="O27" s="17" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="12:20" ht="24" customHeight="1">
       <c r="L28" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M28" s="17" t="s">
         <v>52</v>
@@ -5624,113 +5628,113 @@
         <v>2</v>
       </c>
       <c r="O28" s="17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="29" spans="12:20" ht="24" customHeight="1">
       <c r="L29" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M29" s="18" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="N29" s="18">
         <v>1</v>
       </c>
       <c r="O29" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="30" spans="12:20" ht="24" customHeight="1">
       <c r="L30" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="M30" s="18" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="N30" s="18">
         <v>1</v>
       </c>
       <c r="O30" s="19" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="12:20" ht="24" customHeight="1">
       <c r="L31" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M31" s="18" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N31" s="18">
         <v>1</v>
       </c>
       <c r="O31" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="32" spans="12:20" ht="24" customHeight="1">
       <c r="L32" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M32" s="18" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="N32" s="18">
         <v>1</v>
       </c>
       <c r="O32" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" spans="12:15" ht="24" customHeight="1">
       <c r="L33" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="M33" s="18" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="N33" s="18">
         <v>1</v>
       </c>
       <c r="O33" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="34" spans="12:15" ht="24" customHeight="1">
       <c r="L34" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M34" s="18" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="N34" s="18">
         <v>1</v>
       </c>
       <c r="O34" s="19" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="35" spans="12:15" ht="24" customHeight="1">
       <c r="L35" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M35" s="18" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="N35" s="18">
         <v>1</v>
       </c>
       <c r="O35" s="19" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="36" spans="12:15" ht="24" customHeight="1">
       <c r="L36" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="M36" s="18" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="N36" s="18">
         <v>1</v>
@@ -5741,21 +5745,21 @@
     </row>
     <row r="37" spans="12:15" ht="24.75" customHeight="1">
       <c r="L37" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="M37" s="18" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="N37" s="18">
         <v>1</v>
       </c>
       <c r="O37" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="38" spans="12:15" ht="24.75" customHeight="1">
       <c r="L38" s="17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M38" s="17" t="s">
         <v>63</v>
@@ -5769,7 +5773,7 @@
     </row>
     <row r="39" spans="12:15" ht="24.75" customHeight="1">
       <c r="L39" s="17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M39" s="17" t="s">
         <v>65</v>
@@ -5783,7 +5787,7 @@
     </row>
     <row r="40" spans="12:15" ht="24.75" customHeight="1">
       <c r="L40" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M40" s="17" t="s">
         <v>66</v>
@@ -5792,12 +5796,12 @@
         <v>1</v>
       </c>
       <c r="O40" s="17" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="41" spans="12:15" ht="24.75" customHeight="1">
       <c r="L41" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M41" s="17" t="s">
         <v>39</v>
@@ -5811,7 +5815,7 @@
     </row>
     <row r="42" spans="12:15" ht="24.75" customHeight="1">
       <c r="L42" s="17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M42" s="17" t="s">
         <v>67</v>
@@ -5825,7 +5829,7 @@
     </row>
     <row r="43" spans="12:15" ht="24.75" customHeight="1">
       <c r="L43" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="M43" s="17" t="s">
         <v>53</v>
@@ -5834,12 +5838,12 @@
         <v>1</v>
       </c>
       <c r="O43" s="17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" spans="12:15" ht="24.75" customHeight="1">
       <c r="L44" s="17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="M44" s="17" t="s">
         <v>68</v>
@@ -5848,15 +5852,15 @@
         <v>1</v>
       </c>
       <c r="O44" s="17" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="45" spans="12:15" ht="24.75" customHeight="1">
       <c r="L45" s="17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="M45" s="17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N45" s="17">
         <v>1</v>
@@ -5867,7 +5871,7 @@
     </row>
     <row r="46" spans="12:15" ht="24.75" customHeight="1">
       <c r="L46" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M46" s="17" t="s">
         <v>42</v>
@@ -5876,29 +5880,29 @@
         <v>1</v>
       </c>
       <c r="O46" s="17" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="47" spans="12:15" ht="24.75" customHeight="1">
       <c r="L47" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M47" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="N47" s="17">
         <v>1</v>
       </c>
       <c r="O47" s="17" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="48" spans="12:15" ht="24.75" customHeight="1">
       <c r="L48" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="M48" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="N48" s="17">
         <v>1</v>
@@ -5909,10 +5913,10 @@
     </row>
     <row r="49" spans="12:15" ht="24.75" customHeight="1">
       <c r="L49" s="17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M49" s="17" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N49" s="17">
         <v>1</v>
@@ -5923,10 +5927,10 @@
     </row>
     <row r="50" spans="12:15" ht="24.75" customHeight="1">
       <c r="L50" s="17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="M50" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="N50" s="17">
         <v>1</v>
@@ -5937,7 +5941,7 @@
     </row>
     <row r="51" spans="12:15" ht="24.75" customHeight="1">
       <c r="L51" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M51" s="17" t="s">
         <v>58</v>
@@ -5951,10 +5955,10 @@
     </row>
     <row r="52" spans="12:15" ht="24.75" customHeight="1">
       <c r="L52" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M52" s="17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N52" s="17">
         <v>1</v>
@@ -5965,66 +5969,66 @@
     </row>
     <row r="53" spans="12:15" ht="24.75" customHeight="1">
       <c r="L53" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M53" s="19" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="N53" s="17">
         <v>1</v>
       </c>
       <c r="O53" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="12:15" ht="24.75" customHeight="1">
       <c r="L54" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M54" s="19" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="N54" s="17">
         <v>1</v>
       </c>
       <c r="O54" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="12:15" ht="24.75" customHeight="1">
       <c r="L55" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="M55" s="19" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N55" s="17">
         <v>1</v>
       </c>
       <c r="O55" s="19" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="56" spans="12:15" ht="24.75" customHeight="1">
       <c r="L56" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M56" s="19" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="N56" s="17">
         <v>1</v>
       </c>
       <c r="O56" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="12:15" ht="24.75" customHeight="1">
       <c r="L57" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M57" s="17" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="N57" s="17"/>
       <c r="O57" s="17" t="s">
@@ -6033,7 +6037,7 @@
     </row>
     <row r="58" spans="12:15" ht="24.75" customHeight="1">
       <c r="L58" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="M58" s="17"/>
       <c r="N58" s="17"/>
@@ -6041,7 +6045,7 @@
     </row>
     <row r="59" spans="12:15" ht="24.75" customHeight="1">
       <c r="L59" s="17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M59" s="17"/>
       <c r="N59" s="17"/>
@@ -6049,7 +6053,7 @@
     </row>
     <row r="60" spans="12:15" ht="24.75" customHeight="1">
       <c r="L60" s="17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="M60" s="17"/>
       <c r="N60" s="17"/>
@@ -6057,7 +6061,7 @@
     </row>
     <row r="61" spans="12:15" ht="24.75" customHeight="1">
       <c r="L61" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M61" s="17"/>
       <c r="N61" s="17"/>
@@ -6065,7 +6069,7 @@
     </row>
     <row r="62" spans="12:15" ht="24.75" customHeight="1">
       <c r="L62" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M62" s="17"/>
       <c r="N62" s="17"/>
@@ -6073,7 +6077,7 @@
     </row>
     <row r="63" spans="12:15" ht="24.75" customHeight="1">
       <c r="L63" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M63" s="17"/>
       <c r="N63" s="17"/>
@@ -6081,7 +6085,7 @@
     </row>
     <row r="64" spans="12:15" ht="24.75" customHeight="1">
       <c r="L64" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M64" s="17"/>
       <c r="N64" s="17"/>
@@ -6089,7 +6093,7 @@
     </row>
     <row r="65" spans="12:15" ht="24.75" customHeight="1">
       <c r="L65" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="M65" s="17"/>
       <c r="N65" s="17"/>
@@ -6097,7 +6101,7 @@
     </row>
     <row r="66" spans="12:15" ht="24.75" customHeight="1">
       <c r="L66" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M66" s="17"/>
       <c r="N66" s="17"/>
@@ -6105,7 +6109,7 @@
     </row>
     <row r="67" spans="12:15" ht="24.75" customHeight="1">
       <c r="L67" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M67" s="17"/>
       <c r="N67" s="17"/>
@@ -6113,7 +6117,7 @@
     </row>
     <row r="68" spans="12:15" ht="24.75" customHeight="1">
       <c r="L68" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M68" s="17"/>
       <c r="N68" s="17"/>
@@ -6121,7 +6125,7 @@
     </row>
     <row r="69" spans="12:15" ht="24.75" customHeight="1">
       <c r="L69" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M69" s="17"/>
       <c r="N69" s="17"/>
@@ -6129,7 +6133,7 @@
     </row>
     <row r="70" spans="12:15" ht="24.75" customHeight="1">
       <c r="L70" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M70" s="17"/>
       <c r="N70" s="17"/>
@@ -6137,7 +6141,7 @@
     </row>
     <row r="71" spans="12:15" ht="24.75" customHeight="1">
       <c r="L71" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M71" s="17"/>
       <c r="N71" s="17"/>
@@ -6145,7 +6149,7 @@
     </row>
     <row r="72" spans="12:15" ht="24.75" customHeight="1">
       <c r="L72" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M72" s="17"/>
       <c r="N72" s="17"/>
@@ -6153,7 +6157,7 @@
     </row>
     <row r="73" spans="12:15" ht="24.75" customHeight="1">
       <c r="L73" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M73" s="17"/>
       <c r="N73" s="17"/>
@@ -6161,7 +6165,7 @@
     </row>
     <row r="74" spans="12:15" ht="24.75" customHeight="1">
       <c r="L74" s="17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="M74" s="17"/>
       <c r="N74" s="17"/>
@@ -6169,7 +6173,7 @@
     </row>
     <row r="75" spans="12:15" ht="24.75" customHeight="1">
       <c r="L75" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M75" s="17"/>
       <c r="N75" s="17"/>
@@ -6177,7 +6181,7 @@
     </row>
     <row r="76" spans="12:15" ht="24.75" customHeight="1">
       <c r="L76" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M76" s="17"/>
       <c r="N76" s="17"/>
@@ -6185,7 +6189,7 @@
     </row>
     <row r="77" spans="12:15" ht="24.75" customHeight="1">
       <c r="L77" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M77" s="17"/>
       <c r="N77" s="17"/>
@@ -6193,7 +6197,7 @@
     </row>
     <row r="78" spans="12:15" ht="24.75" customHeight="1">
       <c r="L78" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="M78" s="17"/>
       <c r="N78" s="17"/>
@@ -6201,7 +6205,7 @@
     </row>
     <row r="79" spans="12:15" ht="24.75" customHeight="1">
       <c r="L79" s="17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M79" s="17"/>
       <c r="N79" s="17"/>
@@ -6209,7 +6213,7 @@
     </row>
     <row r="80" spans="12:15" ht="24.75" customHeight="1">
       <c r="L80" s="17" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M80" s="17"/>
       <c r="N80" s="17"/>
@@ -6217,7 +6221,7 @@
     </row>
     <row r="81" spans="12:15" ht="24.75" customHeight="1">
       <c r="L81" s="17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M81" s="17"/>
       <c r="N81" s="17"/>
@@ -6225,7 +6229,7 @@
     </row>
     <row r="82" spans="12:15" ht="24.75" customHeight="1">
       <c r="L82" s="17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="M82" s="17"/>
       <c r="N82" s="17"/>
@@ -6233,7 +6237,7 @@
     </row>
     <row r="83" spans="12:15" ht="24.75" customHeight="1">
       <c r="L83" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M83" s="17"/>
       <c r="N83" s="17"/>
@@ -6241,7 +6245,7 @@
     </row>
     <row r="84" spans="12:15" ht="24.75" customHeight="1">
       <c r="L84" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M84" s="17"/>
       <c r="N84" s="17"/>
@@ -6249,14 +6253,14 @@
     </row>
     <row r="85" spans="12:15" ht="24.75" customHeight="1">
       <c r="L85" s="17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="M85" s="17"/>
       <c r="N85" s="17"/>
       <c r="O85" s="17"/>
     </row>
   </sheetData>
-  <sortState ref="L3:O85">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L3:O85">
     <sortCondition descending="1" ref="N3:N85"/>
   </sortState>
   <mergeCells count="1">
@@ -6290,7 +6294,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="O3:O85">
+    <dataValidation type="list" allowBlank="1" sqref="O3:O85" xr:uid="{5FBE52AE-3741-4E38-B007-666BED576502}">
       <formula1>"Internazionale,Arsenal,Barcelona,Manchester City,Juventus,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6300,11 +6304,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D960C3E-E2A1-4F5E-9B7E-CC59E9774824}">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6364,13 +6368,13 @@
         <v>81</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>35</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="24" customHeight="1">
@@ -6414,13 +6418,13 @@
         <v>36</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>48</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="24" customHeight="1">
@@ -6454,7 +6458,7 @@
         <v>81</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="M3" s="10" t="s">
         <v>36</v>
@@ -6464,13 +6468,13 @@
         <v>35</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Q3" s="10" t="s">
         <v>36</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="24" customHeight="1">
@@ -6520,7 +6524,7 @@
         <v>48</v>
       </c>
       <c r="R4" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="24" customHeight="1">
@@ -6551,10 +6555,10 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M5" s="10" t="s">
         <v>48</v>
@@ -6592,7 +6596,7 @@
         <v>36</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M6" s="10" t="s">
         <v>43</v>
@@ -6630,7 +6634,7 @@
         <v>81</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M7" s="10" t="s">
         <v>37</v>
@@ -6668,7 +6672,7 @@
         <v>48</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M8" s="10" t="s">
         <v>35</v>
@@ -6706,7 +6710,7 @@
         <v>35</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M9" s="10" t="s">
         <v>81</v>
@@ -6725,10 +6729,10 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M10" s="10" t="s">
         <v>43</v>
@@ -6750,7 +6754,7 @@
         <v>36</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M11" s="10" t="s">
         <v>37</v>
@@ -6772,7 +6776,7 @@
         <v>86</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M12" s="10" t="s">
         <v>35</v>
@@ -6794,7 +6798,7 @@
         <v>81</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M13" s="10" t="s">
         <v>48</v>
@@ -6812,15 +6816,9 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="L14" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:18" ht="36" customHeight="1">
@@ -6931,10 +6929,10 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M21" s="10" t="s">
         <v>35</v>
@@ -6944,13 +6942,13 @@
         <v>36</v>
       </c>
       <c r="P21" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q21" s="10" t="s">
         <v>35</v>
       </c>
       <c r="R21" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="24" customHeight="1">
@@ -6981,10 +6979,10 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M22" s="10" t="s">
         <v>81</v>
@@ -6994,13 +6992,13 @@
         <v>43</v>
       </c>
       <c r="P22" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Q22" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R22" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="24" customHeight="1">
@@ -7031,26 +7029,26 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="N23" s="4"/>
       <c r="O23" s="10" t="s">
         <v>36</v>
       </c>
       <c r="P23" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Q23" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R23" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="24" customHeight="1">
@@ -7084,7 +7082,7 @@
         <v>81</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M24" s="10" t="s">
         <v>35</v>
@@ -7094,18 +7092,18 @@
         <v>43</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Q24" s="14" t="s">
         <v>35</v>
       </c>
       <c r="R24" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="24" customHeight="1">
       <c r="A25" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B25" s="15">
         <v>3</v>
@@ -7131,10 +7129,10 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M25" s="10" t="s">
         <v>81</v>
@@ -7172,10 +7170,10 @@
         <v>35</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N26" s="4"/>
     </row>
@@ -7206,15 +7204,9 @@
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
-      <c r="K27" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="L27" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="M27" s="10" t="s">
-        <v>36</v>
-      </c>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:18" ht="30.75" customHeight="1">
@@ -7251,7 +7243,7 @@
         <v>111</v>
       </c>
       <c r="M28" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N28" s="4"/>
     </row>
@@ -7283,13 +7275,13 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="10" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="L29" s="10" t="s">
         <v>112</v>
       </c>
       <c r="M29" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N29" s="4"/>
     </row>
@@ -7304,6 +7296,15 @@
       <c r="H30" s="15"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
+      <c r="K30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L30" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="M30" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="N30" s="4"/>
     </row>
     <row r="31" spans="1:18" ht="24" customHeight="1">
@@ -7366,30 +7367,30 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L33" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M33" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O33" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="P33" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Q33" s="10" t="s">
         <v>81</v>
       </c>
       <c r="R33" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="30" customHeight="1">
       <c r="A34" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B34" s="11">
         <v>2</v>
@@ -7415,25 +7416,25 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M34" s="10" t="s">
         <v>81</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="P34" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="Q34" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R34" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="30" customHeight="1">
@@ -7467,22 +7468,22 @@
         <v>81</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M35" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O35" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="P35" s="10" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="Q35" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R35" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="30" customHeight="1">
@@ -7513,10 +7514,10 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M36" s="10" t="s">
         <v>81</v>
@@ -7525,13 +7526,13 @@
         <v>81</v>
       </c>
       <c r="P36" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q36" s="14" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="R36" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="30" customHeight="1">
@@ -7560,18 +7561,18 @@
         <v>80</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="L37" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M37" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="30" customHeight="1">
       <c r="A38" s="11" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B38" s="11">
         <v>3</v>
@@ -7595,18 +7596,18 @@
         <v>7</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M38" s="10" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="30" customHeight="1">
       <c r="A39" s="11" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B39" s="11">
         <v>3</v>
@@ -7630,10 +7631,10 @@
         <v>5</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M39" s="10" t="s">
         <v>36</v>
@@ -7641,7 +7642,7 @@
     </row>
     <row r="40" spans="1:18" ht="30" customHeight="1">
       <c r="A40" s="12" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B40" s="12">
         <v>3</v>
@@ -7665,10 +7666,10 @@
         <v>2</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M40" s="10" t="s">
         <v>36</v>
@@ -7700,50 +7701,50 @@
         <v>1</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L41" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M41" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="30" customHeight="1">
       <c r="K42" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M42" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="30" customHeight="1">
+    <row r="46" spans="1:18">
       <c r="K46" s="10" t="s">
         <v>81</v>
       </c>
       <c r="L46" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M46" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O46" s="10" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="P46" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Q46" s="10" t="s">
         <v>81</v>
       </c>
       <c r="R46" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" ht="30" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="21">
       <c r="A47" s="9" t="s">
         <v>78</v>
       </c>
@@ -7769,10 +7770,10 @@
         <v>80</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="L47" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="M47" s="10" t="s">
         <v>35</v>
@@ -7781,16 +7782,16 @@
         <v>35</v>
       </c>
       <c r="P47" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Q47" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="R47" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" ht="30" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
       <c r="A48" s="11" t="s">
         <v>35</v>
       </c>
@@ -7819,7 +7820,7 @@
         <v>81</v>
       </c>
       <c r="L48" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M48" s="10" t="s">
         <v>36</v>
@@ -7828,16 +7829,16 @@
         <v>35</v>
       </c>
       <c r="P48" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="Q48" s="10" t="s">
         <v>81</v>
       </c>
       <c r="R48" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" ht="30" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
       <c r="A49" s="11" t="s">
         <v>81</v>
       </c>
@@ -7866,25 +7867,25 @@
         <v>35</v>
       </c>
       <c r="L49" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M49" s="10" t="s">
         <v>36</v>
       </c>
       <c r="O49" s="13" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="P49" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q49" s="14" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="R49" s="13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" ht="30" customHeight="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
       <c r="A50" s="15" t="s">
         <v>36</v>
       </c>
@@ -7913,13 +7914,13 @@
         <v>35</v>
       </c>
       <c r="L50" s="10" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="M50" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="30" customHeight="1">
+    <row r="51" spans="1:18" ht="21">
       <c r="A51" s="9" t="s">
         <v>78</v>
       </c>
@@ -7945,18 +7946,18 @@
         <v>80</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="L51" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M51" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="30" customHeight="1">
+    <row r="52" spans="1:18">
       <c r="A52" s="11" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B52" s="11">
         <v>4</v>
@@ -7979,19 +7980,10 @@
       <c r="H52" s="11">
         <v>7</v>
       </c>
-      <c r="K52" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="L52" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="M52" s="10" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" ht="30" customHeight="1">
+    </row>
+    <row r="53" spans="1:18">
       <c r="A53" s="11" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B53" s="11">
         <v>4</v>
@@ -8015,18 +8007,18 @@
         <v>5</v>
       </c>
       <c r="K53" s="10" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="L53" s="10" t="s">
-        <v>345</v>
+        <v>112</v>
       </c>
       <c r="M53" s="10" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" ht="30" customHeight="1">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
       <c r="A54" s="15" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B54" s="15">
         <v>4</v>
@@ -8050,51 +8042,61 @@
         <v>4</v>
       </c>
       <c r="K54" s="10" t="s">
-        <v>310</v>
+        <v>326</v>
       </c>
       <c r="L54" s="10" t="s">
-        <v>107</v>
+        <v>346</v>
       </c>
       <c r="M54" s="10" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" ht="30" customHeight="1">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
       <c r="K55" s="10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L55" s="10" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M55" s="10" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" ht="30" customHeight="1">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18">
       <c r="K56" s="10" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L56" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M56" s="10" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" ht="30" customHeight="1">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18">
       <c r="K57" s="10" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="L57" s="10" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="M57" s="10" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" ht="30" customHeight="1"/>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
+      <c r="K58" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="L58" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="M58" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A34:H35">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A34:H35">
     <sortCondition ref="A34:A35"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -8103,11 +8105,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042CEF4B-51C6-46DD-9493-7BEA1AB5B2B1}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="69" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:G8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8138,7 +8140,7 @@
       </c>
       <c r="G1" s="45"/>
       <c r="H1" s="35" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1">
@@ -8146,13 +8148,13 @@
         <v>18</v>
       </c>
       <c r="B2" s="36">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" s="36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" s="36">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="36">
         <v>17</v>
@@ -8202,13 +8204,13 @@
         <v>20</v>
       </c>
       <c r="B5" s="23">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="23">
+        <v>8</v>
+      </c>
+      <c r="D5" s="23">
         <v>5</v>
-      </c>
-      <c r="D5" s="23">
-        <v>3</v>
       </c>
       <c r="E5" s="23">
         <v>22</v>
@@ -8250,7 +8252,7 @@
       </c>
       <c r="G7" s="49"/>
       <c r="H7" s="40" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="24" customHeight="1">
@@ -8258,13 +8260,13 @@
         <v>18</v>
       </c>
       <c r="B8" s="41">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C8" s="41">
+        <v>4</v>
+      </c>
+      <c r="D8" s="41">
         <v>3</v>
-      </c>
-      <c r="D8" s="41">
-        <v>1</v>
       </c>
       <c r="E8" s="41">
         <v>36</v>
@@ -8317,10 +8319,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11" s="24">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E11" s="24">
         <v>18</v>
@@ -8362,7 +8364,7 @@
       </c>
       <c r="G13" s="52"/>
       <c r="H13" s="37" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="24" customHeight="1">
@@ -8370,13 +8372,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" s="38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E14" s="38">
         <v>16</v>
@@ -8418,7 +8420,7 @@
       </c>
       <c r="G16" s="54"/>
       <c r="H16" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="24" customHeight="1">
@@ -8474,7 +8476,7 @@
       </c>
       <c r="G19" s="56"/>
       <c r="H19" s="26" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="24" customHeight="1">
@@ -8538,13 +8540,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="29">
+        <v>9</v>
+      </c>
+      <c r="C23" s="29">
+        <v>5</v>
+      </c>
+      <c r="D23" s="29">
         <v>6</v>
-      </c>
-      <c r="C23" s="29">
-        <v>3</v>
-      </c>
-      <c r="D23" s="29">
-        <v>5</v>
       </c>
       <c r="E23" s="29">
         <v>22</v>

</xml_diff>

<commit_message>
Att do site para 5 torneio. Att de elenco o Madrid
</commit_message>
<xml_diff>
--- a/Dados/Dados_Torneio.xlsx
+++ b/Dados/Dados_Torneio.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Site\Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmarinho\Desktop\Site\tuf.github.io\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC306D97-E3B2-495B-9E13-C3E85AA5B0DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Artilharia" sheetId="1" r:id="rId1"/>
-    <sheet name="Melhor_jogador" sheetId="5" r:id="rId2"/>
+    <sheet name="Melhor_jogador" sheetId="5" r:id="rId1"/>
+    <sheet name="Artilharia" sheetId="1" r:id="rId2"/>
     <sheet name="Assistências" sheetId="6" r:id="rId3"/>
     <sheet name="Torneio" sheetId="9" r:id="rId4"/>
     <sheet name="KDA" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Artilharia!$A$2:$D$208</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Artilharia!$A$2:$D$208</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Assistências!$L$2:$O$85</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="360">
   <si>
     <t>Melhores Jogadores</t>
   </si>
@@ -1077,12 +1076,48 @@
   </si>
   <si>
     <t xml:space="preserve">Arsenal </t>
+  </si>
+  <si>
+    <t>Seri</t>
+  </si>
+  <si>
+    <t>Bacca</t>
+  </si>
+  <si>
+    <t>Januzaj</t>
+  </si>
+  <si>
+    <t>Hazard</t>
+  </si>
+  <si>
+    <t>C. Ronaldo</t>
+  </si>
+  <si>
+    <t>Perotti</t>
+  </si>
+  <si>
+    <t>Fernando</t>
+  </si>
+  <si>
+    <t>Salah</t>
+  </si>
+  <si>
+    <t>Messi</t>
+  </si>
+  <si>
+    <t>Ismaily</t>
+  </si>
+  <si>
+    <t>0 x 5</t>
+  </si>
+  <si>
+    <t>Neymar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="27">
     <font>
       <sz val="11"/>
@@ -1370,7 +1405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1481,6 +1516,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1698,6 +1739,122 @@
       <font>
         <b/>
         <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD2122E"/>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFED1C24"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF171616"/>
+          <bgColor rgb="FF171616"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF034694"/>
+          <bgColor rgb="FF6CA6DA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7030A0"/>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFCDBC97"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEF0107"/>
+          <bgColor rgb="FFEF0107"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color theme="3"/>
       </font>
       <fill>
@@ -1762,122 +1919,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7030A0"/>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFCDBC97"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEF0107"/>
-          <bgColor rgb="FFEF0107"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD2122E"/>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFED1C24"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF171616"/>
-          <bgColor rgb="FF171616"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF034694"/>
-          <bgColor rgb="FF6CA6DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0"/>
           <bgColor theme="1"/>
         </patternFill>
       </fill>
@@ -2112,11 +2153,233 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" customHeight="1">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+    </row>
+    <row r="2" spans="1:3" ht="24" customHeight="1">
+      <c r="A2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="24" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="24" customHeight="1">
+      <c r="A4" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="24" customHeight="1">
+      <c r="A5" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="24" customHeight="1">
+      <c r="A6" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="24" customHeight="1">
+      <c r="A7" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="24" customHeight="1">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:3" ht="24" customHeight="1">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:3" ht="24" customHeight="1">
+      <c r="A10" s="17"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:3" ht="24" customHeight="1">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:3" ht="24" customHeight="1">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+    </row>
+    <row r="13" spans="1:3" ht="24" customHeight="1">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+    </row>
+    <row r="14" spans="1:3" ht="24" customHeight="1">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+    </row>
+    <row r="15" spans="1:3" ht="24" customHeight="1">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:3" ht="24" customHeight="1">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+    </row>
+    <row r="17" spans="1:3" ht="24" customHeight="1">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+    </row>
+    <row r="18" spans="1:3" ht="24" customHeight="1">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+    </row>
+    <row r="19" spans="1:3" ht="24" customHeight="1">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+    </row>
+    <row r="20" spans="1:3" ht="24" customHeight="1">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+    </row>
+    <row r="21" spans="1:3" ht="24" customHeight="1">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+    </row>
+    <row r="22" spans="1:3" ht="24" customHeight="1">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+    </row>
+    <row r="23" spans="1:3" ht="24" customHeight="1">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+    </row>
+    <row r="24" spans="1:3" ht="24" customHeight="1">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+    </row>
+    <row r="25" spans="1:3" ht="24" customHeight="1">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+    </row>
+    <row r="26" spans="1:3" ht="24" customHeight="1">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A3:C26">
+    <cfRule type="expression" dxfId="23" priority="1">
+      <formula>$B3="Juventus"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="2">
+      <formula>$B3="Real Madrid"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="3">
+      <formula>$B3="Manchester City"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="4">
+      <formula>$B3="Bayern Munique"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="5">
+      <formula>$B3="Bayer Leverkusen"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="6">
+      <formula>$B3="Internazionale"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="7">
+      <formula>$B3="Arsenal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="8">
+      <formula>$B3="Barcelona"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="B3:B26">
+      <formula1>"Internazionale,Arsenal,Barcelona,Manchester City,Juventus,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1009"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A56"/>
+    <sheetView showWhiteSpace="0" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2139,12 +2402,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1">
@@ -2170,7 +2433,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="17">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>35</v>
@@ -2185,7 +2448,7 @@
         <v>178</v>
       </c>
       <c r="C4" s="17">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>313</v>
@@ -2196,13 +2459,13 @@
       <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="18">
-        <v>7</v>
-      </c>
-      <c r="D5" s="34" t="s">
+      <c r="B5" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="17">
+        <v>9</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>312</v>
       </c>
       <c r="F5" s="1"/>
@@ -2211,14 +2474,14 @@
       <c r="A6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="C6" s="17">
-        <v>6</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>311</v>
+      <c r="B6" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="18">
+        <v>7</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>312</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -2227,13 +2490,13 @@
         <v>13</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>72</v>
+        <v>315</v>
       </c>
       <c r="C7" s="17">
         <v>6</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -2242,13 +2505,13 @@
         <v>14</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C8" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -2257,13 +2520,13 @@
         <v>15</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C9" s="17">
-        <v>5</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>34</v>
+        <v>6</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>312</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -2272,13 +2535,13 @@
         <v>16</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C10" s="17">
         <v>5</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>34</v>
+      <c r="D10" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -2287,12 +2550,12 @@
         <v>17</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" s="17">
-        <v>4</v>
-      </c>
-      <c r="D11" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="1"/>
@@ -2302,13 +2565,13 @@
         <v>18</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C12" s="17">
-        <v>4</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>312</v>
+        <v>5</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -2320,7 +2583,7 @@
         <v>61</v>
       </c>
       <c r="C13" s="17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>312</v>
@@ -2332,13 +2595,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C14" s="17">
-        <v>3</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>313</v>
+        <v>4</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>311</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -2346,14 +2609,14 @@
       <c r="A15" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="17">
-        <v>3</v>
+      <c r="B15" s="42" t="s">
+        <v>351</v>
+      </c>
+      <c r="C15" s="43">
+        <v>4</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -2362,13 +2625,13 @@
         <v>22</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C16" s="17">
         <v>3</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>36</v>
+        <v>313</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -2377,13 +2640,13 @@
         <v>23</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>319</v>
+        <v>45</v>
       </c>
       <c r="C17" s="17">
         <v>3</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>118</v>
+        <v>36</v>
       </c>
       <c r="F17" s="1"/>
       <c r="I17" s="2"/>
@@ -2392,14 +2655,14 @@
       <c r="A18" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>69</v>
+      <c r="B18" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="C18" s="17">
         <v>3</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F18" s="1"/>
     </row>
@@ -2408,13 +2671,13 @@
         <v>25</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>66</v>
+        <v>319</v>
       </c>
       <c r="C19" s="17">
         <v>3</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>311</v>
+      <c r="D19" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -2422,14 +2685,14 @@
       <c r="A20" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>44</v>
+      <c r="B20" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="C20" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -2438,13 +2701,13 @@
         <v>27</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C21" s="17">
-        <v>2</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>36</v>
+        <v>3</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>312</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -2452,11 +2715,11 @@
       <c r="A22" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>51</v>
+      <c r="B22" s="17" t="s">
+        <v>352</v>
       </c>
       <c r="C22" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>312</v>
@@ -2468,13 +2731,13 @@
         <v>29</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C23" s="17">
         <v>2</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" s="1"/>
     </row>
@@ -2483,13 +2746,13 @@
         <v>30</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C24" s="17">
         <v>2</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -2498,13 +2761,13 @@
         <v>31</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>330</v>
+        <v>51</v>
       </c>
       <c r="C25" s="17">
         <v>2</v>
       </c>
-      <c r="D25" s="17" t="s">
-        <v>35</v>
+      <c r="D25" s="19" t="s">
+        <v>312</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -2513,7 +2776,7 @@
         <v>32</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>177</v>
+        <v>58</v>
       </c>
       <c r="C26" s="17">
         <v>2</v>
@@ -2528,13 +2791,13 @@
         <v>120</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>171</v>
+        <v>62</v>
       </c>
       <c r="C27" s="17">
         <v>2</v>
       </c>
-      <c r="D27" s="19" t="s">
-        <v>311</v>
+      <c r="D27" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="F27" s="1"/>
     </row>
@@ -2543,13 +2806,13 @@
         <v>121</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C28" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>311</v>
+        <v>35</v>
       </c>
       <c r="F28" s="1"/>
     </row>
@@ -2558,13 +2821,13 @@
         <v>122</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>337</v>
+        <v>177</v>
       </c>
       <c r="C29" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F29" s="1"/>
     </row>
@@ -2573,12 +2836,12 @@
         <v>123</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>335</v>
+        <v>171</v>
       </c>
       <c r="C30" s="17">
-        <v>1</v>
-      </c>
-      <c r="D30" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="19" t="s">
         <v>311</v>
       </c>
       <c r="F30" s="1"/>
@@ -2588,13 +2851,13 @@
         <v>124</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C31" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -2606,7 +2869,7 @@
         <v>116</v>
       </c>
       <c r="C32" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>313</v>
@@ -2618,13 +2881,13 @@
         <v>126</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="C33" s="17">
         <v>1</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="24.75" customHeight="1">
@@ -2632,13 +2895,13 @@
         <v>127</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>47</v>
+        <v>337</v>
       </c>
       <c r="C34" s="17">
         <v>1</v>
       </c>
-      <c r="D34" s="19" t="s">
-        <v>312</v>
+      <c r="D34" s="17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="24.75" customHeight="1">
@@ -2646,12 +2909,12 @@
         <v>128</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>50</v>
+        <v>334</v>
       </c>
       <c r="C35" s="17">
         <v>1</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="17" t="s">
         <v>312</v>
       </c>
     </row>
@@ -2660,13 +2923,13 @@
         <v>129</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>52</v>
+        <v>333</v>
       </c>
       <c r="C36" s="17">
         <v>1</v>
       </c>
-      <c r="D36" s="19" t="s">
-        <v>312</v>
+      <c r="D36" s="17" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="24.75" customHeight="1">
@@ -2674,7 +2937,7 @@
         <v>130</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C37" s="17">
         <v>1</v>
@@ -2688,13 +2951,13 @@
         <v>131</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C38" s="17">
         <v>1</v>
       </c>
-      <c r="D38" s="17" t="s">
-        <v>35</v>
+      <c r="D38" s="19" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="24.75" customHeight="1">
@@ -2702,13 +2965,13 @@
         <v>132</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C39" s="17">
         <v>1</v>
       </c>
-      <c r="D39" s="17" t="s">
-        <v>35</v>
+      <c r="D39" s="19" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="24.75" customHeight="1">
@@ -2716,41 +2979,41 @@
         <v>133</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C40" s="17">
         <v>1</v>
       </c>
-      <c r="D40" s="19" t="s">
-        <v>311</v>
+      <c r="D40" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="24.75" customHeight="1">
       <c r="A41" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B41" s="17" t="s">
-        <v>303</v>
+      <c r="B41" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="C41" s="17">
         <v>1</v>
       </c>
-      <c r="D41" s="19" t="s">
-        <v>311</v>
+      <c r="D41" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="24.75" customHeight="1">
       <c r="A42" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="B42" s="17" t="s">
-        <v>304</v>
+      <c r="B42" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="C42" s="17">
         <v>1</v>
       </c>
-      <c r="D42" s="17" t="s">
-        <v>84</v>
+      <c r="D42" s="19" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="24.75" customHeight="1">
@@ -2758,13 +3021,13 @@
         <v>136</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C43" s="17">
         <v>1</v>
       </c>
-      <c r="D43" s="17" t="s">
-        <v>118</v>
+      <c r="D43" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="24.75" customHeight="1">
@@ -2772,13 +3035,13 @@
         <v>137</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>64</v>
+        <v>304</v>
       </c>
       <c r="C44" s="17">
         <v>1</v>
       </c>
-      <c r="D44" s="19" t="s">
-        <v>311</v>
+      <c r="D44" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="24.75" customHeight="1">
@@ -2786,7 +3049,7 @@
         <v>138</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C45" s="17">
         <v>1</v>
@@ -2800,13 +3063,13 @@
         <v>139</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="C46" s="17">
         <v>1</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="24.75" customHeight="1">
@@ -2814,13 +3077,13 @@
         <v>140</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C47" s="17">
         <v>1</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="24.75" customHeight="1">
@@ -2828,13 +3091,13 @@
         <v>141</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>308</v>
+        <v>115</v>
       </c>
       <c r="C48" s="17">
         <v>1</v>
       </c>
-      <c r="D48" s="17" t="s">
-        <v>84</v>
+      <c r="D48" s="19" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="24.75" customHeight="1">
@@ -2842,13 +3105,13 @@
         <v>142</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>116</v>
+        <v>307</v>
       </c>
       <c r="C49" s="17">
         <v>1</v>
       </c>
-      <c r="D49" s="19" t="s">
-        <v>313</v>
+      <c r="D49" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="24.75" customHeight="1">
@@ -2856,13 +3119,13 @@
         <v>143</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>169</v>
+        <v>308</v>
       </c>
       <c r="C50" s="17">
         <v>1</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="24.75" customHeight="1">
@@ -2870,27 +3133,27 @@
         <v>144</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>309</v>
+        <v>169</v>
       </c>
       <c r="C51" s="17">
         <v>1</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="24.75" customHeight="1">
       <c r="A52" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="B52" s="19" t="s">
-        <v>316</v>
+      <c r="B52" s="17" t="s">
+        <v>309</v>
       </c>
       <c r="C52" s="17">
         <v>1</v>
       </c>
-      <c r="D52" s="19" t="s">
-        <v>34</v>
+      <c r="D52" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="24.75" customHeight="1">
@@ -2898,13 +3161,13 @@
         <v>146</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C53" s="17">
         <v>1</v>
       </c>
-      <c r="D53" s="17" t="s">
-        <v>118</v>
+      <c r="D53" s="19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="24.75" customHeight="1">
@@ -2912,13 +3175,13 @@
         <v>147</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C54" s="17">
         <v>1</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="24.75" customHeight="1">
@@ -2926,7 +3189,7 @@
         <v>148</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="C55" s="17">
         <v>1</v>
@@ -2940,77 +3203,115 @@
         <v>149</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C56" s="17">
         <v>1</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="24.75" customHeight="1">
       <c r="A57" s="17" t="s">
-        <v>141</v>
+        <v>150</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="C57" s="17">
+        <v>1</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="24.75" customHeight="1">
       <c r="A58" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
+        <v>151</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="C58" s="17">
+        <v>1</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>84</v>
+      </c>
       <c r="K58" s="3"/>
     </row>
     <row r="59" spans="1:11" ht="24.75" customHeight="1">
       <c r="A59" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
+        <v>152</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="C59" s="17">
+        <v>1</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="60" spans="1:11" ht="24.75" customHeight="1">
       <c r="A60" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
+        <v>153</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="C60" s="17">
+        <v>1</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="61" spans="1:11" ht="24.75" customHeight="1">
       <c r="A61" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
+        <v>154</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="C61" s="17">
+        <v>1</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="62" spans="1:11" ht="24.75" customHeight="1">
       <c r="A62" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
+        <v>155</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="C62" s="17">
+        <v>1</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="63" spans="1:11" ht="24.75" customHeight="1">
       <c r="A63" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-    </row>
-    <row r="64" spans="1:11" ht="24.75" customHeight="1">
-      <c r="A64" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-    </row>
+        <v>156</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="C63" s="17">
+        <v>1</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="24.75" customHeight="1"/>
     <row r="65" spans="1:4" ht="24.75" customHeight="1">
       <c r="A65" s="17" t="s">
         <v>149</v>
@@ -4965,44 +5266,44 @@
     <row r="1008" ht="15.75" customHeight="1"/>
     <row r="1009" ht="15.75" customHeight="1"/>
   </sheetData>
-  <sortState ref="A3:D1012">
-    <sortCondition descending="1" ref="C3:C1012"/>
+  <sortState ref="B3:D63">
+    <sortCondition descending="1" ref="C3:C63"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="A58:D208 A57 A3:D56">
-    <cfRule type="expression" dxfId="23" priority="41">
+  <conditionalFormatting sqref="A65:D208 A3:D63">
+    <cfRule type="expression" dxfId="15" priority="49">
       <formula>$D3="Juventus"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="42">
+    <cfRule type="expression" dxfId="14" priority="50">
       <formula>$D3="Real Madrid"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="43">
+    <cfRule type="expression" dxfId="13" priority="51">
       <formula>$D3="Manchester City"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="44">
+    <cfRule type="expression" dxfId="12" priority="52">
       <formula>$D3="Bayern Munique"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="45">
+    <cfRule type="expression" dxfId="11" priority="53">
       <formula>$D3="Bayer Leverkusen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="46">
+    <cfRule type="expression" dxfId="10" priority="54">
       <formula>$D3="Internazionale"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="47">
+    <cfRule type="expression" dxfId="9" priority="55">
       <formula>$D3="Arsenal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="48">
+    <cfRule type="expression" dxfId="8" priority="56">
       <formula>$D3="Barcelona"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" sqref="D3:D42" xr:uid="{CEF6A7C0-1AC2-4F68-8866-4B12B6E80CD5}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" sqref="D3:D42 D58 D60 D62:D63">
       <formula1>"Internazionale,Arsenal,Barcelona,Manchester City,Juventus,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D58:D208 D43:D56" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="D65:D208 D59 D61 D43:D50 D51:D57">
       <formula1>"Ajax,Arsenal,Barcelona,Liverpool,Milan,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5011,228 +5312,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5365B4F2-D15B-4A5D-9EFD-6769AA916B3D}">
-  <dimension ref="A1:C26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1">
-      <c r="A1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-    </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1">
-      <c r="A2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="24" customHeight="1">
-      <c r="A3" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1">
-      <c r="A4" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1">
-      <c r="A5" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>312</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="A6" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="24" customHeight="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-    </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" spans="1:3" ht="24" customHeight="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="17"/>
-    </row>
-    <row r="11" spans="1:3" ht="24" customHeight="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-    </row>
-    <row r="12" spans="1:3" ht="24" customHeight="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-    </row>
-    <row r="13" spans="1:3" ht="24" customHeight="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-    </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-    </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-    </row>
-    <row r="16" spans="1:3" ht="24" customHeight="1">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-    </row>
-    <row r="17" spans="1:3" ht="24" customHeight="1">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-    </row>
-    <row r="18" spans="1:3" ht="24" customHeight="1">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="1:3" ht="24" customHeight="1">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-    </row>
-    <row r="20" spans="1:3" ht="24" customHeight="1">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-    </row>
-    <row r="21" spans="1:3" ht="24" customHeight="1">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-    </row>
-    <row r="22" spans="1:3" ht="24" customHeight="1">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-    </row>
-    <row r="23" spans="1:3" ht="24" customHeight="1">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-    </row>
-    <row r="24" spans="1:3" ht="24" customHeight="1">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-    </row>
-    <row r="25" spans="1:3" ht="24" customHeight="1">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-    </row>
-    <row r="26" spans="1:3" ht="24" customHeight="1">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="A3:C26">
-    <cfRule type="expression" dxfId="15" priority="1">
-      <formula>$B3="Juventus"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2">
-      <formula>$B3="Real Madrid"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="3">
-      <formula>$B3="Manchester City"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="4">
-      <formula>$B3="Bayern Munique"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="5">
-      <formula>$B3="Bayer Leverkusen"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
-      <formula>$B3="Internazionale"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="7">
-      <formula>$B3="Arsenal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
-      <formula>$B3="Barcelona"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="B3:B26" xr:uid="{4BB2EE2B-7E6E-46C4-ADDA-EC1BF214C8F9}">
-      <formula1>"Internazionale,Arsenal,Barcelona,Manchester City,Juventus,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F94794-2326-4125-84B0-613C359A2BCD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="L1:T85"/>
   <sheetViews>
     <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="R54" sqref="R54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5244,12 +5329,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="12:15" ht="30" customHeight="1">
-      <c r="L1" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
+      <c r="L1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="12:15" ht="30" customHeight="1">
       <c r="L2" s="16" t="s">
@@ -5273,7 +5358,7 @@
         <v>54</v>
       </c>
       <c r="N3" s="17">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O3" s="17" t="s">
         <v>312</v>
@@ -5297,56 +5382,56 @@
       <c r="L5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="18">
-        <v>5</v>
-      </c>
-      <c r="O5" s="19" t="s">
-        <v>34</v>
+      <c r="M5" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5" s="17">
+        <v>6</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="12:15" ht="24" customHeight="1">
       <c r="L6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="N6" s="17">
+      <c r="M6" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="18">
         <v>5</v>
       </c>
-      <c r="O6" s="17" t="s">
-        <v>35</v>
+      <c r="O6" s="19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="12:15" ht="24" customHeight="1">
       <c r="L7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="18" t="s">
-        <v>338</v>
-      </c>
-      <c r="N7" s="18">
-        <v>4</v>
-      </c>
-      <c r="O7" s="19" t="s">
-        <v>312</v>
+      <c r="M7" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="N7" s="17">
+        <v>5</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="12:15" ht="24" customHeight="1">
       <c r="L8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="N8" s="17">
+      <c r="M8" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="N8" s="18">
         <v>4</v>
       </c>
-      <c r="O8" s="17" t="s">
-        <v>311</v>
+      <c r="O8" s="19" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="12:15" ht="24" customHeight="1">
@@ -5354,13 +5439,13 @@
         <v>15</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>115</v>
+        <v>171</v>
       </c>
       <c r="N9" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="12:15" ht="24" customHeight="1">
@@ -5368,27 +5453,27 @@
         <v>16</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N10" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O10" s="17" t="s">
-        <v>36</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="12:15" ht="24" customHeight="1">
       <c r="L11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M11" s="17" t="s">
-        <v>116</v>
+      <c r="M11" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="N11" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>313</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="12:15" ht="24" customHeight="1">
@@ -5396,13 +5481,13 @@
         <v>18</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>59</v>
+        <v>173</v>
       </c>
       <c r="N12" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>36</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="12:15" ht="24" customHeight="1">
@@ -5410,12 +5495,12 @@
         <v>19</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="N13" s="17">
-        <v>3</v>
-      </c>
-      <c r="O13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="O13" s="17" t="s">
         <v>312</v>
       </c>
     </row>
@@ -5423,28 +5508,28 @@
       <c r="L14" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="M14" s="19" t="s">
-        <v>41</v>
+      <c r="M14" s="17" t="s">
+        <v>115</v>
       </c>
       <c r="N14" s="17">
         <v>3</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>34</v>
+        <v>313</v>
       </c>
     </row>
     <row r="15" spans="12:15" ht="24" customHeight="1">
       <c r="L15" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="M15" s="19" t="s">
-        <v>321</v>
+      <c r="M15" s="17" t="s">
+        <v>119</v>
       </c>
       <c r="N15" s="17">
         <v>3</v>
       </c>
-      <c r="O15" s="19" t="s">
-        <v>311</v>
+      <c r="O15" s="17" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="12:15" ht="24" customHeight="1">
@@ -5452,13 +5537,13 @@
         <v>22</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N16" s="17">
-        <v>2</v>
-      </c>
-      <c r="O16" s="19" t="s">
-        <v>34</v>
+        <v>3</v>
+      </c>
+      <c r="O16" s="17" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="12:20" ht="24" customHeight="1">
@@ -5466,12 +5551,12 @@
         <v>23</v>
       </c>
       <c r="M17" s="17" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="N17" s="17">
-        <v>2</v>
-      </c>
-      <c r="O17" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="19" t="s">
         <v>312</v>
       </c>
     </row>
@@ -5479,14 +5564,14 @@
       <c r="L18" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="M18" s="17" t="s">
-        <v>51</v>
+      <c r="M18" s="19" t="s">
+        <v>321</v>
       </c>
       <c r="N18" s="17">
-        <v>2</v>
-      </c>
-      <c r="O18" s="17" t="s">
-        <v>312</v>
+        <v>3</v>
+      </c>
+      <c r="O18" s="19" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="19" spans="12:20" ht="24" customHeight="1">
@@ -5494,13 +5579,13 @@
         <v>25</v>
       </c>
       <c r="M19" s="17" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="N19" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="20" spans="12:20" ht="24" customHeight="1">
@@ -5508,12 +5593,12 @@
         <v>26</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="N20" s="17">
         <v>2</v>
       </c>
-      <c r="O20" s="17" t="s">
+      <c r="O20" s="19" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5522,13 +5607,13 @@
         <v>27</v>
       </c>
       <c r="M21" s="17" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="N21" s="17">
         <v>2</v>
       </c>
       <c r="O21" s="17" t="s">
-        <v>118</v>
+        <v>312</v>
       </c>
       <c r="T21" s="2"/>
     </row>
@@ -5537,13 +5622,13 @@
         <v>28</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>169</v>
+        <v>51</v>
       </c>
       <c r="N22" s="17">
         <v>2</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>35</v>
+        <v>312</v>
       </c>
       <c r="T22" s="2"/>
     </row>
@@ -5552,13 +5637,13 @@
         <v>29</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>173</v>
+        <v>62</v>
       </c>
       <c r="N23" s="17">
         <v>2</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>312</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="12:20" ht="24" customHeight="1">
@@ -5566,68 +5651,68 @@
         <v>30</v>
       </c>
       <c r="M24" s="17" t="s">
-        <v>310</v>
+        <v>117</v>
       </c>
       <c r="N24" s="17">
         <v>2</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="12:20" ht="24" customHeight="1">
       <c r="L25" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="M25" s="19" t="s">
-        <v>320</v>
+      <c r="M25" s="17" t="s">
+        <v>169</v>
       </c>
       <c r="N25" s="17">
         <v>2</v>
       </c>
       <c r="O25" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="12:20" ht="24" customHeight="1">
       <c r="L26" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="M26" s="19" t="s">
-        <v>61</v>
+      <c r="M26" s="17" t="s">
+        <v>310</v>
       </c>
       <c r="N26" s="17">
         <v>2</v>
       </c>
-      <c r="O26" s="19" t="s">
-        <v>312</v>
+      <c r="O26" s="17" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="12:20" ht="24" customHeight="1">
       <c r="L27" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="M27" s="17" t="s">
-        <v>64</v>
+      <c r="M27" s="19" t="s">
+        <v>320</v>
       </c>
       <c r="N27" s="17">
         <v>2</v>
       </c>
       <c r="O27" s="17" t="s">
-        <v>311</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="12:20" ht="24" customHeight="1">
       <c r="L28" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="M28" s="17" t="s">
-        <v>52</v>
+      <c r="M28" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="N28" s="17">
         <v>2</v>
       </c>
-      <c r="O28" s="17" t="s">
+      <c r="O28" s="19" t="s">
         <v>312</v>
       </c>
     </row>
@@ -5636,13 +5721,13 @@
         <v>122</v>
       </c>
       <c r="M29" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="N29" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O29" s="19" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="30" spans="12:20" ht="24" customHeight="1">
@@ -5650,41 +5735,41 @@
         <v>123</v>
       </c>
       <c r="M30" s="18" t="s">
-        <v>344</v>
+        <v>315</v>
       </c>
       <c r="N30" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O30" s="19" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31" spans="12:20" ht="24" customHeight="1">
       <c r="L31" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="M31" s="18" t="s">
-        <v>315</v>
-      </c>
-      <c r="N31" s="18">
-        <v>1</v>
-      </c>
-      <c r="O31" s="19" t="s">
-        <v>311</v>
+      <c r="M31" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N31" s="17">
+        <v>2</v>
+      </c>
+      <c r="O31" s="17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="12:20" ht="24" customHeight="1">
       <c r="L32" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="M32" s="18" t="s">
-        <v>343</v>
-      </c>
-      <c r="N32" s="18">
-        <v>1</v>
-      </c>
-      <c r="O32" s="19" t="s">
-        <v>311</v>
+      <c r="M32" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="N32" s="17">
+        <v>2</v>
+      </c>
+      <c r="O32" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="12:15" ht="24" customHeight="1">
@@ -5692,7 +5777,7 @@
         <v>126</v>
       </c>
       <c r="M33" s="18" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="N33" s="18">
         <v>1</v>
@@ -5706,13 +5791,13 @@
         <v>127</v>
       </c>
       <c r="M34" s="18" t="s">
-        <v>178</v>
+        <v>343</v>
       </c>
       <c r="N34" s="18">
         <v>1</v>
       </c>
       <c r="O34" s="19" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="35" spans="12:15" ht="24" customHeight="1">
@@ -5720,13 +5805,13 @@
         <v>128</v>
       </c>
       <c r="M35" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="N35" s="18">
         <v>1</v>
       </c>
       <c r="O35" s="19" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="36" spans="12:15" ht="24" customHeight="1">
@@ -5734,13 +5819,13 @@
         <v>129</v>
       </c>
       <c r="M36" s="18" t="s">
-        <v>340</v>
+        <v>178</v>
       </c>
       <c r="N36" s="18">
         <v>1</v>
       </c>
       <c r="O36" s="19" t="s">
-        <v>34</v>
+        <v>313</v>
       </c>
     </row>
     <row r="37" spans="12:15" ht="24.75" customHeight="1">
@@ -5748,41 +5833,41 @@
         <v>130</v>
       </c>
       <c r="M37" s="18" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="N37" s="18">
         <v>1</v>
       </c>
       <c r="O37" s="19" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="12:15" ht="24.75" customHeight="1">
       <c r="L38" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="M38" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="N38" s="17">
+      <c r="M38" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="N38" s="18">
         <v>1</v>
       </c>
       <c r="O38" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="12:15" ht="24.75" customHeight="1">
       <c r="L39" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="M39" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="N39" s="17">
-        <v>1</v>
-      </c>
-      <c r="O39" s="17" t="s">
-        <v>34</v>
+      <c r="M39" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="N39" s="18">
+        <v>1</v>
+      </c>
+      <c r="O39" s="19" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="40" spans="12:15" ht="24.75" customHeight="1">
@@ -5790,13 +5875,13 @@
         <v>133</v>
       </c>
       <c r="M40" s="17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N40" s="17">
         <v>1</v>
       </c>
-      <c r="O40" s="17" t="s">
-        <v>311</v>
+      <c r="O40" s="19" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="12:15" ht="24.75" customHeight="1">
@@ -5804,7 +5889,7 @@
         <v>134</v>
       </c>
       <c r="M41" s="17" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="N41" s="17">
         <v>1</v>
@@ -5818,13 +5903,13 @@
         <v>135</v>
       </c>
       <c r="M42" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N42" s="17">
         <v>1</v>
       </c>
       <c r="O42" s="17" t="s">
-        <v>36</v>
+        <v>311</v>
       </c>
     </row>
     <row r="43" spans="12:15" ht="24.75" customHeight="1">
@@ -5832,13 +5917,13 @@
         <v>136</v>
       </c>
       <c r="M43" s="17" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="N43" s="17">
         <v>1</v>
       </c>
       <c r="O43" s="17" t="s">
-        <v>312</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="12:15" ht="24.75" customHeight="1">
@@ -5846,13 +5931,13 @@
         <v>137</v>
       </c>
       <c r="M44" s="17" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="N44" s="17">
         <v>1</v>
       </c>
       <c r="O44" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="45" spans="12:15" ht="24.75" customHeight="1">
@@ -5860,13 +5945,13 @@
         <v>138</v>
       </c>
       <c r="M45" s="17" t="s">
-        <v>170</v>
+        <v>68</v>
       </c>
       <c r="N45" s="17">
         <v>1</v>
       </c>
       <c r="O45" s="17" t="s">
-        <v>84</v>
+        <v>313</v>
       </c>
     </row>
     <row r="46" spans="12:15" ht="24.75" customHeight="1">
@@ -5874,13 +5959,13 @@
         <v>139</v>
       </c>
       <c r="M46" s="17" t="s">
-        <v>42</v>
+        <v>170</v>
       </c>
       <c r="N46" s="17">
         <v>1</v>
       </c>
       <c r="O46" s="17" t="s">
-        <v>313</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="12:15" ht="24.75" customHeight="1">
@@ -5888,7 +5973,7 @@
         <v>140</v>
       </c>
       <c r="M47" s="17" t="s">
-        <v>172</v>
+        <v>42</v>
       </c>
       <c r="N47" s="17">
         <v>1</v>
@@ -5902,13 +5987,13 @@
         <v>141</v>
       </c>
       <c r="M48" s="17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="N48" s="17">
         <v>1</v>
       </c>
       <c r="O48" s="17" t="s">
-        <v>34</v>
+        <v>313</v>
       </c>
     </row>
     <row r="49" spans="12:15" ht="24.75" customHeight="1">
@@ -5916,13 +6001,13 @@
         <v>142</v>
       </c>
       <c r="M49" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N49" s="17">
         <v>1</v>
       </c>
       <c r="O49" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="12:15" ht="24.75" customHeight="1">
@@ -5930,13 +6015,13 @@
         <v>143</v>
       </c>
       <c r="M50" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N50" s="17">
         <v>1</v>
       </c>
       <c r="O50" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="12:15" ht="24.75" customHeight="1">
@@ -5944,7 +6029,7 @@
         <v>144</v>
       </c>
       <c r="M51" s="17" t="s">
-        <v>58</v>
+        <v>176</v>
       </c>
       <c r="N51" s="17">
         <v>1</v>
@@ -5958,7 +6043,7 @@
         <v>145</v>
       </c>
       <c r="M52" s="17" t="s">
-        <v>177</v>
+        <v>58</v>
       </c>
       <c r="N52" s="17">
         <v>1</v>
@@ -5971,14 +6056,14 @@
       <c r="L53" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="M53" s="19" t="s">
-        <v>322</v>
+      <c r="M53" s="17" t="s">
+        <v>177</v>
       </c>
       <c r="N53" s="17">
         <v>1</v>
       </c>
       <c r="O53" s="17" t="s">
-        <v>118</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="12:15" ht="24.75" customHeight="1">
@@ -5986,7 +6071,7 @@
         <v>147</v>
       </c>
       <c r="M54" s="19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N54" s="17">
         <v>1</v>
@@ -6000,13 +6085,13 @@
         <v>148</v>
       </c>
       <c r="M55" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N55" s="17">
         <v>1</v>
       </c>
-      <c r="O55" s="19" t="s">
-        <v>313</v>
+      <c r="O55" s="17" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="12:15" ht="24.75" customHeight="1">
@@ -6014,99 +6099,142 @@
         <v>149</v>
       </c>
       <c r="M56" s="19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="N56" s="17">
         <v>1</v>
       </c>
-      <c r="O56" s="17" t="s">
-        <v>118</v>
+      <c r="O56" s="19" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="57" spans="12:15" ht="24.75" customHeight="1">
       <c r="L57" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="M57" s="17" t="s">
-        <v>329</v>
-      </c>
-      <c r="N57" s="17"/>
+      <c r="M57" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="N57" s="17">
+        <v>1</v>
+      </c>
       <c r="O57" s="17" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="12:15" ht="24.75" customHeight="1">
       <c r="L58" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="M58" s="17"/>
-      <c r="N58" s="17"/>
-      <c r="O58" s="17"/>
+        <v>151</v>
+      </c>
+      <c r="M58" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="N58" s="17">
+        <v>1</v>
+      </c>
+      <c r="O58" s="17" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="59" spans="12:15" ht="24.75" customHeight="1">
       <c r="L59" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="M59" s="17"/>
-      <c r="N59" s="17"/>
-      <c r="O59" s="17"/>
+        <v>152</v>
+      </c>
+      <c r="M59" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="N59" s="17">
+        <v>1</v>
+      </c>
+      <c r="O59" s="17" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="60" spans="12:15" ht="24.75" customHeight="1">
       <c r="L60" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="M60" s="17"/>
-      <c r="N60" s="17"/>
-      <c r="O60" s="17"/>
+        <v>153</v>
+      </c>
+      <c r="M60" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="N60" s="17">
+        <v>1</v>
+      </c>
+      <c r="O60" s="17" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="61" spans="12:15" ht="24.75" customHeight="1">
       <c r="L61" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="M61" s="17"/>
-      <c r="N61" s="17"/>
-      <c r="O61" s="17"/>
+        <v>154</v>
+      </c>
+      <c r="M61" s="19" t="s">
+        <v>356</v>
+      </c>
+      <c r="N61" s="17">
+        <v>1</v>
+      </c>
+      <c r="O61" s="17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="62" spans="12:15" ht="24.75" customHeight="1">
       <c r="L62" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="M62" s="17"/>
-      <c r="N62" s="17"/>
-      <c r="O62" s="17"/>
+        <v>155</v>
+      </c>
+      <c r="M62" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="N62" s="17">
+        <v>1</v>
+      </c>
+      <c r="O62" s="19" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="63" spans="12:15" ht="24.75" customHeight="1">
       <c r="L63" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="M63" s="17"/>
-      <c r="N63" s="17"/>
-      <c r="O63" s="17"/>
+        <v>156</v>
+      </c>
+      <c r="M63" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="N63" s="17">
+        <v>1</v>
+      </c>
+      <c r="O63" s="19" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="64" spans="12:15" ht="24.75" customHeight="1">
       <c r="L64" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="M64" s="17"/>
-      <c r="N64" s="17"/>
-      <c r="O64" s="17"/>
+        <v>157</v>
+      </c>
+      <c r="M64" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="N64" s="17">
+        <v>1</v>
+      </c>
+      <c r="O64" s="19" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="65" spans="12:15" ht="24.75" customHeight="1">
       <c r="L65" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="M65" s="17"/>
-      <c r="N65" s="17"/>
-      <c r="O65" s="17"/>
-    </row>
-    <row r="66" spans="12:15" ht="24.75" customHeight="1">
-      <c r="L66" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="M66" s="17"/>
-      <c r="N66" s="17"/>
-      <c r="O66" s="17"/>
-    </row>
+        <v>159</v>
+      </c>
+      <c r="M65" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="N65" s="17">
+        <v>1</v>
+      </c>
+      <c r="O65" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="12:15" ht="24.75" customHeight="1"/>
     <row r="67" spans="12:15" ht="24.75" customHeight="1">
       <c r="L67" s="17" t="s">
         <v>150</v>
@@ -6260,14 +6388,14 @@
       <c r="O85" s="17"/>
     </row>
   </sheetData>
-  <sortState ref="L3:O85">
-    <sortCondition descending="1" ref="N3:N85"/>
+  <sortState ref="M2:O65">
+    <sortCondition descending="1" ref="N2:N65"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="L1:O1"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="L3:O85">
+  <conditionalFormatting sqref="L67:O85 L3:O65">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>$O3="Juventus"</formula>
     </cfRule>
@@ -6294,7 +6422,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="O3:O85" xr:uid="{5FBE52AE-3741-4E38-B007-666BED576502}">
+    <dataValidation type="list" allowBlank="1" sqref="O3:O65 O67:O85">
       <formula1>"Internazionale,Arsenal,Barcelona,Manchester City,Juventus,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6304,11 +6432,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D960C3E-E2A1-4F5E-9B7E-CC59E9774824}">
-  <dimension ref="A1:R58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P56" sqref="P56"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R68" sqref="R68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8094,21 +8222,381 @@
       </c>
     </row>
     <row r="58" spans="1:18" ht="30" customHeight="1"/>
+    <row r="60" spans="1:18" ht="30" customHeight="1">
+      <c r="A60" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="K60" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="L60" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="M60" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="O60" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="P60" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q60" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="R60" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" ht="30" customHeight="1">
+      <c r="A61" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="B61" s="11">
+        <v>3</v>
+      </c>
+      <c r="C61" s="11">
+        <v>2</v>
+      </c>
+      <c r="D61" s="11">
+        <v>0</v>
+      </c>
+      <c r="E61" s="11">
+        <v>1</v>
+      </c>
+      <c r="F61" s="11">
+        <v>4</v>
+      </c>
+      <c r="G61" s="11">
+        <v>3</v>
+      </c>
+      <c r="H61" s="11">
+        <v>6</v>
+      </c>
+      <c r="K61" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="L61" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="M61" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="O61" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="P61" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q61" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="R61" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" ht="30" customHeight="1">
+      <c r="A62" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="B62" s="11">
+        <v>3</v>
+      </c>
+      <c r="C62" s="11">
+        <v>2</v>
+      </c>
+      <c r="D62" s="11">
+        <v>0</v>
+      </c>
+      <c r="E62" s="11">
+        <v>1</v>
+      </c>
+      <c r="F62" s="11">
+        <v>3</v>
+      </c>
+      <c r="G62" s="11">
+        <v>2</v>
+      </c>
+      <c r="H62" s="11">
+        <v>6</v>
+      </c>
+      <c r="K62" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="L62" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="M62" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="O62" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P62" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q62" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="R62" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" ht="30" customHeight="1">
+      <c r="A63" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" s="15">
+        <v>3</v>
+      </c>
+      <c r="C63" s="15">
+        <v>1</v>
+      </c>
+      <c r="D63" s="15">
+        <v>0</v>
+      </c>
+      <c r="E63" s="15">
+        <v>2</v>
+      </c>
+      <c r="F63" s="15">
+        <v>2</v>
+      </c>
+      <c r="G63" s="15">
+        <v>2</v>
+      </c>
+      <c r="H63" s="15">
+        <v>3</v>
+      </c>
+      <c r="K63" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="L63" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="M63" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="O63" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="P63" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="Q63" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="R63" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" ht="30" customHeight="1">
+      <c r="A64" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="B64" s="15">
+        <v>3</v>
+      </c>
+      <c r="C64" s="15">
+        <v>1</v>
+      </c>
+      <c r="D64" s="15">
+        <v>0</v>
+      </c>
+      <c r="E64" s="15">
+        <v>2</v>
+      </c>
+      <c r="F64" s="15">
+        <v>3</v>
+      </c>
+      <c r="G64" s="15">
+        <v>5</v>
+      </c>
+      <c r="H64" s="15">
+        <v>3</v>
+      </c>
+      <c r="K64" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="L64" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="M64" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="30" customHeight="1">
+      <c r="A65" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="K65" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L65" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="M65" s="10" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="30" customHeight="1">
+      <c r="A66" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" s="11">
+        <v>2</v>
+      </c>
+      <c r="C66" s="11">
+        <v>2</v>
+      </c>
+      <c r="D66" s="11">
+        <v>0</v>
+      </c>
+      <c r="E66" s="11">
+        <v>0</v>
+      </c>
+      <c r="F66" s="11">
+        <v>3</v>
+      </c>
+      <c r="G66" s="11">
+        <v>0</v>
+      </c>
+      <c r="H66" s="11">
+        <v>6</v>
+      </c>
+      <c r="K66" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="L66" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="M66" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="30" customHeight="1">
+      <c r="A67" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67" s="11">
+        <v>2</v>
+      </c>
+      <c r="C67" s="11">
+        <v>1</v>
+      </c>
+      <c r="D67" s="11">
+        <v>0</v>
+      </c>
+      <c r="E67" s="11">
+        <v>1</v>
+      </c>
+      <c r="F67" s="11">
+        <v>1</v>
+      </c>
+      <c r="G67" s="11">
+        <v>2</v>
+      </c>
+      <c r="H67" s="11">
+        <v>3</v>
+      </c>
+      <c r="K67" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="L67" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="M67" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="30" customHeight="1">
+      <c r="A68" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B68" s="15">
+        <v>2</v>
+      </c>
+      <c r="C68" s="15">
+        <v>0</v>
+      </c>
+      <c r="D68" s="15">
+        <v>0</v>
+      </c>
+      <c r="E68" s="15">
+        <v>2</v>
+      </c>
+      <c r="F68" s="15">
+        <v>0</v>
+      </c>
+      <c r="G68" s="15">
+        <v>2</v>
+      </c>
+      <c r="H68" s="15">
+        <v>0</v>
+      </c>
+      <c r="K68" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L68" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="M68" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A34:H35">
-    <sortCondition ref="A34:A35"/>
-  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042CEF4B-51C6-46DD-9493-7BEA1AB5B2B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="69" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:G20"/>
+    <sheetView showGridLines="0" zoomScale="69" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8134,34 +8622,34 @@
       <c r="E1" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="45"/>
+      <c r="G1" s="47"/>
       <c r="H1" s="35" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1">
       <c r="A2" s="36">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" s="36">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="36">
         <v>3</v>
       </c>
       <c r="D2" s="36">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" s="36">
-        <v>17</v>
-      </c>
-      <c r="F2" s="46">
-        <v>22</v>
-      </c>
-      <c r="G2" s="46"/>
+        <v>20</v>
+      </c>
+      <c r="F2" s="48">
+        <v>27</v>
+      </c>
+      <c r="G2" s="48"/>
       <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1">
@@ -8190,34 +8678,34 @@
       <c r="E4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="47" t="s">
+      <c r="F4" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="47"/>
+      <c r="G4" s="49"/>
       <c r="H4" s="33" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="24" customHeight="1">
       <c r="A5" s="23">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="23">
         <v>8</v>
       </c>
       <c r="D5" s="23">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E5" s="23">
-        <v>22</v>
-      </c>
-      <c r="F5" s="48">
-        <v>15</v>
-      </c>
-      <c r="G5" s="48"/>
+        <v>24</v>
+      </c>
+      <c r="F5" s="50">
+        <v>17</v>
+      </c>
+      <c r="G5" s="50"/>
       <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:8" ht="24" customHeight="1">
@@ -8246,34 +8734,34 @@
       <c r="E7" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="49"/>
+      <c r="G7" s="51"/>
       <c r="H7" s="40" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="24" customHeight="1">
       <c r="A8" s="41">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B8" s="41">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" s="41">
         <v>4</v>
       </c>
       <c r="D8" s="41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8" s="41">
-        <v>36</v>
-      </c>
-      <c r="F8" s="44">
-        <v>17</v>
-      </c>
-      <c r="G8" s="44"/>
+        <v>47</v>
+      </c>
+      <c r="F8" s="46">
+        <v>21</v>
+      </c>
+      <c r="G8" s="46"/>
       <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" ht="24" customHeight="1">
@@ -8302,17 +8790,17 @@
       <c r="E10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="50" t="s">
+      <c r="F10" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="50"/>
+      <c r="G10" s="52"/>
       <c r="H10" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="24" customHeight="1">
       <c r="A11" s="24">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B11" s="24">
         <v>4</v>
@@ -8321,15 +8809,15 @@
         <v>4</v>
       </c>
       <c r="D11" s="24">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E11" s="24">
         <v>18</v>
       </c>
-      <c r="F11" s="51">
-        <v>30</v>
-      </c>
-      <c r="G11" s="51"/>
+      <c r="F11" s="53">
+        <v>32</v>
+      </c>
+      <c r="G11" s="53"/>
       <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" ht="24" customHeight="1">
@@ -8358,34 +8846,34 @@
       <c r="E13" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="52" t="s">
+      <c r="F13" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="52"/>
+      <c r="G13" s="54"/>
       <c r="H13" s="37" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="24" customHeight="1">
       <c r="A14" s="38">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B14" s="38">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C14" s="38">
         <v>4</v>
       </c>
       <c r="D14" s="38">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E14" s="38">
-        <v>16</v>
-      </c>
-      <c r="F14" s="53">
-        <v>20</v>
-      </c>
-      <c r="G14" s="53"/>
+        <v>21</v>
+      </c>
+      <c r="F14" s="55">
+        <v>28</v>
+      </c>
+      <c r="G14" s="55"/>
       <c r="H14" s="39"/>
     </row>
     <row r="15" spans="1:8" ht="24" customHeight="1">
@@ -8414,10 +8902,10 @@
       <c r="E16" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="54" t="s">
+      <c r="F16" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="54"/>
+      <c r="G16" s="56"/>
       <c r="H16" s="6" t="s">
         <v>103</v>
       </c>
@@ -8438,10 +8926,10 @@
       <c r="E17" s="25">
         <v>6</v>
       </c>
-      <c r="F17" s="55">
+      <c r="F17" s="57">
         <v>9</v>
       </c>
-      <c r="G17" s="55"/>
+      <c r="G17" s="57"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="24" customHeight="1">
@@ -8470,34 +8958,34 @@
       <c r="E19" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="56" t="s">
+      <c r="F19" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="56"/>
+      <c r="G19" s="58"/>
       <c r="H19" s="26" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="24" customHeight="1">
       <c r="A20" s="27">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B20" s="27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C20" s="27">
         <v>0</v>
       </c>
       <c r="D20" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="27">
-        <v>0</v>
-      </c>
-      <c r="F20" s="57">
-        <v>0</v>
-      </c>
-      <c r="G20" s="57"/>
+        <v>7</v>
+      </c>
+      <c r="F20" s="59">
+        <v>3</v>
+      </c>
+      <c r="G20" s="59"/>
       <c r="H20" s="32"/>
     </row>
     <row r="21" spans="1:8" ht="24" customHeight="1">
@@ -8526,34 +9014,34 @@
       <c r="E22" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="58" t="s">
+      <c r="F22" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="58"/>
+      <c r="G22" s="60"/>
       <c r="H22" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="24" customHeight="1">
       <c r="A23" s="29">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B23" s="29">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" s="29">
         <v>5</v>
       </c>
       <c r="D23" s="29">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E23" s="29">
-        <v>22</v>
-      </c>
-      <c r="F23" s="59">
-        <v>16</v>
-      </c>
-      <c r="G23" s="59"/>
+        <v>25</v>
+      </c>
+      <c r="F23" s="61">
+        <v>23</v>
+      </c>
+      <c r="G23" s="61"/>
       <c r="H23" s="32"/>
     </row>
     <row r="27" spans="1:8">

</xml_diff>

<commit_message>
Alteração de cores do sporting em planilha apenas
</commit_message>
<xml_diff>
--- a/Dados/Dados_Torneio.xlsx
+++ b/Dados/Dados_Torneio.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Site\tuf.github.io\Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmarinho\Desktop\Site\tuf.github.io\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADF3FBE-2776-4765-B43D-74B5AA76A847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Melhor_jogador" sheetId="5" r:id="rId1"/>
@@ -1190,7 +1189,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="28">
     <font>
       <sz val="11"/>
@@ -1468,7 +1467,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF003300"/>
+        <fgColor rgb="FF186E45"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1601,37 +1600,15 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1650,11 +1627,33 @@
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1665,7 +1664,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="48">
     <dxf>
       <font>
         <b/>
@@ -1708,7 +1707,7 @@
       <font>
         <b/>
         <i val="0"/>
-        <color theme="3"/>
+        <color theme="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -1771,7 +1770,7 @@
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor auto="1"/>
+          <fgColor rgb="FF044C15"/>
           <bgColor rgb="FF003300"/>
         </patternFill>
       </fill>
@@ -2004,7 +2003,64 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor theme="1"/>
+          <bgColor rgb="FF003300"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF044C15"/>
+          <bgColor rgb="FF186E45"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF005400"/>
+          <bgColor rgb="FF186E45"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF186E45"/>
         </patternFill>
       </fill>
       <border>
@@ -2110,160 +2166,6 @@
       <fill>
         <patternFill patternType="none"/>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF005400"/>
-          <bgColor rgb="FF044C15"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7030A0"/>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFCDBC97"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEF0107"/>
-          <bgColor rgb="FFEF0107"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD2122E"/>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFED1C24"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF171616"/>
-          <bgColor rgb="FF171616"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF034694"/>
-          <bgColor rgb="FF6CA6DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF044C15"/>
-          <bgColor rgb="FF003300"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2459,29 +2361,11 @@
         <patternFill patternType="none"/>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF186E45"/>
       <color rgb="FF003300"/>
       <color rgb="FF044C15"/>
       <color rgb="FF005400"/>
@@ -2491,7 +2375,6 @@
       <color rgb="FF62A0D8"/>
       <color rgb="FFA2214B"/>
       <color rgb="FFC71D3A"/>
-      <color rgb="FFED124E"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2702,7 +2585,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2717,11 +2600,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="A2" s="16" t="s">
@@ -2895,33 +2778,33 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:C26">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="25" priority="1">
       <formula>$B3="Sporting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="47" priority="2">
       <formula>$B3="Real Madrid"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="46" priority="3">
       <formula>$B3="Manchester City"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="45" priority="4">
       <formula>$B3="Bayern Munique"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="44" priority="5">
       <formula>$B3="Bayer Leverkusen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="43" priority="6">
       <formula>$B3="Internazionale"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="42" priority="7">
       <formula>$B3="Arsenal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="41" priority="8">
       <formula>$B3="Barcelona"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="B3:B26" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B3:B26">
       <formula1>"Internazionale,Arsenal,Barcelona,Manchester City,Sporting,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2930,12 +2813,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1009"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D216" sqref="D216"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2958,12 +2840,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1">
@@ -2981,7 +2863,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="24" hidden="1" customHeight="1">
+    <row r="3" spans="1:6" ht="24" customHeight="1">
       <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
@@ -3011,7 +2893,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="24" hidden="1" customHeight="1">
+    <row r="5" spans="1:6" ht="24" customHeight="1">
       <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
@@ -3026,7 +2908,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="24" hidden="1" customHeight="1">
+    <row r="6" spans="1:6" ht="24" customHeight="1">
       <c r="A6" s="17" t="s">
         <v>12</v>
       </c>
@@ -3041,7 +2923,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="24" hidden="1" customHeight="1">
+    <row r="7" spans="1:6" ht="24" customHeight="1">
       <c r="A7" s="17" t="s">
         <v>13</v>
       </c>
@@ -3056,7 +2938,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="24" hidden="1" customHeight="1">
+    <row r="8" spans="1:6" ht="24" customHeight="1">
       <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
@@ -3071,7 +2953,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="24" hidden="1" customHeight="1">
+    <row r="9" spans="1:6" ht="24" customHeight="1">
       <c r="A9" s="17" t="s">
         <v>15</v>
       </c>
@@ -3086,7 +2968,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="24" hidden="1" customHeight="1">
+    <row r="10" spans="1:6" ht="24" customHeight="1">
       <c r="A10" s="17" t="s">
         <v>16</v>
       </c>
@@ -3101,7 +2983,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="24" hidden="1" customHeight="1">
+    <row r="11" spans="1:6" ht="24" customHeight="1">
       <c r="A11" s="17" t="s">
         <v>17</v>
       </c>
@@ -3116,7 +2998,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="24" hidden="1" customHeight="1">
+    <row r="12" spans="1:6" ht="24" customHeight="1">
       <c r="A12" s="17" t="s">
         <v>18</v>
       </c>
@@ -3131,7 +3013,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="24" hidden="1" customHeight="1">
+    <row r="13" spans="1:6" ht="24" customHeight="1">
       <c r="A13" s="17" t="s">
         <v>19</v>
       </c>
@@ -3146,7 +3028,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="24" hidden="1" customHeight="1">
+    <row r="14" spans="1:6" ht="24" customHeight="1">
       <c r="A14" s="17" t="s">
         <v>20</v>
       </c>
@@ -3161,7 +3043,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="24" hidden="1" customHeight="1">
+    <row r="15" spans="1:6" ht="24" customHeight="1">
       <c r="A15" s="17" t="s">
         <v>21</v>
       </c>
@@ -3176,7 +3058,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="24" hidden="1" customHeight="1">
+    <row r="16" spans="1:6" ht="24" customHeight="1">
       <c r="A16" s="17" t="s">
         <v>22</v>
       </c>
@@ -3191,7 +3073,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="24" hidden="1" customHeight="1">
+    <row r="17" spans="1:9" ht="24" customHeight="1">
       <c r="A17" s="17" t="s">
         <v>23</v>
       </c>
@@ -3207,7 +3089,7 @@
       <c r="F17" s="1"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" ht="24" hidden="1" customHeight="1">
+    <row r="18" spans="1:9" ht="24" customHeight="1">
       <c r="A18" s="17" t="s">
         <v>24</v>
       </c>
@@ -3222,7 +3104,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="24" hidden="1" customHeight="1">
+    <row r="19" spans="1:9" ht="24" customHeight="1">
       <c r="A19" s="17" t="s">
         <v>25</v>
       </c>
@@ -3252,7 +3134,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="24" hidden="1" customHeight="1">
+    <row r="21" spans="1:9" ht="24" customHeight="1">
       <c r="A21" s="17" t="s">
         <v>27</v>
       </c>
@@ -3282,7 +3164,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="24" hidden="1" customHeight="1">
+    <row r="23" spans="1:9" ht="24" customHeight="1">
       <c r="A23" s="17" t="s">
         <v>29</v>
       </c>
@@ -3297,7 +3179,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="24" hidden="1" customHeight="1">
+    <row r="24" spans="1:9" ht="24" customHeight="1">
       <c r="A24" s="17" t="s">
         <v>30</v>
       </c>
@@ -3312,7 +3194,7 @@
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="24" hidden="1" customHeight="1">
+    <row r="25" spans="1:9" ht="24" customHeight="1">
       <c r="A25" s="17" t="s">
         <v>31</v>
       </c>
@@ -3327,7 +3209,7 @@
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="24" hidden="1" customHeight="1">
+    <row r="26" spans="1:9" ht="24" customHeight="1">
       <c r="A26" s="17" t="s">
         <v>32</v>
       </c>
@@ -3342,7 +3224,7 @@
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="24" hidden="1" customHeight="1">
+    <row r="27" spans="1:9" ht="24" customHeight="1">
       <c r="A27" s="17" t="s">
         <v>120</v>
       </c>
@@ -3372,7 +3254,7 @@
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="24" hidden="1" customHeight="1">
+    <row r="29" spans="1:9" ht="24" customHeight="1">
       <c r="A29" s="17" t="s">
         <v>122</v>
       </c>
@@ -3387,7 +3269,7 @@
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="24" hidden="1" customHeight="1">
+    <row r="30" spans="1:9" ht="24" customHeight="1">
       <c r="A30" s="17" t="s">
         <v>123</v>
       </c>
@@ -3402,7 +3284,7 @@
       </c>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="24" hidden="1" customHeight="1">
+    <row r="31" spans="1:9" ht="24" customHeight="1">
       <c r="A31" s="17" t="s">
         <v>124</v>
       </c>
@@ -3417,7 +3299,7 @@
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="24.75" hidden="1" customHeight="1">
+    <row r="32" spans="1:9" ht="24.75" customHeight="1">
       <c r="A32" s="17" t="s">
         <v>125</v>
       </c>
@@ -3432,7 +3314,7 @@
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="33" spans="1:4" ht="24.75" customHeight="1">
       <c r="A33" s="17" t="s">
         <v>126</v>
       </c>
@@ -3446,7 +3328,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="34" spans="1:4" ht="24.75" customHeight="1">
       <c r="A34" s="17" t="s">
         <v>127</v>
       </c>
@@ -3460,7 +3342,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="35" spans="1:4" ht="24.75" customHeight="1">
       <c r="A35" s="17" t="s">
         <v>128</v>
       </c>
@@ -3474,7 +3356,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="36" spans="1:4" ht="24.75" customHeight="1">
       <c r="A36" s="17" t="s">
         <v>129</v>
       </c>
@@ -3488,7 +3370,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="37" spans="1:4" ht="24.75" customHeight="1">
       <c r="A37" s="17" t="s">
         <v>130</v>
       </c>
@@ -3530,7 +3412,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="40" spans="1:4" ht="24.75" customHeight="1">
       <c r="A40" s="17" t="s">
         <v>133</v>
       </c>
@@ -3544,7 +3426,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="41" spans="1:4" ht="24.75" customHeight="1">
       <c r="A41" s="17" t="s">
         <v>134</v>
       </c>
@@ -3558,7 +3440,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="42" spans="1:4" ht="24.75" customHeight="1">
       <c r="A42" s="17" t="s">
         <v>135</v>
       </c>
@@ -3572,7 +3454,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="43" spans="1:4" ht="24.75" customHeight="1">
       <c r="A43" s="17" t="s">
         <v>136</v>
       </c>
@@ -3600,7 +3482,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="45" spans="1:4" ht="24.75" customHeight="1">
       <c r="A45" s="17" t="s">
         <v>138</v>
       </c>
@@ -3614,7 +3496,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="46" spans="1:4" ht="24.75" customHeight="1">
       <c r="A46" s="17" t="s">
         <v>139</v>
       </c>
@@ -3628,7 +3510,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="47" spans="1:4" ht="24.75" customHeight="1">
       <c r="A47" s="17" t="s">
         <v>140</v>
       </c>
@@ -3642,7 +3524,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="48" spans="1:4" ht="24.75" customHeight="1">
       <c r="A48" s="17" t="s">
         <v>141</v>
       </c>
@@ -3656,7 +3538,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="49" spans="1:11" ht="24.75" customHeight="1">
       <c r="A49" s="17" t="s">
         <v>142</v>
       </c>
@@ -3670,7 +3552,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="50" spans="1:11" ht="24.75" customHeight="1">
       <c r="A50" s="17" t="s">
         <v>143</v>
       </c>
@@ -3684,7 +3566,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="51" spans="1:11" ht="24.75" customHeight="1">
       <c r="A51" s="17" t="s">
         <v>144</v>
       </c>
@@ -3698,7 +3580,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="52" spans="1:11" ht="24.75" customHeight="1">
       <c r="A52" s="17" t="s">
         <v>145</v>
       </c>
@@ -3712,7 +3594,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="53" spans="1:11" ht="24.75" customHeight="1">
       <c r="A53" s="17" t="s">
         <v>146</v>
       </c>
@@ -3726,7 +3608,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="54" spans="1:11" ht="24.75" customHeight="1">
       <c r="A54" s="17" t="s">
         <v>147</v>
       </c>
@@ -3740,7 +3622,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="55" spans="1:11" ht="24.75" customHeight="1">
       <c r="A55" s="17" t="s">
         <v>148</v>
       </c>
@@ -3754,7 +3636,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="56" spans="1:11" ht="24.75" customHeight="1">
       <c r="A56" s="17" t="s">
         <v>149</v>
       </c>
@@ -3768,7 +3650,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="57" spans="1:11" ht="24.75" customHeight="1">
       <c r="A57" s="17" t="s">
         <v>150</v>
       </c>
@@ -3782,7 +3664,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="58" spans="1:11" ht="24.75" customHeight="1">
       <c r="A58" s="17" t="s">
         <v>151</v>
       </c>
@@ -3797,7 +3679,7 @@
       </c>
       <c r="K58" s="3"/>
     </row>
-    <row r="59" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="59" spans="1:11" ht="24.75" customHeight="1">
       <c r="A59" s="17" t="s">
         <v>152</v>
       </c>
@@ -3811,7 +3693,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="60" spans="1:11" ht="24.75" customHeight="1">
       <c r="A60" s="17" t="s">
         <v>153</v>
       </c>
@@ -3825,7 +3707,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="61" spans="1:11" ht="24.75" customHeight="1">
       <c r="A61" s="17" t="s">
         <v>154</v>
       </c>
@@ -3839,7 +3721,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="62" spans="1:11" ht="24.75" customHeight="1">
       <c r="A62" s="17" t="s">
         <v>155</v>
       </c>
@@ -3853,7 +3735,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="63" spans="1:11" ht="24.75" customHeight="1">
       <c r="A63" s="17" t="s">
         <v>156</v>
       </c>
@@ -3867,7 +3749,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="24.75" hidden="1" customHeight="1">
+    <row r="64" spans="1:11" ht="24.75" customHeight="1">
       <c r="A64" s="17" t="s">
         <v>157</v>
       </c>
@@ -3881,7 +3763,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="65" spans="1:4" ht="24.75" customHeight="1">
       <c r="A65" s="17" t="s">
         <v>158</v>
       </c>
@@ -3895,7 +3777,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="66" spans="1:4" ht="24.75" customHeight="1">
       <c r="A66" s="17" t="s">
         <v>159</v>
       </c>
@@ -3923,7 +3805,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="68" spans="1:4" ht="24.75" customHeight="1">
       <c r="A68" s="17" t="s">
         <v>161</v>
       </c>
@@ -3937,7 +3819,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="69" spans="1:4" ht="24.75" customHeight="1">
       <c r="A69" s="17" t="s">
         <v>162</v>
       </c>
@@ -3951,7 +3833,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="70" spans="1:4" ht="24.75" customHeight="1">
       <c r="A70" s="17" t="s">
         <v>163</v>
       </c>
@@ -3965,7 +3847,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="71" spans="1:4" ht="24.75" customHeight="1">
       <c r="A71" s="17" t="s">
         <v>164</v>
       </c>
@@ -3979,7 +3861,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="72" spans="1:4" ht="24.75" customHeight="1">
       <c r="A72" s="17" t="s">
         <v>165</v>
       </c>
@@ -4007,7 +3889,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="74" spans="1:4" ht="24.75" customHeight="1">
       <c r="A74" s="17" t="s">
         <v>167</v>
       </c>
@@ -4015,7 +3897,7 @@
       <c r="C74" s="17"/>
       <c r="D74" s="17"/>
     </row>
-    <row r="75" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="75" spans="1:4" ht="24.75" customHeight="1">
       <c r="A75" s="17" t="s">
         <v>168</v>
       </c>
@@ -4023,7 +3905,7 @@
       <c r="C75" s="17"/>
       <c r="D75" s="17"/>
     </row>
-    <row r="76" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="76" spans="1:4" ht="24.75" customHeight="1">
       <c r="A76" s="17" t="s">
         <v>179</v>
       </c>
@@ -4031,7 +3913,7 @@
       <c r="C76" s="17"/>
       <c r="D76" s="17"/>
     </row>
-    <row r="77" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="77" spans="1:4" ht="24.75" customHeight="1">
       <c r="A77" s="17" t="s">
         <v>180</v>
       </c>
@@ -4039,7 +3921,7 @@
       <c r="C77" s="17"/>
       <c r="D77" s="17"/>
     </row>
-    <row r="78" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="78" spans="1:4" ht="24.75" customHeight="1">
       <c r="A78" s="17" t="s">
         <v>181</v>
       </c>
@@ -4047,7 +3929,7 @@
       <c r="C78" s="17"/>
       <c r="D78" s="17"/>
     </row>
-    <row r="79" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="79" spans="1:4" ht="24.75" customHeight="1">
       <c r="A79" s="17" t="s">
         <v>182</v>
       </c>
@@ -4055,7 +3937,7 @@
       <c r="C79" s="17"/>
       <c r="D79" s="17"/>
     </row>
-    <row r="80" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="80" spans="1:4" ht="24.75" customHeight="1">
       <c r="A80" s="17" t="s">
         <v>183</v>
       </c>
@@ -4063,7 +3945,7 @@
       <c r="C80" s="17"/>
       <c r="D80" s="17"/>
     </row>
-    <row r="81" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="81" spans="1:4" ht="24.75" customHeight="1">
       <c r="A81" s="17" t="s">
         <v>184</v>
       </c>
@@ -4071,7 +3953,7 @@
       <c r="C81" s="17"/>
       <c r="D81" s="17"/>
     </row>
-    <row r="82" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="82" spans="1:4" ht="24.75" customHeight="1">
       <c r="A82" s="17" t="s">
         <v>185</v>
       </c>
@@ -4079,7 +3961,7 @@
       <c r="C82" s="17"/>
       <c r="D82" s="17"/>
     </row>
-    <row r="83" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="83" spans="1:4" ht="24.75" customHeight="1">
       <c r="A83" s="17" t="s">
         <v>186</v>
       </c>
@@ -4087,7 +3969,7 @@
       <c r="C83" s="17"/>
       <c r="D83" s="17"/>
     </row>
-    <row r="84" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="84" spans="1:4" ht="24.75" customHeight="1">
       <c r="A84" s="17" t="s">
         <v>187</v>
       </c>
@@ -4095,7 +3977,7 @@
       <c r="C84" s="17"/>
       <c r="D84" s="17"/>
     </row>
-    <row r="85" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="85" spans="1:4" ht="24.75" customHeight="1">
       <c r="A85" s="17" t="s">
         <v>188</v>
       </c>
@@ -4103,7 +3985,7 @@
       <c r="C85" s="17"/>
       <c r="D85" s="17"/>
     </row>
-    <row r="86" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="86" spans="1:4" ht="24.75" customHeight="1">
       <c r="A86" s="17" t="s">
         <v>189</v>
       </c>
@@ -4111,7 +3993,7 @@
       <c r="C86" s="17"/>
       <c r="D86" s="17"/>
     </row>
-    <row r="87" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="87" spans="1:4" ht="24.75" customHeight="1">
       <c r="A87" s="17" t="s">
         <v>190</v>
       </c>
@@ -4119,7 +4001,7 @@
       <c r="C87" s="17"/>
       <c r="D87" s="17"/>
     </row>
-    <row r="88" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="88" spans="1:4" ht="24.75" customHeight="1">
       <c r="A88" s="17" t="s">
         <v>191</v>
       </c>
@@ -4127,7 +4009,7 @@
       <c r="C88" s="17"/>
       <c r="D88" s="17"/>
     </row>
-    <row r="89" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="89" spans="1:4" ht="24.75" customHeight="1">
       <c r="A89" s="17" t="s">
         <v>192</v>
       </c>
@@ -4135,7 +4017,7 @@
       <c r="C89" s="17"/>
       <c r="D89" s="17"/>
     </row>
-    <row r="90" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="90" spans="1:4" ht="24.75" customHeight="1">
       <c r="A90" s="17" t="s">
         <v>193</v>
       </c>
@@ -4143,7 +4025,7 @@
       <c r="C90" s="17"/>
       <c r="D90" s="17"/>
     </row>
-    <row r="91" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="91" spans="1:4" ht="24.75" customHeight="1">
       <c r="A91" s="17" t="s">
         <v>194</v>
       </c>
@@ -4151,7 +4033,7 @@
       <c r="C91" s="17"/>
       <c r="D91" s="17"/>
     </row>
-    <row r="92" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="92" spans="1:4" ht="24.75" customHeight="1">
       <c r="A92" s="17" t="s">
         <v>195</v>
       </c>
@@ -4159,7 +4041,7 @@
       <c r="C92" s="17"/>
       <c r="D92" s="17"/>
     </row>
-    <row r="93" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="93" spans="1:4" ht="24.75" customHeight="1">
       <c r="A93" s="17" t="s">
         <v>196</v>
       </c>
@@ -4167,7 +4049,7 @@
       <c r="C93" s="17"/>
       <c r="D93" s="17"/>
     </row>
-    <row r="94" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="94" spans="1:4" ht="24.75" customHeight="1">
       <c r="A94" s="17" t="s">
         <v>197</v>
       </c>
@@ -4175,7 +4057,7 @@
       <c r="C94" s="17"/>
       <c r="D94" s="17"/>
     </row>
-    <row r="95" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="95" spans="1:4" ht="24.75" customHeight="1">
       <c r="A95" s="17" t="s">
         <v>198</v>
       </c>
@@ -4183,7 +4065,7 @@
       <c r="C95" s="17"/>
       <c r="D95" s="17"/>
     </row>
-    <row r="96" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="96" spans="1:4" ht="24.75" customHeight="1">
       <c r="A96" s="17" t="s">
         <v>199</v>
       </c>
@@ -4191,7 +4073,7 @@
       <c r="C96" s="17"/>
       <c r="D96" s="17"/>
     </row>
-    <row r="97" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="97" spans="1:4" ht="24.75" customHeight="1">
       <c r="A97" s="17" t="s">
         <v>200</v>
       </c>
@@ -4199,7 +4081,7 @@
       <c r="C97" s="17"/>
       <c r="D97" s="17"/>
     </row>
-    <row r="98" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="98" spans="1:4" ht="24.75" customHeight="1">
       <c r="A98" s="17" t="s">
         <v>201</v>
       </c>
@@ -4207,7 +4089,7 @@
       <c r="C98" s="17"/>
       <c r="D98" s="17"/>
     </row>
-    <row r="99" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="99" spans="1:4" ht="24.75" customHeight="1">
       <c r="A99" s="17" t="s">
         <v>202</v>
       </c>
@@ -4215,7 +4097,7 @@
       <c r="C99" s="17"/>
       <c r="D99" s="17"/>
     </row>
-    <row r="100" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="100" spans="1:4" ht="24.75" customHeight="1">
       <c r="A100" s="17" t="s">
         <v>203</v>
       </c>
@@ -4223,7 +4105,7 @@
       <c r="C100" s="17"/>
       <c r="D100" s="17"/>
     </row>
-    <row r="101" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="101" spans="1:4" ht="24.75" customHeight="1">
       <c r="A101" s="17" t="s">
         <v>204</v>
       </c>
@@ -4231,7 +4113,7 @@
       <c r="C101" s="17"/>
       <c r="D101" s="17"/>
     </row>
-    <row r="102" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="102" spans="1:4" ht="24.75" customHeight="1">
       <c r="A102" s="17" t="s">
         <v>205</v>
       </c>
@@ -4239,7 +4121,7 @@
       <c r="C102" s="17"/>
       <c r="D102" s="17"/>
     </row>
-    <row r="103" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="103" spans="1:4" ht="24.75" customHeight="1">
       <c r="A103" s="17" t="s">
         <v>206</v>
       </c>
@@ -4247,7 +4129,7 @@
       <c r="C103" s="17"/>
       <c r="D103" s="17"/>
     </row>
-    <row r="104" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="104" spans="1:4" ht="24.75" customHeight="1">
       <c r="A104" s="17" t="s">
         <v>207</v>
       </c>
@@ -4255,7 +4137,7 @@
       <c r="C104" s="17"/>
       <c r="D104" s="17"/>
     </row>
-    <row r="105" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="105" spans="1:4" ht="24.75" customHeight="1">
       <c r="A105" s="17" t="s">
         <v>208</v>
       </c>
@@ -4263,7 +4145,7 @@
       <c r="C105" s="17"/>
       <c r="D105" s="17"/>
     </row>
-    <row r="106" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="106" spans="1:4" ht="24.75" customHeight="1">
       <c r="A106" s="17" t="s">
         <v>209</v>
       </c>
@@ -4271,7 +4153,7 @@
       <c r="C106" s="17"/>
       <c r="D106" s="17"/>
     </row>
-    <row r="107" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="107" spans="1:4" ht="24.75" customHeight="1">
       <c r="A107" s="17" t="s">
         <v>210</v>
       </c>
@@ -4279,7 +4161,7 @@
       <c r="C107" s="17"/>
       <c r="D107" s="17"/>
     </row>
-    <row r="108" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="108" spans="1:4" ht="24.75" customHeight="1">
       <c r="A108" s="17" t="s">
         <v>211</v>
       </c>
@@ -4287,7 +4169,7 @@
       <c r="C108" s="17"/>
       <c r="D108" s="17"/>
     </row>
-    <row r="109" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="109" spans="1:4" ht="24.75" customHeight="1">
       <c r="A109" s="17" t="s">
         <v>212</v>
       </c>
@@ -4295,7 +4177,7 @@
       <c r="C109" s="17"/>
       <c r="D109" s="17"/>
     </row>
-    <row r="110" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="110" spans="1:4" ht="24.75" customHeight="1">
       <c r="A110" s="17" t="s">
         <v>213</v>
       </c>
@@ -4303,7 +4185,7 @@
       <c r="C110" s="17"/>
       <c r="D110" s="17"/>
     </row>
-    <row r="111" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="111" spans="1:4" ht="24.75" customHeight="1">
       <c r="A111" s="17" t="s">
         <v>214</v>
       </c>
@@ -4311,7 +4193,7 @@
       <c r="C111" s="17"/>
       <c r="D111" s="17"/>
     </row>
-    <row r="112" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="112" spans="1:4" ht="24.75" customHeight="1">
       <c r="A112" s="17" t="s">
         <v>206</v>
       </c>
@@ -4319,7 +4201,7 @@
       <c r="C112" s="17"/>
       <c r="D112" s="17"/>
     </row>
-    <row r="113" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="113" spans="1:4" ht="24.75" customHeight="1">
       <c r="A113" s="17" t="s">
         <v>207</v>
       </c>
@@ -4327,7 +4209,7 @@
       <c r="C113" s="17"/>
       <c r="D113" s="17"/>
     </row>
-    <row r="114" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="114" spans="1:4" ht="24.75" customHeight="1">
       <c r="A114" s="17" t="s">
         <v>208</v>
       </c>
@@ -4335,7 +4217,7 @@
       <c r="C114" s="17"/>
       <c r="D114" s="17"/>
     </row>
-    <row r="115" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="115" spans="1:4" ht="24.75" customHeight="1">
       <c r="A115" s="17" t="s">
         <v>209</v>
       </c>
@@ -4343,7 +4225,7 @@
       <c r="C115" s="17"/>
       <c r="D115" s="17"/>
     </row>
-    <row r="116" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="116" spans="1:4" ht="24.75" customHeight="1">
       <c r="A116" s="17" t="s">
         <v>210</v>
       </c>
@@ -4351,7 +4233,7 @@
       <c r="C116" s="17"/>
       <c r="D116" s="17"/>
     </row>
-    <row r="117" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="117" spans="1:4" ht="24.75" customHeight="1">
       <c r="A117" s="17" t="s">
         <v>211</v>
       </c>
@@ -4359,7 +4241,7 @@
       <c r="C117" s="17"/>
       <c r="D117" s="17"/>
     </row>
-    <row r="118" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="118" spans="1:4" ht="24.75" customHeight="1">
       <c r="A118" s="17" t="s">
         <v>212</v>
       </c>
@@ -4367,7 +4249,7 @@
       <c r="C118" s="17"/>
       <c r="D118" s="17"/>
     </row>
-    <row r="119" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="119" spans="1:4" ht="24.75" customHeight="1">
       <c r="A119" s="17" t="s">
         <v>213</v>
       </c>
@@ -4375,7 +4257,7 @@
       <c r="C119" s="17"/>
       <c r="D119" s="17"/>
     </row>
-    <row r="120" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="120" spans="1:4" ht="24.75" customHeight="1">
       <c r="A120" s="17" t="s">
         <v>214</v>
       </c>
@@ -4383,7 +4265,7 @@
       <c r="C120" s="17"/>
       <c r="D120" s="17"/>
     </row>
-    <row r="121" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="121" spans="1:4" ht="24.75" customHeight="1">
       <c r="A121" s="17" t="s">
         <v>215</v>
       </c>
@@ -4391,7 +4273,7 @@
       <c r="C121" s="17"/>
       <c r="D121" s="17"/>
     </row>
-    <row r="122" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="122" spans="1:4" ht="24.75" customHeight="1">
       <c r="A122" s="17" t="s">
         <v>216</v>
       </c>
@@ -4399,7 +4281,7 @@
       <c r="C122" s="17"/>
       <c r="D122" s="17"/>
     </row>
-    <row r="123" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="123" spans="1:4" ht="24.75" customHeight="1">
       <c r="A123" s="17" t="s">
         <v>217</v>
       </c>
@@ -4407,7 +4289,7 @@
       <c r="C123" s="17"/>
       <c r="D123" s="17"/>
     </row>
-    <row r="124" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="124" spans="1:4" ht="24.75" customHeight="1">
       <c r="A124" s="17" t="s">
         <v>218</v>
       </c>
@@ -4415,7 +4297,7 @@
       <c r="C124" s="17"/>
       <c r="D124" s="17"/>
     </row>
-    <row r="125" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="125" spans="1:4" ht="24.75" customHeight="1">
       <c r="A125" s="17" t="s">
         <v>219</v>
       </c>
@@ -4423,7 +4305,7 @@
       <c r="C125" s="17"/>
       <c r="D125" s="17"/>
     </row>
-    <row r="126" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="126" spans="1:4" ht="24.75" customHeight="1">
       <c r="A126" s="17" t="s">
         <v>220</v>
       </c>
@@ -4431,7 +4313,7 @@
       <c r="C126" s="17"/>
       <c r="D126" s="17"/>
     </row>
-    <row r="127" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="127" spans="1:4" ht="24.75" customHeight="1">
       <c r="A127" s="17" t="s">
         <v>221</v>
       </c>
@@ -4439,7 +4321,7 @@
       <c r="C127" s="17"/>
       <c r="D127" s="17"/>
     </row>
-    <row r="128" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="128" spans="1:4" ht="24.75" customHeight="1">
       <c r="A128" s="17" t="s">
         <v>222</v>
       </c>
@@ -4447,7 +4329,7 @@
       <c r="C128" s="17"/>
       <c r="D128" s="17"/>
     </row>
-    <row r="129" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="129" spans="1:4" ht="24.75" customHeight="1">
       <c r="A129" s="17" t="s">
         <v>223</v>
       </c>
@@ -4455,7 +4337,7 @@
       <c r="C129" s="17"/>
       <c r="D129" s="17"/>
     </row>
-    <row r="130" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="130" spans="1:4" ht="24.75" customHeight="1">
       <c r="A130" s="17" t="s">
         <v>224</v>
       </c>
@@ -4463,7 +4345,7 @@
       <c r="C130" s="17"/>
       <c r="D130" s="17"/>
     </row>
-    <row r="131" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="131" spans="1:4" ht="24.75" customHeight="1">
       <c r="A131" s="17" t="s">
         <v>225</v>
       </c>
@@ -4471,7 +4353,7 @@
       <c r="C131" s="17"/>
       <c r="D131" s="17"/>
     </row>
-    <row r="132" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="132" spans="1:4" ht="24.75" customHeight="1">
       <c r="A132" s="17" t="s">
         <v>226</v>
       </c>
@@ -4479,7 +4361,7 @@
       <c r="C132" s="17"/>
       <c r="D132" s="17"/>
     </row>
-    <row r="133" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="133" spans="1:4" ht="24.75" customHeight="1">
       <c r="A133" s="17" t="s">
         <v>227</v>
       </c>
@@ -4487,7 +4369,7 @@
       <c r="C133" s="17"/>
       <c r="D133" s="17"/>
     </row>
-    <row r="134" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="134" spans="1:4" ht="24.75" customHeight="1">
       <c r="A134" s="17" t="s">
         <v>228</v>
       </c>
@@ -4495,7 +4377,7 @@
       <c r="C134" s="17"/>
       <c r="D134" s="17"/>
     </row>
-    <row r="135" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="135" spans="1:4" ht="24.75" customHeight="1">
       <c r="A135" s="17" t="s">
         <v>229</v>
       </c>
@@ -4503,7 +4385,7 @@
       <c r="C135" s="17"/>
       <c r="D135" s="17"/>
     </row>
-    <row r="136" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="136" spans="1:4" ht="24.75" customHeight="1">
       <c r="A136" s="17" t="s">
         <v>230</v>
       </c>
@@ -4511,7 +4393,7 @@
       <c r="C136" s="17"/>
       <c r="D136" s="17"/>
     </row>
-    <row r="137" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="137" spans="1:4" ht="24.75" customHeight="1">
       <c r="A137" s="17" t="s">
         <v>231</v>
       </c>
@@ -4519,7 +4401,7 @@
       <c r="C137" s="17"/>
       <c r="D137" s="17"/>
     </row>
-    <row r="138" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="138" spans="1:4" ht="24.75" customHeight="1">
       <c r="A138" s="17" t="s">
         <v>232</v>
       </c>
@@ -4527,7 +4409,7 @@
       <c r="C138" s="17"/>
       <c r="D138" s="17"/>
     </row>
-    <row r="139" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="139" spans="1:4" ht="24.75" customHeight="1">
       <c r="A139" s="17" t="s">
         <v>233</v>
       </c>
@@ -4535,7 +4417,7 @@
       <c r="C139" s="17"/>
       <c r="D139" s="17"/>
     </row>
-    <row r="140" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="140" spans="1:4" ht="24.75" customHeight="1">
       <c r="A140" s="17" t="s">
         <v>234</v>
       </c>
@@ -4543,7 +4425,7 @@
       <c r="C140" s="17"/>
       <c r="D140" s="17"/>
     </row>
-    <row r="141" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="141" spans="1:4" ht="24.75" customHeight="1">
       <c r="A141" s="17" t="s">
         <v>235</v>
       </c>
@@ -4551,7 +4433,7 @@
       <c r="C141" s="17"/>
       <c r="D141" s="17"/>
     </row>
-    <row r="142" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="142" spans="1:4" ht="24.75" customHeight="1">
       <c r="A142" s="17" t="s">
         <v>236</v>
       </c>
@@ -4559,7 +4441,7 @@
       <c r="C142" s="17"/>
       <c r="D142" s="17"/>
     </row>
-    <row r="143" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="143" spans="1:4" ht="24.75" customHeight="1">
       <c r="A143" s="17" t="s">
         <v>237</v>
       </c>
@@ -4567,7 +4449,7 @@
       <c r="C143" s="17"/>
       <c r="D143" s="17"/>
     </row>
-    <row r="144" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="144" spans="1:4" ht="24.75" customHeight="1">
       <c r="A144" s="17" t="s">
         <v>238</v>
       </c>
@@ -4575,7 +4457,7 @@
       <c r="C144" s="17"/>
       <c r="D144" s="17"/>
     </row>
-    <row r="145" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="145" spans="1:4" ht="24.75" customHeight="1">
       <c r="A145" s="17" t="s">
         <v>239</v>
       </c>
@@ -4583,7 +4465,7 @@
       <c r="C145" s="17"/>
       <c r="D145" s="17"/>
     </row>
-    <row r="146" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="146" spans="1:4" ht="24.75" customHeight="1">
       <c r="A146" s="17" t="s">
         <v>240</v>
       </c>
@@ -4591,7 +4473,7 @@
       <c r="C146" s="17"/>
       <c r="D146" s="17"/>
     </row>
-    <row r="147" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="147" spans="1:4" ht="24.75" customHeight="1">
       <c r="A147" s="17" t="s">
         <v>241</v>
       </c>
@@ -4599,7 +4481,7 @@
       <c r="C147" s="17"/>
       <c r="D147" s="17"/>
     </row>
-    <row r="148" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="148" spans="1:4" ht="24.75" customHeight="1">
       <c r="A148" s="17" t="s">
         <v>242</v>
       </c>
@@ -4607,7 +4489,7 @@
       <c r="C148" s="17"/>
       <c r="D148" s="17"/>
     </row>
-    <row r="149" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="149" spans="1:4" ht="24.75" customHeight="1">
       <c r="A149" s="17" t="s">
         <v>243</v>
       </c>
@@ -4615,7 +4497,7 @@
       <c r="C149" s="17"/>
       <c r="D149" s="17"/>
     </row>
-    <row r="150" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="150" spans="1:4" ht="24.75" customHeight="1">
       <c r="A150" s="17" t="s">
         <v>244</v>
       </c>
@@ -4623,7 +4505,7 @@
       <c r="C150" s="17"/>
       <c r="D150" s="17"/>
     </row>
-    <row r="151" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="151" spans="1:4" ht="24.75" customHeight="1">
       <c r="A151" s="17" t="s">
         <v>245</v>
       </c>
@@ -4631,7 +4513,7 @@
       <c r="C151" s="17"/>
       <c r="D151" s="17"/>
     </row>
-    <row r="152" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="152" spans="1:4" ht="24.75" customHeight="1">
       <c r="A152" s="17" t="s">
         <v>246</v>
       </c>
@@ -4639,7 +4521,7 @@
       <c r="C152" s="17"/>
       <c r="D152" s="17"/>
     </row>
-    <row r="153" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="153" spans="1:4" ht="24.75" customHeight="1">
       <c r="A153" s="17" t="s">
         <v>247</v>
       </c>
@@ -4647,7 +4529,7 @@
       <c r="C153" s="17"/>
       <c r="D153" s="17"/>
     </row>
-    <row r="154" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="154" spans="1:4" ht="24.75" customHeight="1">
       <c r="A154" s="17" t="s">
         <v>248</v>
       </c>
@@ -4655,7 +4537,7 @@
       <c r="C154" s="17"/>
       <c r="D154" s="17"/>
     </row>
-    <row r="155" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="155" spans="1:4" ht="24.75" customHeight="1">
       <c r="A155" s="17" t="s">
         <v>249</v>
       </c>
@@ -4663,7 +4545,7 @@
       <c r="C155" s="17"/>
       <c r="D155" s="17"/>
     </row>
-    <row r="156" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="156" spans="1:4" ht="24.75" customHeight="1">
       <c r="A156" s="17" t="s">
         <v>250</v>
       </c>
@@ -4671,7 +4553,7 @@
       <c r="C156" s="17"/>
       <c r="D156" s="17"/>
     </row>
-    <row r="157" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="157" spans="1:4" ht="24.75" customHeight="1">
       <c r="A157" s="17" t="s">
         <v>251</v>
       </c>
@@ -4679,7 +4561,7 @@
       <c r="C157" s="17"/>
       <c r="D157" s="17"/>
     </row>
-    <row r="158" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="158" spans="1:4" ht="24.75" customHeight="1">
       <c r="A158" s="17" t="s">
         <v>252</v>
       </c>
@@ -4687,7 +4569,7 @@
       <c r="C158" s="17"/>
       <c r="D158" s="17"/>
     </row>
-    <row r="159" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="159" spans="1:4" ht="24.75" customHeight="1">
       <c r="A159" s="17" t="s">
         <v>253</v>
       </c>
@@ -4695,7 +4577,7 @@
       <c r="C159" s="17"/>
       <c r="D159" s="17"/>
     </row>
-    <row r="160" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="160" spans="1:4" ht="24.75" customHeight="1">
       <c r="A160" s="17" t="s">
         <v>254</v>
       </c>
@@ -4703,7 +4585,7 @@
       <c r="C160" s="17"/>
       <c r="D160" s="17"/>
     </row>
-    <row r="161" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="161" spans="1:4" ht="24.75" customHeight="1">
       <c r="A161" s="17" t="s">
         <v>255</v>
       </c>
@@ -4711,7 +4593,7 @@
       <c r="C161" s="17"/>
       <c r="D161" s="17"/>
     </row>
-    <row r="162" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="162" spans="1:4" ht="24.75" customHeight="1">
       <c r="A162" s="17" t="s">
         <v>256</v>
       </c>
@@ -4719,7 +4601,7 @@
       <c r="C162" s="17"/>
       <c r="D162" s="17"/>
     </row>
-    <row r="163" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="163" spans="1:4" ht="24.75" customHeight="1">
       <c r="A163" s="17" t="s">
         <v>257</v>
       </c>
@@ -4727,7 +4609,7 @@
       <c r="C163" s="17"/>
       <c r="D163" s="17"/>
     </row>
-    <row r="164" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="164" spans="1:4" ht="24.75" customHeight="1">
       <c r="A164" s="17" t="s">
         <v>258</v>
       </c>
@@ -4735,7 +4617,7 @@
       <c r="C164" s="17"/>
       <c r="D164" s="17"/>
     </row>
-    <row r="165" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="165" spans="1:4" ht="24.75" customHeight="1">
       <c r="A165" s="17" t="s">
         <v>259</v>
       </c>
@@ -4743,7 +4625,7 @@
       <c r="C165" s="17"/>
       <c r="D165" s="17"/>
     </row>
-    <row r="166" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="166" spans="1:4" ht="24.75" customHeight="1">
       <c r="A166" s="17" t="s">
         <v>260</v>
       </c>
@@ -4751,7 +4633,7 @@
       <c r="C166" s="17"/>
       <c r="D166" s="17"/>
     </row>
-    <row r="167" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="167" spans="1:4" ht="24.75" customHeight="1">
       <c r="A167" s="17" t="s">
         <v>261</v>
       </c>
@@ -4759,7 +4641,7 @@
       <c r="C167" s="17"/>
       <c r="D167" s="17"/>
     </row>
-    <row r="168" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="168" spans="1:4" ht="24.75" customHeight="1">
       <c r="A168" s="17" t="s">
         <v>262</v>
       </c>
@@ -4767,7 +4649,7 @@
       <c r="C168" s="17"/>
       <c r="D168" s="17"/>
     </row>
-    <row r="169" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="169" spans="1:4" ht="24.75" customHeight="1">
       <c r="A169" s="17" t="s">
         <v>263</v>
       </c>
@@ -4775,7 +4657,7 @@
       <c r="C169" s="17"/>
       <c r="D169" s="17"/>
     </row>
-    <row r="170" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="170" spans="1:4" ht="24.75" customHeight="1">
       <c r="A170" s="17" t="s">
         <v>264</v>
       </c>
@@ -4783,7 +4665,7 @@
       <c r="C170" s="17"/>
       <c r="D170" s="17"/>
     </row>
-    <row r="171" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="171" spans="1:4" ht="24.75" customHeight="1">
       <c r="A171" s="17" t="s">
         <v>265</v>
       </c>
@@ -4791,7 +4673,7 @@
       <c r="C171" s="17"/>
       <c r="D171" s="17"/>
     </row>
-    <row r="172" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="172" spans="1:4" ht="24.75" customHeight="1">
       <c r="A172" s="17" t="s">
         <v>266</v>
       </c>
@@ -4799,7 +4681,7 @@
       <c r="C172" s="17"/>
       <c r="D172" s="17"/>
     </row>
-    <row r="173" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="173" spans="1:4" ht="24.75" customHeight="1">
       <c r="A173" s="17" t="s">
         <v>267</v>
       </c>
@@ -4807,7 +4689,7 @@
       <c r="C173" s="17"/>
       <c r="D173" s="17"/>
     </row>
-    <row r="174" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="174" spans="1:4" ht="24.75" customHeight="1">
       <c r="A174" s="17" t="s">
         <v>268</v>
       </c>
@@ -4815,7 +4697,7 @@
       <c r="C174" s="17"/>
       <c r="D174" s="17"/>
     </row>
-    <row r="175" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="175" spans="1:4" ht="24.75" customHeight="1">
       <c r="A175" s="17" t="s">
         <v>269</v>
       </c>
@@ -4823,7 +4705,7 @@
       <c r="C175" s="17"/>
       <c r="D175" s="17"/>
     </row>
-    <row r="176" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="176" spans="1:4" ht="24.75" customHeight="1">
       <c r="A176" s="17" t="s">
         <v>270</v>
       </c>
@@ -4831,7 +4713,7 @@
       <c r="C176" s="17"/>
       <c r="D176" s="17"/>
     </row>
-    <row r="177" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="177" spans="1:4" ht="24.75" customHeight="1">
       <c r="A177" s="17" t="s">
         <v>271</v>
       </c>
@@ -4839,7 +4721,7 @@
       <c r="C177" s="17"/>
       <c r="D177" s="17"/>
     </row>
-    <row r="178" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="178" spans="1:4" ht="24.75" customHeight="1">
       <c r="A178" s="17" t="s">
         <v>272</v>
       </c>
@@ -4847,7 +4729,7 @@
       <c r="C178" s="17"/>
       <c r="D178" s="17"/>
     </row>
-    <row r="179" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="179" spans="1:4" ht="24.75" customHeight="1">
       <c r="A179" s="17" t="s">
         <v>273</v>
       </c>
@@ -4855,7 +4737,7 @@
       <c r="C179" s="17"/>
       <c r="D179" s="17"/>
     </row>
-    <row r="180" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="180" spans="1:4" ht="24.75" customHeight="1">
       <c r="A180" s="17" t="s">
         <v>274</v>
       </c>
@@ -4863,7 +4745,7 @@
       <c r="C180" s="17"/>
       <c r="D180" s="17"/>
     </row>
-    <row r="181" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="181" spans="1:4" ht="24.75" customHeight="1">
       <c r="A181" s="17" t="s">
         <v>275</v>
       </c>
@@ -4871,7 +4753,7 @@
       <c r="C181" s="17"/>
       <c r="D181" s="17"/>
     </row>
-    <row r="182" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="182" spans="1:4" ht="24.75" customHeight="1">
       <c r="A182" s="17" t="s">
         <v>276</v>
       </c>
@@ -4879,7 +4761,7 @@
       <c r="C182" s="17"/>
       <c r="D182" s="17"/>
     </row>
-    <row r="183" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="183" spans="1:4" ht="24.75" customHeight="1">
       <c r="A183" s="17" t="s">
         <v>277</v>
       </c>
@@ -4887,7 +4769,7 @@
       <c r="C183" s="17"/>
       <c r="D183" s="17"/>
     </row>
-    <row r="184" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="184" spans="1:4" ht="24.75" customHeight="1">
       <c r="A184" s="17" t="s">
         <v>278</v>
       </c>
@@ -4895,7 +4777,7 @@
       <c r="C184" s="17"/>
       <c r="D184" s="17"/>
     </row>
-    <row r="185" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="185" spans="1:4" ht="24.75" customHeight="1">
       <c r="A185" s="17" t="s">
         <v>279</v>
       </c>
@@ -4903,7 +4785,7 @@
       <c r="C185" s="17"/>
       <c r="D185" s="17"/>
     </row>
-    <row r="186" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="186" spans="1:4" ht="24.75" customHeight="1">
       <c r="A186" s="17" t="s">
         <v>280</v>
       </c>
@@ -4911,7 +4793,7 @@
       <c r="C186" s="17"/>
       <c r="D186" s="17"/>
     </row>
-    <row r="187" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="187" spans="1:4" ht="24.75" customHeight="1">
       <c r="A187" s="17" t="s">
         <v>281</v>
       </c>
@@ -4919,7 +4801,7 @@
       <c r="C187" s="17"/>
       <c r="D187" s="17"/>
     </row>
-    <row r="188" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="188" spans="1:4" ht="24.75" customHeight="1">
       <c r="A188" s="17" t="s">
         <v>282</v>
       </c>
@@ -4927,7 +4809,7 @@
       <c r="C188" s="17"/>
       <c r="D188" s="17"/>
     </row>
-    <row r="189" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="189" spans="1:4" ht="24.75" customHeight="1">
       <c r="A189" s="17" t="s">
         <v>283</v>
       </c>
@@ -4935,7 +4817,7 @@
       <c r="C189" s="17"/>
       <c r="D189" s="17"/>
     </row>
-    <row r="190" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="190" spans="1:4" ht="24.75" customHeight="1">
       <c r="A190" s="17" t="s">
         <v>284</v>
       </c>
@@ -4943,7 +4825,7 @@
       <c r="C190" s="17"/>
       <c r="D190" s="17"/>
     </row>
-    <row r="191" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="191" spans="1:4" ht="24.75" customHeight="1">
       <c r="A191" s="17" t="s">
         <v>285</v>
       </c>
@@ -4951,7 +4833,7 @@
       <c r="C191" s="17"/>
       <c r="D191" s="17"/>
     </row>
-    <row r="192" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="192" spans="1:4" ht="24.75" customHeight="1">
       <c r="A192" s="17" t="s">
         <v>286</v>
       </c>
@@ -4959,7 +4841,7 @@
       <c r="C192" s="17"/>
       <c r="D192" s="17"/>
     </row>
-    <row r="193" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="193" spans="1:4" ht="24.75" customHeight="1">
       <c r="A193" s="17" t="s">
         <v>287</v>
       </c>
@@ -4967,7 +4849,7 @@
       <c r="C193" s="17"/>
       <c r="D193" s="17"/>
     </row>
-    <row r="194" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="194" spans="1:4" ht="24.75" customHeight="1">
       <c r="A194" s="17" t="s">
         <v>288</v>
       </c>
@@ -4975,7 +4857,7 @@
       <c r="C194" s="17"/>
       <c r="D194" s="17"/>
     </row>
-    <row r="195" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="195" spans="1:4" ht="24.75" customHeight="1">
       <c r="A195" s="17" t="s">
         <v>289</v>
       </c>
@@ -4983,7 +4865,7 @@
       <c r="C195" s="17"/>
       <c r="D195" s="17"/>
     </row>
-    <row r="196" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="196" spans="1:4" ht="24.75" customHeight="1">
       <c r="A196" s="17" t="s">
         <v>290</v>
       </c>
@@ -4991,7 +4873,7 @@
       <c r="C196" s="17"/>
       <c r="D196" s="17"/>
     </row>
-    <row r="197" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="197" spans="1:4" ht="24.75" customHeight="1">
       <c r="A197" s="17" t="s">
         <v>291</v>
       </c>
@@ -4999,7 +4881,7 @@
       <c r="C197" s="17"/>
       <c r="D197" s="17"/>
     </row>
-    <row r="198" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="198" spans="1:4" ht="24.75" customHeight="1">
       <c r="A198" s="17" t="s">
         <v>292</v>
       </c>
@@ -5007,7 +4889,7 @@
       <c r="C198" s="17"/>
       <c r="D198" s="17"/>
     </row>
-    <row r="199" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="199" spans="1:4" ht="24.75" customHeight="1">
       <c r="A199" s="17" t="s">
         <v>293</v>
       </c>
@@ -5015,7 +4897,7 @@
       <c r="C199" s="17"/>
       <c r="D199" s="17"/>
     </row>
-    <row r="200" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="200" spans="1:4" ht="24.75" customHeight="1">
       <c r="A200" s="17" t="s">
         <v>294</v>
       </c>
@@ -5023,7 +4905,7 @@
       <c r="C200" s="17"/>
       <c r="D200" s="17"/>
     </row>
-    <row r="201" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="201" spans="1:4" ht="24.75" customHeight="1">
       <c r="A201" s="17" t="s">
         <v>295</v>
       </c>
@@ -5031,7 +4913,7 @@
       <c r="C201" s="17"/>
       <c r="D201" s="17"/>
     </row>
-    <row r="202" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="202" spans="1:4" ht="24.75" customHeight="1">
       <c r="A202" s="17" t="s">
         <v>296</v>
       </c>
@@ -5039,7 +4921,7 @@
       <c r="C202" s="17"/>
       <c r="D202" s="17"/>
     </row>
-    <row r="203" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="203" spans="1:4" ht="24.75" customHeight="1">
       <c r="A203" s="17" t="s">
         <v>297</v>
       </c>
@@ -5047,7 +4929,7 @@
       <c r="C203" s="17"/>
       <c r="D203" s="17"/>
     </row>
-    <row r="204" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="204" spans="1:4" ht="24.75" customHeight="1">
       <c r="A204" s="17" t="s">
         <v>298</v>
       </c>
@@ -5055,7 +4937,7 @@
       <c r="C204" s="17"/>
       <c r="D204" s="17"/>
     </row>
-    <row r="205" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="205" spans="1:4" ht="24.75" customHeight="1">
       <c r="A205" s="17" t="s">
         <v>299</v>
       </c>
@@ -5063,7 +4945,7 @@
       <c r="C205" s="17"/>
       <c r="D205" s="17"/>
     </row>
-    <row r="206" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="206" spans="1:4" ht="24.75" customHeight="1">
       <c r="A206" s="17" t="s">
         <v>300</v>
       </c>
@@ -5071,7 +4953,7 @@
       <c r="C206" s="17"/>
       <c r="D206" s="17"/>
     </row>
-    <row r="207" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="207" spans="1:4" ht="24.75" customHeight="1">
       <c r="A207" s="17" t="s">
         <v>301</v>
       </c>
@@ -5079,7 +4961,7 @@
       <c r="C207" s="17"/>
       <c r="D207" s="17"/>
     </row>
-    <row r="208" spans="1:4" ht="24.75" hidden="1" customHeight="1">
+    <row r="208" spans="1:4" ht="24.75" customHeight="1">
       <c r="A208" s="17" t="s">
         <v>302</v>
       </c>
@@ -5095,7 +4977,7 @@
     <row r="214" spans="4:4" ht="15.75" customHeight="1"/>
     <row r="215" spans="4:4" ht="15.75" customHeight="1"/>
     <row r="216" spans="4:4" ht="15.75" customHeight="1">
-      <c r="D216" s="60"/>
+      <c r="D216" s="43"/>
     </row>
     <row r="217" spans="4:4" ht="15.75" customHeight="1"/>
     <row r="218" spans="4:4" ht="15.75" customHeight="1"/>
@@ -5891,13 +5773,7 @@
     <row r="1008" ht="15.75" customHeight="1"/>
     <row r="1009" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A2:D208" xr:uid="{54F87435-68F9-4D5A-9FDE-BB4561CF712F}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Sporting"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:D208"/>
   <sortState ref="B3:D73">
     <sortCondition descending="1" ref="C3:C73"/>
   </sortState>
@@ -5906,36 +5782,36 @@
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="A3:D208">
-    <cfRule type="expression" dxfId="40" priority="49">
+    <cfRule type="expression" dxfId="24" priority="49">
       <formula>$D3="Sporting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="50">
+    <cfRule type="expression" dxfId="40" priority="50">
       <formula>$D3="Real Madrid"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="51">
+    <cfRule type="expression" dxfId="39" priority="51">
       <formula>$D3="Manchester City"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="52">
+    <cfRule type="expression" dxfId="38" priority="52">
       <formula>$D3="Bayern Munique"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="53">
+    <cfRule type="expression" dxfId="37" priority="53">
       <formula>$D3="Bayer Leverkusen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="54">
+    <cfRule type="expression" dxfId="36" priority="54">
       <formula>$D3="Internazionale"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="55">
+    <cfRule type="expression" dxfId="35" priority="55">
       <formula>$D3="Arsenal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="56">
+    <cfRule type="expression" dxfId="34" priority="56">
       <formula>$D3="Barcelona"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" sqref="D3:D42 D58 D60 D62:D111" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" sqref="D3:D42 D58 D60 D62:D111">
       <formula1>"Internazionale,Arsenal,Barcelona,Manchester City,Sporting,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D59 D61 D43:D57 D112:D208" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="D59 D61 D43:D57 D112:D208">
       <formula1>"Ajax,Arsenal,Barcelona,Liverpool,Milan,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5945,12 +5821,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="L1:T88"/>
   <sheetViews>
-    <sheetView topLeftCell="L8" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView topLeftCell="L1" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5962,12 +5837,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="12:15" ht="30" customHeight="1">
-      <c r="L1" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
+      <c r="L1" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
     </row>
     <row r="2" spans="12:15" ht="30" customHeight="1">
       <c r="L2" s="16" t="s">
@@ -5983,7 +5858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="3" spans="12:15" ht="24" customHeight="1">
       <c r="L3" s="17" t="s">
         <v>9</v>
       </c>
@@ -5997,7 +5872,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="4" spans="12:15" ht="24" customHeight="1">
       <c r="L4" s="17" t="s">
         <v>10</v>
       </c>
@@ -6011,7 +5886,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="5" spans="12:15" ht="24" customHeight="1">
       <c r="L5" s="17" t="s">
         <v>11</v>
       </c>
@@ -6025,7 +5900,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="6" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="6" spans="12:15" ht="24" customHeight="1">
       <c r="L6" s="17" t="s">
         <v>12</v>
       </c>
@@ -6039,7 +5914,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="7" spans="12:15" ht="24" customHeight="1">
       <c r="L7" s="17" t="s">
         <v>13</v>
       </c>
@@ -6067,7 +5942,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="9" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="9" spans="12:15" ht="24" customHeight="1">
       <c r="L9" s="17" t="s">
         <v>15</v>
       </c>
@@ -6095,7 +5970,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="11" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="11" spans="12:15" ht="24" customHeight="1">
       <c r="L11" s="17" t="s">
         <v>17</v>
       </c>
@@ -6109,7 +5984,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="12" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="12" spans="12:15" ht="24" customHeight="1">
       <c r="L12" s="17" t="s">
         <v>18</v>
       </c>
@@ -6123,7 +5998,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="13" spans="12:15" ht="24" customHeight="1">
       <c r="L13" s="17" t="s">
         <v>19</v>
       </c>
@@ -6137,7 +6012,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="14" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="14" spans="12:15" ht="24" customHeight="1">
       <c r="L14" s="17" t="s">
         <v>20</v>
       </c>
@@ -6151,7 +6026,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="15" spans="12:15" ht="24" customHeight="1">
       <c r="L15" s="17" t="s">
         <v>21</v>
       </c>
@@ -6165,7 +6040,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="16" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="16" spans="12:15" ht="24" customHeight="1">
       <c r="L16" s="17" t="s">
         <v>22</v>
       </c>
@@ -6179,7 +6054,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="17" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="17" spans="12:20" ht="24" customHeight="1">
       <c r="L17" s="17" t="s">
         <v>23</v>
       </c>
@@ -6193,7 +6068,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="18" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="18" spans="12:20" ht="24" customHeight="1">
       <c r="L18" s="17" t="s">
         <v>24</v>
       </c>
@@ -6221,7 +6096,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="20" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="20" spans="12:20" ht="24" customHeight="1">
       <c r="L20" s="17" t="s">
         <v>26</v>
       </c>
@@ -6235,7 +6110,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="21" spans="12:20" ht="24" customHeight="1">
       <c r="L21" s="17" t="s">
         <v>27</v>
       </c>
@@ -6250,7 +6125,7 @@
       </c>
       <c r="T21" s="2"/>
     </row>
-    <row r="22" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="22" spans="12:20" ht="24" customHeight="1">
       <c r="L22" s="17" t="s">
         <v>28</v>
       </c>
@@ -6265,7 +6140,7 @@
       </c>
       <c r="T22" s="2"/>
     </row>
-    <row r="23" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="23" spans="12:20" ht="24" customHeight="1">
       <c r="L23" s="17" t="s">
         <v>29</v>
       </c>
@@ -6279,7 +6154,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="24" spans="12:20" ht="24" customHeight="1">
       <c r="L24" s="17" t="s">
         <v>30</v>
       </c>
@@ -6293,7 +6168,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="25" spans="12:20" ht="24" customHeight="1">
       <c r="L25" s="17" t="s">
         <v>31</v>
       </c>
@@ -6307,7 +6182,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="26" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="26" spans="12:20" ht="24" customHeight="1">
       <c r="L26" s="17" t="s">
         <v>32</v>
       </c>
@@ -6321,7 +6196,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="27" spans="12:20" ht="24" customHeight="1">
       <c r="L27" s="17" t="s">
         <v>120</v>
       </c>
@@ -6335,7 +6210,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="28" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="28" spans="12:20" ht="24" customHeight="1">
       <c r="L28" s="17" t="s">
         <v>121</v>
       </c>
@@ -6349,7 +6224,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="29" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="29" spans="12:20" ht="24" customHeight="1">
       <c r="L29" s="17" t="s">
         <v>122</v>
       </c>
@@ -6363,7 +6238,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="30" spans="12:20" ht="24" customHeight="1">
       <c r="L30" s="17" t="s">
         <v>123</v>
       </c>
@@ -6377,7 +6252,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="12:20" ht="24" hidden="1" customHeight="1">
+    <row r="31" spans="12:20" ht="24" customHeight="1">
       <c r="L31" s="17" t="s">
         <v>124</v>
       </c>
@@ -6405,7 +6280,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="33" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="33" spans="12:15" ht="24" customHeight="1">
       <c r="L33" s="17" t="s">
         <v>126</v>
       </c>
@@ -6419,7 +6294,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="34" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="34" spans="12:15" ht="24" customHeight="1">
       <c r="L34" s="17" t="s">
         <v>127</v>
       </c>
@@ -6433,7 +6308,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="35" spans="12:15" ht="24" customHeight="1">
       <c r="L35" s="17" t="s">
         <v>128</v>
       </c>
@@ -6447,7 +6322,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="12:15" ht="24" hidden="1" customHeight="1">
+    <row r="36" spans="12:15" ht="24" customHeight="1">
       <c r="L36" s="17" t="s">
         <v>129</v>
       </c>
@@ -6461,7 +6336,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="37" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="37" spans="12:15" ht="24.75" customHeight="1">
       <c r="L37" s="17" t="s">
         <v>130</v>
       </c>
@@ -6475,7 +6350,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="38" spans="12:15" ht="24.75" customHeight="1">
       <c r="L38" s="17" t="s">
         <v>131</v>
       </c>
@@ -6489,7 +6364,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="39" spans="12:15" ht="24.75" customHeight="1">
       <c r="L39" s="17" t="s">
         <v>132</v>
       </c>
@@ -6503,7 +6378,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="40" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="40" spans="12:15" ht="24.75" customHeight="1">
       <c r="L40" s="17" t="s">
         <v>133</v>
       </c>
@@ -6545,7 +6420,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="43" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="43" spans="12:15" ht="24.75" customHeight="1">
       <c r="L43" s="17" t="s">
         <v>136</v>
       </c>
@@ -6559,7 +6434,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="44" spans="12:15" ht="24.75" customHeight="1">
       <c r="L44" s="17" t="s">
         <v>137</v>
       </c>
@@ -6573,7 +6448,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="45" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="45" spans="12:15" ht="24.75" customHeight="1">
       <c r="L45" s="17" t="s">
         <v>138</v>
       </c>
@@ -6587,7 +6462,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="46" spans="12:15" ht="24.75" customHeight="1">
       <c r="L46" s="17" t="s">
         <v>139</v>
       </c>
@@ -6601,7 +6476,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="47" spans="12:15" ht="24.75" customHeight="1">
       <c r="L47" s="17" t="s">
         <v>140</v>
       </c>
@@ -6615,7 +6490,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="48" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="48" spans="12:15" ht="24.75" customHeight="1">
       <c r="L48" s="17" t="s">
         <v>141</v>
       </c>
@@ -6629,7 +6504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="49" spans="12:15" ht="24.75" customHeight="1">
       <c r="L49" s="17" t="s">
         <v>142</v>
       </c>
@@ -6657,7 +6532,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="51" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="51" spans="12:15" ht="24.75" customHeight="1">
       <c r="L51" s="17" t="s">
         <v>144</v>
       </c>
@@ -6699,7 +6574,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="54" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="54" spans="12:15" ht="24.75" customHeight="1">
       <c r="L54" s="17" t="s">
         <v>147</v>
       </c>
@@ -6713,7 +6588,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="55" spans="12:15" ht="24.75" customHeight="1">
       <c r="L55" s="17" t="s">
         <v>148</v>
       </c>
@@ -6727,7 +6602,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="56" spans="12:15" ht="24.75" customHeight="1">
       <c r="L56" s="17" t="s">
         <v>149</v>
       </c>
@@ -6741,7 +6616,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="57" spans="12:15" ht="24.75" customHeight="1">
       <c r="L57" s="17" t="s">
         <v>150</v>
       </c>
@@ -6755,7 +6630,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="58" spans="12:15" ht="24.75" customHeight="1">
       <c r="L58" s="17" t="s">
         <v>151</v>
       </c>
@@ -6769,7 +6644,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="59" spans="12:15" ht="24.75" customHeight="1">
       <c r="L59" s="17" t="s">
         <v>152</v>
       </c>
@@ -6783,7 +6658,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="60" spans="12:15" ht="24.75" customHeight="1">
       <c r="L60" s="17" t="s">
         <v>153</v>
       </c>
@@ -6811,7 +6686,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="62" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="62" spans="12:15" ht="24.75" customHeight="1">
       <c r="L62" s="17" t="s">
         <v>155</v>
       </c>
@@ -6825,7 +6700,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="63" spans="12:15" ht="24.75" customHeight="1">
       <c r="L63" s="17" t="s">
         <v>156</v>
       </c>
@@ -6839,7 +6714,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="64" spans="12:15" ht="24.75" customHeight="1">
       <c r="L64" s="17" t="s">
         <v>157</v>
       </c>
@@ -6853,7 +6728,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="65" spans="12:15" ht="24.75" customHeight="1">
       <c r="L65" s="17" t="s">
         <v>159</v>
       </c>
@@ -6867,7 +6742,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="66" spans="12:15" ht="24.75" customHeight="1">
       <c r="L66" s="17" t="s">
         <v>160</v>
       </c>
@@ -6881,7 +6756,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="67" spans="12:15" ht="24.75" customHeight="1">
       <c r="L67" s="17" t="s">
         <v>161</v>
       </c>
@@ -6909,7 +6784,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="69" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="69" spans="12:15" ht="24.75" customHeight="1">
       <c r="L69" s="17" t="s">
         <v>163</v>
       </c>
@@ -6937,7 +6812,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="71" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="71" spans="12:15" ht="24.75" customHeight="1">
       <c r="L71" s="17" t="s">
         <v>165</v>
       </c>
@@ -6951,7 +6826,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="72" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="72" spans="12:15" ht="24.75" customHeight="1">
       <c r="L72" s="17" t="s">
         <v>166</v>
       </c>
@@ -6965,7 +6840,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="73" spans="12:15" ht="24.75" customHeight="1">
       <c r="L73" s="17" t="s">
         <v>167</v>
       </c>
@@ -6979,7 +6854,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="74" spans="12:15" ht="24.75" customHeight="1">
       <c r="L74" s="17" t="s">
         <v>168</v>
       </c>
@@ -6993,7 +6868,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="75" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="75" spans="12:15" ht="24.75" customHeight="1">
       <c r="L75" s="17" t="s">
         <v>179</v>
       </c>
@@ -7007,7 +6882,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="76" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="76" spans="12:15" ht="24.75" customHeight="1">
       <c r="L76" s="17" t="s">
         <v>180</v>
       </c>
@@ -7021,7 +6896,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="77" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="77" spans="12:15" ht="24.75" customHeight="1">
       <c r="L77" s="17" t="s">
         <v>181</v>
       </c>
@@ -7035,7 +6910,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="78" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="78" spans="12:15" ht="24.75" customHeight="1">
       <c r="L78" s="17" t="s">
         <v>182</v>
       </c>
@@ -7049,7 +6924,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="79" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="79" spans="12:15" ht="24.75" customHeight="1">
       <c r="L79" s="17" t="s">
         <v>183</v>
       </c>
@@ -7063,7 +6938,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="12:15" ht="24.75" hidden="1" customHeight="1">
+    <row r="80" spans="12:15" ht="24.75" customHeight="1">
       <c r="L80" s="17" t="s">
         <v>184</v>
       </c>
@@ -7071,7 +6946,7 @@
       <c r="N80" s="17"/>
       <c r="O80" s="19"/>
     </row>
-    <row r="81" spans="12:15" ht="24.95" hidden="1" customHeight="1">
+    <row r="81" spans="12:15" ht="24.95" customHeight="1">
       <c r="L81" s="17" t="s">
         <v>185</v>
       </c>
@@ -7079,7 +6954,7 @@
       <c r="N81" s="17"/>
       <c r="O81" s="19"/>
     </row>
-    <row r="82" spans="12:15" ht="24.95" hidden="1" customHeight="1">
+    <row r="82" spans="12:15" ht="24.95" customHeight="1">
       <c r="L82" s="17" t="s">
         <v>186</v>
       </c>
@@ -7087,7 +6962,7 @@
       <c r="N82" s="17"/>
       <c r="O82" s="19"/>
     </row>
-    <row r="83" spans="12:15" ht="24.95" hidden="1" customHeight="1">
+    <row r="83" spans="12:15" ht="24.95" customHeight="1">
       <c r="L83" s="17" t="s">
         <v>187</v>
       </c>
@@ -7095,7 +6970,7 @@
       <c r="N83" s="17"/>
       <c r="O83" s="19"/>
     </row>
-    <row r="84" spans="12:15" ht="24.95" hidden="1" customHeight="1">
+    <row r="84" spans="12:15" ht="24.95" customHeight="1">
       <c r="L84" s="17" t="s">
         <v>188</v>
       </c>
@@ -7103,7 +6978,7 @@
       <c r="N84" s="17"/>
       <c r="O84" s="19"/>
     </row>
-    <row r="85" spans="12:15" ht="24.95" hidden="1" customHeight="1">
+    <row r="85" spans="12:15" ht="24.95" customHeight="1">
       <c r="L85" s="17" t="s">
         <v>189</v>
       </c>
@@ -7111,7 +6986,7 @@
       <c r="N85" s="17"/>
       <c r="O85" s="19"/>
     </row>
-    <row r="86" spans="12:15" ht="24.95" hidden="1" customHeight="1">
+    <row r="86" spans="12:15" ht="24.95" customHeight="1">
       <c r="L86" s="17" t="s">
         <v>190</v>
       </c>
@@ -7119,7 +6994,7 @@
       <c r="N86" s="17"/>
       <c r="O86" s="19"/>
     </row>
-    <row r="87" spans="12:15" ht="24.95" hidden="1" customHeight="1">
+    <row r="87" spans="12:15" ht="24.95" customHeight="1">
       <c r="L87" s="17" t="s">
         <v>191</v>
       </c>
@@ -7127,7 +7002,7 @@
       <c r="N87" s="17"/>
       <c r="O87" s="19"/>
     </row>
-    <row r="88" spans="12:15" ht="24.95" hidden="1" customHeight="1">
+    <row r="88" spans="12:15" ht="24.95" customHeight="1">
       <c r="L88" s="17" t="s">
         <v>192</v>
       </c>
@@ -7136,13 +7011,7 @@
       <c r="O88" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="L2:O88" xr:uid="{8B4F5866-1724-4EB7-BC7B-9E366F71039B}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Sporting"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="L2:O88"/>
   <sortState ref="M3:O79">
     <sortCondition descending="1" ref="N3:N79"/>
   </sortState>
@@ -7151,33 +7020,33 @@
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="L3:O88">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="26" priority="1">
       <formula>$O3="Sporting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="33" priority="2">
       <formula>$O3="Real Madrid"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="32" priority="3">
       <formula>$O3="Manchester City"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="31" priority="4">
       <formula>$O3="Bayern Munique"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="30" priority="5">
       <formula>$O3="Bayer Leverkusen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="29" priority="6">
       <formula>$O3="Internazionale"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="28" priority="7">
       <formula>$O3="Arsenal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="27" priority="8">
       <formula>$O3="Barcelona"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="O3:O88" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="O3:O88">
       <formula1>"Internazionale,Arsenal,Barcelona,Manchester City,Juventus,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7187,7 +7056,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S80"/>
   <sheetViews>
     <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -9339,7 +9208,7 @@
       <c r="M68" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="R68" s="60"/>
+      <c r="R68" s="43"/>
     </row>
     <row r="71" spans="1:19" ht="14.25" customHeight="1"/>
     <row r="72" spans="1:19" ht="30" customHeight="1">
@@ -9526,7 +9395,7 @@
       <c r="P75" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="Q75" s="61" t="s">
+      <c r="Q75" s="44" t="s">
         <v>103</v>
       </c>
       <c r="R75" s="13" t="s">
@@ -9558,7 +9427,7 @@
       <c r="H76" s="15">
         <v>0</v>
       </c>
-      <c r="J76" s="60"/>
+      <c r="J76" s="43"/>
       <c r="K76" s="10" t="s">
         <v>326</v>
       </c>
@@ -9708,7 +9577,7 @@
       <c r="M80" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="R80" s="60"/>
+      <c r="R80" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -9717,11 +9586,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:G17"/>
+    <sheetView showGridLines="0" zoomScale="69" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9747,10 +9616,10 @@
       <c r="E1" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="55"/>
+      <c r="G1" s="49"/>
       <c r="H1" s="34" t="s">
         <v>311</v>
       </c>
@@ -9771,10 +9640,10 @@
       <c r="E2" s="35">
         <v>28</v>
       </c>
-      <c r="F2" s="56">
+      <c r="F2" s="50">
         <v>28</v>
       </c>
-      <c r="G2" s="56"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1">
@@ -9803,10 +9672,10 @@
       <c r="E4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="57"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="42" t="s">
         <v>81</v>
       </c>
@@ -9827,11 +9696,11 @@
       <c r="E5" s="23">
         <v>27</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="52">
         <v>17</v>
       </c>
-      <c r="G5" s="58"/>
-      <c r="H5" s="62"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="1:8" ht="24" customHeight="1">
       <c r="A6" s="32"/>
@@ -9859,10 +9728,10 @@
       <c r="E7" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="59"/>
+      <c r="G7" s="53"/>
       <c r="H7" s="38" t="s">
         <v>314</v>
       </c>
@@ -9883,10 +9752,10 @@
       <c r="E8" s="39">
         <v>61</v>
       </c>
-      <c r="F8" s="54">
+      <c r="F8" s="48">
         <v>33</v>
       </c>
-      <c r="G8" s="54"/>
+      <c r="G8" s="48"/>
       <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" ht="24" customHeight="1">
@@ -9915,10 +9784,10 @@
       <c r="E10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="50" t="s">
+      <c r="F10" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="50"/>
+      <c r="G10" s="54"/>
       <c r="H10" s="5" t="s">
         <v>36</v>
       </c>
@@ -9939,10 +9808,10 @@
       <c r="E11" s="24">
         <v>19</v>
       </c>
-      <c r="F11" s="51">
+      <c r="F11" s="55">
         <v>36</v>
       </c>
-      <c r="G11" s="51"/>
+      <c r="G11" s="55"/>
       <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" ht="24" customHeight="1">
@@ -9995,10 +9864,10 @@
       <c r="E14" s="36">
         <v>29</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="56">
         <v>35</v>
       </c>
-      <c r="G14" s="52"/>
+      <c r="G14" s="56"/>
       <c r="H14" s="37"/>
     </row>
     <row r="15" spans="1:8" ht="24" customHeight="1">
@@ -10027,10 +9896,10 @@
       <c r="E16" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="53" t="s">
+      <c r="F16" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="53"/>
+      <c r="G16" s="57"/>
       <c r="H16" s="6" t="s">
         <v>103</v>
       </c>
@@ -10051,10 +9920,10 @@
       <c r="E17" s="25">
         <v>15</v>
       </c>
-      <c r="F17" s="45">
+      <c r="F17" s="58">
         <v>21</v>
       </c>
-      <c r="G17" s="45"/>
+      <c r="G17" s="58"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:11" ht="24" customHeight="1">
@@ -10083,10 +9952,10 @@
       <c r="E19" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="46"/>
+      <c r="G19" s="59"/>
       <c r="H19" s="26" t="s">
         <v>104</v>
       </c>
@@ -10107,10 +9976,10 @@
       <c r="E20" s="27">
         <v>7</v>
       </c>
-      <c r="F20" s="47">
+      <c r="F20" s="60">
         <v>3</v>
       </c>
-      <c r="G20" s="47"/>
+      <c r="G20" s="60"/>
       <c r="H20" s="32"/>
     </row>
     <row r="21" spans="1:11" ht="24" customHeight="1">
@@ -10139,10 +10008,10 @@
       <c r="E22" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="48" t="s">
+      <c r="F22" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="48"/>
+      <c r="G22" s="61"/>
       <c r="H22" s="28" t="s">
         <v>35</v>
       </c>
@@ -10163,14 +10032,14 @@
       <c r="E23" s="29">
         <v>29</v>
       </c>
-      <c r="F23" s="49">
+      <c r="F23" s="62">
         <v>34</v>
       </c>
-      <c r="G23" s="49"/>
+      <c r="G23" s="62"/>
       <c r="H23" s="32"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="K24" s="60"/>
+      <c r="K24" s="43"/>
     </row>
     <row r="27" spans="1:11">
       <c r="G27" s="2"/>
@@ -10186,22 +10055,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização comppleta, conforme resultado do sétimo torneio
</commit_message>
<xml_diff>
--- a/Dados/Dados_Torneio.xlsx
+++ b/Dados/Dados_Torneio.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmarinho\Desktop\Site\tuf.github.io\Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Site\tuf.github.io\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3F10F5-6ED8-4205-BD68-64FE9EC0E9F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Melhor_jogador" sheetId="5" r:id="rId1"/>
@@ -22,8 +23,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Artilharia!$A$2:$D$208</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Assistências!$L$2:$O$88</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mjRhCzJXjykQ+ehJRy/U6qyvWzECg=="/>
     </ext>
@@ -32,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="393">
   <si>
     <t>Melhores Jogadores</t>
   </si>
@@ -1156,9 +1163,6 @@
     <t>Kostic</t>
   </si>
   <si>
-    <t>Felix</t>
-  </si>
-  <si>
     <t>Sissoko</t>
   </si>
   <si>
@@ -1184,12 +1188,42 @@
   </si>
   <si>
     <t>Moura</t>
+  </si>
+  <si>
+    <t>Son</t>
+  </si>
+  <si>
+    <t>Bem Yedder</t>
+  </si>
+  <si>
+    <t>Joe Gomez</t>
+  </si>
+  <si>
+    <t>Ben Yedder</t>
+  </si>
+  <si>
+    <t>Bellerin</t>
+  </si>
+  <si>
+    <t>Arnold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 x 4 </t>
+  </si>
+  <si>
+    <t>2 x 3</t>
+  </si>
+  <si>
+    <t>2 x 4</t>
+  </si>
+  <si>
+    <t>Neymar Jr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="28">
     <font>
       <sz val="11"/>
@@ -1605,6 +1639,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1633,6 +1670,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1654,17 +1694,127 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7030A0"/>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFCDBC97"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEF0107"/>
+          <bgColor rgb="FFEF0107"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="3"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD2122E"/>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFED1C24"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF171616"/>
+          <bgColor rgb="FF171616"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF034694"/>
+          <bgColor rgb="FF6CA6DA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF186E45"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1771,7 +1921,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF044C15"/>
-          <bgColor rgb="FF003300"/>
+          <bgColor rgb="FF186E45"/>
         </patternFill>
       </fill>
       <border>
@@ -1887,141 +2037,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF005400"/>
-          <bgColor rgb="FF003300"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7030A0"/>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFCDBC97"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEF0107"/>
-          <bgColor rgb="FFEF0107"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD2122E"/>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFED1C24"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF171616"/>
-          <bgColor rgb="FF171616"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF034694"/>
-          <bgColor rgb="FF6CA6DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF003300"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF044C15"/>
           <bgColor rgb="FF186E45"/>
         </patternFill>
       </fill>
@@ -2031,335 +2046,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF005400"/>
-          <bgColor rgb="FF186E45"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF186E45"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7030A0"/>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFCDBC97"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEF0107"/>
-          <bgColor rgb="FFEF0107"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD2122E"/>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFED1C24"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF171616"/>
-          <bgColor rgb="FF171616"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF034694"/>
-          <bgColor rgb="FF6CA6DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7030A0"/>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFCDBC97"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEF0107"/>
-          <bgColor rgb="FFEF0107"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD2122E"/>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFED1C24"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF171616"/>
-          <bgColor rgb="FF171616"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF034694"/>
-          <bgColor rgb="FF6CA6DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7030A0"/>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFCDBC97"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEF0107"/>
-          <bgColor rgb="FFEF0107"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD2122E"/>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFED1C24"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF171616"/>
-          <bgColor rgb="FF171616"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF034694"/>
-          <bgColor rgb="FF6CA6DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2585,11 +2271,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2600,11 +2286,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="A2" s="16" t="s">
@@ -2684,9 +2370,15 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="A9" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="A10" s="17"/>
@@ -2778,33 +2470,33 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:C26">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>$B3="Sporting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>$B3="Real Madrid"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>$B3="Manchester City"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>$B3="Bayern Munique"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>$B3="Bayer Leverkusen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="6">
+    <cfRule type="expression" dxfId="18" priority="6">
       <formula>$B3="Internazionale"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="7">
+    <cfRule type="expression" dxfId="17" priority="7">
       <formula>$B3="Arsenal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="8">
+    <cfRule type="expression" dxfId="16" priority="8">
       <formula>$B3="Barcelona"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="B3:B26">
+    <dataValidation type="list" allowBlank="1" sqref="B3:B26" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Internazionale,Arsenal,Barcelona,Manchester City,Sporting,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2813,11 +2505,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2840,12 +2532,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1">
@@ -2868,13 +2560,13 @@
         <v>9</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>56</v>
+        <v>372</v>
       </c>
       <c r="C3" s="17">
-        <v>10</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>35</v>
+        <v>12</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>312</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -2882,14 +2574,14 @@
       <c r="A4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>178</v>
+      <c r="B4" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="C4" s="17">
-        <v>10</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>360</v>
+        <v>11</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -2898,13 +2590,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C5" s="17">
-        <v>9</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>312</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -2912,14 +2604,14 @@
       <c r="A6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>315</v>
+      <c r="B6" s="17" t="s">
+        <v>178</v>
       </c>
       <c r="C6" s="17">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>311</v>
+        <v>360</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -2927,14 +2619,14 @@
       <c r="A7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="18">
-        <v>7</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>312</v>
+      <c r="B7" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="17">
+        <v>9</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -2943,10 +2635,10 @@
         <v>14</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="C8" s="17">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>312</v>
@@ -2958,13 +2650,13 @@
         <v>15</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C9" s="17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>34</v>
+        <v>312</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -2973,13 +2665,13 @@
         <v>16</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>372</v>
+        <v>315</v>
       </c>
       <c r="C10" s="17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -2988,13 +2680,13 @@
         <v>17</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C11" s="17">
-        <v>6</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>34</v>
+        <v>7</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>312</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -3003,13 +2695,13 @@
         <v>18</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="C12" s="17">
-        <v>6</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>34</v>
+        <v>7</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>311</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -3018,13 +2710,13 @@
         <v>19</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>61</v>
+        <v>381</v>
       </c>
       <c r="C13" s="17">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -3033,13 +2725,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C14" s="17">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -3047,14 +2739,14 @@
       <c r="A15" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>367</v>
-      </c>
-      <c r="C15" s="17">
-        <v>5</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>118</v>
+      <c r="B15" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="18">
+        <v>7</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>312</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -3062,13 +2754,13 @@
       <c r="A16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>66</v>
+      <c r="B16" s="17" t="s">
+        <v>383</v>
       </c>
       <c r="C16" s="17">
-        <v>4</v>
-      </c>
-      <c r="D16" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>311</v>
       </c>
       <c r="F16" s="1"/>
@@ -3077,14 +2769,14 @@
       <c r="A17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="40" t="s">
-        <v>351</v>
-      </c>
-      <c r="C17" s="41">
-        <v>4</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>84</v>
+      <c r="B17" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="C17" s="17">
+        <v>6</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>312</v>
       </c>
       <c r="F17" s="1"/>
       <c r="I17" s="2"/>
@@ -3094,13 +2786,13 @@
         <v>24</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>45</v>
+        <v>367</v>
       </c>
       <c r="C18" s="17">
-        <v>4</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>36</v>
+        <v>5</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="F18" s="1"/>
     </row>
@@ -3109,13 +2801,13 @@
         <v>25</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="C19" s="17">
-        <v>4</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>311</v>
+        <v>5</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>35</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -3123,14 +2815,14 @@
       <c r="A20" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>354</v>
+      <c r="B20" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="C20" s="17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>360</v>
+        <v>36</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -3138,14 +2830,14 @@
       <c r="A21" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>380</v>
+      <c r="B21" s="17" t="s">
+        <v>354</v>
       </c>
       <c r="C21" s="17">
-        <v>4</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>312</v>
+        <v>5</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>360</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -3154,10 +2846,10 @@
         <v>28</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="C22" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>360</v>
@@ -3169,10 +2861,10 @@
         <v>29</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C23" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>36</v>
@@ -3184,13 +2876,13 @@
         <v>30</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>319</v>
+        <v>177</v>
       </c>
       <c r="C24" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>118</v>
+        <v>35</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -3198,14 +2890,14 @@
       <c r="A25" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="17">
-        <v>3</v>
+      <c r="B25" s="40" t="s">
+        <v>351</v>
+      </c>
+      <c r="C25" s="41">
+        <v>4</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -3214,13 +2906,13 @@
         <v>32</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>52</v>
+        <v>335</v>
       </c>
       <c r="C26" s="17">
-        <v>3</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>312</v>
+        <v>4</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>311</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -3229,13 +2921,13 @@
         <v>120</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>177</v>
+        <v>49</v>
       </c>
       <c r="C27" s="17">
         <v>3</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F27" s="1"/>
     </row>
@@ -3244,13 +2936,13 @@
         <v>121</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>116</v>
+        <v>319</v>
       </c>
       <c r="C28" s="17">
         <v>3</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>360</v>
+        <v>118</v>
       </c>
       <c r="F28" s="1"/>
     </row>
@@ -3259,13 +2951,13 @@
         <v>122</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>382</v>
+        <v>52</v>
       </c>
       <c r="C29" s="17">
         <v>3</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F29" s="1"/>
     </row>
@@ -3274,13 +2966,13 @@
         <v>123</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>355</v>
+        <v>62</v>
       </c>
       <c r="C30" s="17">
         <v>3</v>
       </c>
-      <c r="D30" s="19" t="s">
-        <v>35</v>
+      <c r="D30" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="F30" s="1"/>
     </row>
@@ -3288,14 +2980,14 @@
       <c r="A31" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B31" s="19" t="s">
-        <v>44</v>
+      <c r="B31" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="C31" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -3304,13 +2996,13 @@
         <v>125</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="C32" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>36</v>
+        <v>360</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -3318,28 +3010,28 @@
       <c r="A33" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>51</v>
+      <c r="B33" s="17" t="s">
+        <v>115</v>
       </c>
       <c r="C33" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>312</v>
+        <v>360</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="24.75" customHeight="1">
       <c r="A34" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>58</v>
+      <c r="B34" s="17" t="s">
+        <v>378</v>
       </c>
       <c r="C34" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>35</v>
+        <v>312</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="24.75" customHeight="1">
@@ -3347,13 +3039,13 @@
         <v>128</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>62</v>
+        <v>377</v>
       </c>
       <c r="C35" s="17">
         <v>2</v>
       </c>
-      <c r="D35" s="17" t="s">
-        <v>34</v>
+      <c r="D35" s="19" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.75" customHeight="1">
@@ -3375,55 +3067,55 @@
         <v>130</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>171</v>
+        <v>51</v>
       </c>
       <c r="C37" s="17">
         <v>2</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="24.75" customHeight="1">
       <c r="A38" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="B38" s="17" t="s">
-        <v>115</v>
+      <c r="B38" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="C38" s="17">
         <v>2</v>
       </c>
-      <c r="D38" s="19" t="s">
-        <v>360</v>
+      <c r="D38" s="17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="24.75" customHeight="1">
       <c r="A39" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B39" s="17" t="s">
-        <v>344</v>
+      <c r="B39" s="19" t="s">
+        <v>316</v>
       </c>
       <c r="C39" s="17">
         <v>2</v>
       </c>
-      <c r="D39" s="17" t="s">
-        <v>360</v>
+      <c r="D39" s="19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="24.75" customHeight="1">
       <c r="A40" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>378</v>
+      <c r="B40" s="17" t="s">
+        <v>344</v>
       </c>
       <c r="C40" s="17">
         <v>2</v>
       </c>
-      <c r="D40" s="19" t="s">
-        <v>118</v>
+      <c r="D40" s="17" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="24.75" customHeight="1">
@@ -3431,27 +3123,27 @@
         <v>134</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>336</v>
+        <v>58</v>
       </c>
       <c r="C41" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>311</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="24.75" customHeight="1">
       <c r="A42" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>337</v>
+      <c r="B42" s="17" t="s">
+        <v>169</v>
       </c>
       <c r="C42" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="24.75" customHeight="1">
@@ -3459,13 +3151,13 @@
         <v>136</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>334</v>
+        <v>59</v>
       </c>
       <c r="C43" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>312</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="24.75" customHeight="1">
@@ -3473,41 +3165,41 @@
         <v>137</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>333</v>
+        <v>171</v>
       </c>
       <c r="C44" s="17">
-        <v>1</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>360</v>
+        <v>2</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="24.75" customHeight="1">
       <c r="A45" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>47</v>
+      <c r="B45" s="17" t="s">
+        <v>376</v>
       </c>
       <c r="C45" s="17">
         <v>1</v>
       </c>
-      <c r="D45" s="19" t="s">
-        <v>312</v>
+      <c r="D45" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="24.75" customHeight="1">
       <c r="A46" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="B46" s="19" t="s">
-        <v>50</v>
+      <c r="B46" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="C46" s="17">
         <v>1</v>
       </c>
-      <c r="D46" s="19" t="s">
-        <v>312</v>
+      <c r="D46" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="24.75" customHeight="1">
@@ -3515,27 +3207,27 @@
         <v>140</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C47" s="17">
         <v>1</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="24.75" customHeight="1">
       <c r="A48" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>60</v>
+      <c r="B48" s="17" t="s">
+        <v>384</v>
       </c>
       <c r="C48" s="17">
         <v>1</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>35</v>
+        <v>360</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="24.75" customHeight="1">
@@ -3543,13 +3235,13 @@
         <v>142</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C49" s="17">
         <v>1</v>
       </c>
-      <c r="D49" s="17" t="s">
-        <v>35</v>
+      <c r="D49" s="19" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="24.75" customHeight="1">
@@ -3557,12 +3249,12 @@
         <v>143</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>57</v>
+        <v>336</v>
       </c>
       <c r="C50" s="17">
         <v>1</v>
       </c>
-      <c r="D50" s="19" t="s">
+      <c r="D50" s="17" t="s">
         <v>311</v>
       </c>
     </row>
@@ -3570,36 +3262,36 @@
       <c r="A51" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="B51" s="17" t="s">
-        <v>303</v>
+      <c r="B51" s="19" t="s">
+        <v>333</v>
       </c>
       <c r="C51" s="17">
         <v>1</v>
       </c>
-      <c r="D51" s="19" t="s">
-        <v>84</v>
+      <c r="D51" s="17" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="24.75" customHeight="1">
       <c r="A52" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="B52" s="17" t="s">
-        <v>304</v>
+      <c r="B52" s="19" t="s">
+        <v>53</v>
       </c>
       <c r="C52" s="17">
         <v>1</v>
       </c>
-      <c r="D52" s="17" t="s">
-        <v>84</v>
+      <c r="D52" s="19" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="24.75" customHeight="1">
       <c r="A53" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="B53" s="17" t="s">
-        <v>305</v>
+      <c r="B53" s="19" t="s">
+        <v>317</v>
       </c>
       <c r="C53" s="17">
         <v>1</v>
@@ -3613,13 +3305,13 @@
         <v>147</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>64</v>
+        <v>309</v>
       </c>
       <c r="C54" s="17">
         <v>1</v>
       </c>
-      <c r="D54" s="19" t="s">
-        <v>311</v>
+      <c r="D54" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="24.75" customHeight="1">
@@ -3627,13 +3319,13 @@
         <v>148</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C55" s="17">
         <v>1</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="24.75" customHeight="1">
@@ -3641,13 +3333,13 @@
         <v>149</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>307</v>
+        <v>353</v>
       </c>
       <c r="C56" s="17">
         <v>1</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>84</v>
+        <v>360</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="24.75" customHeight="1">
@@ -3655,12 +3347,12 @@
         <v>150</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C57" s="17">
         <v>1</v>
       </c>
-      <c r="D57" s="17" t="s">
+      <c r="D57" s="19" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3668,14 +3360,14 @@
       <c r="A58" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B58" s="17" t="s">
-        <v>169</v>
+      <c r="B58" s="19" t="s">
+        <v>337</v>
       </c>
       <c r="C58" s="17">
         <v>1</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K58" s="3"/>
     </row>
@@ -3683,14 +3375,14 @@
       <c r="A59" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="B59" s="17" t="s">
-        <v>309</v>
+      <c r="B59" s="19" t="s">
+        <v>341</v>
       </c>
       <c r="C59" s="17">
         <v>1</v>
       </c>
-      <c r="D59" s="17" t="s">
-        <v>84</v>
+      <c r="D59" s="19" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="24.75" customHeight="1">
@@ -3698,41 +3390,41 @@
         <v>153</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="C60" s="17">
         <v>1</v>
       </c>
       <c r="D60" s="19" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="24.75" customHeight="1">
       <c r="A61" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="B61" s="19" t="s">
-        <v>317</v>
+      <c r="B61" s="17" t="s">
+        <v>385</v>
       </c>
       <c r="C61" s="17">
         <v>1</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>118</v>
+        <v>312</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="24.75" customHeight="1">
       <c r="A62" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="B62" s="19" t="s">
-        <v>318</v>
+      <c r="B62" s="17" t="s">
+        <v>306</v>
       </c>
       <c r="C62" s="17">
         <v>1</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="24.75" customHeight="1">
@@ -3740,7 +3432,7 @@
         <v>156</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="C63" s="17">
         <v>1</v>
@@ -3754,27 +3446,27 @@
         <v>157</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>332</v>
+        <v>60</v>
       </c>
       <c r="C64" s="17">
         <v>1</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="24.75" customHeight="1">
       <c r="A65" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="B65" s="17" t="s">
-        <v>349</v>
+      <c r="B65" s="19" t="s">
+        <v>382</v>
       </c>
       <c r="C65" s="17">
         <v>1</v>
       </c>
-      <c r="D65" s="17" t="s">
-        <v>84</v>
+      <c r="D65" s="19" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="24.75" customHeight="1">
@@ -3782,55 +3474,55 @@
         <v>159</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>352</v>
+        <v>305</v>
       </c>
       <c r="C66" s="17">
         <v>1</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="24.75" customHeight="1">
       <c r="A67" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="B67" s="17" t="s">
-        <v>353</v>
+      <c r="B67" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="C67" s="17">
         <v>1</v>
       </c>
-      <c r="D67" s="17" t="s">
-        <v>360</v>
+      <c r="D67" s="19" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="24.75" customHeight="1">
       <c r="A68" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B68" s="17" t="s">
-        <v>321</v>
+      <c r="B68" s="19" t="s">
+        <v>332</v>
       </c>
       <c r="C68" s="17">
         <v>1</v>
       </c>
-      <c r="D68" s="19" t="s">
-        <v>311</v>
+      <c r="D68" s="17" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="24.75" customHeight="1">
       <c r="A69" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="B69" s="19" t="s">
-        <v>341</v>
+      <c r="B69" s="17" t="s">
+        <v>352</v>
       </c>
       <c r="C69" s="17">
         <v>1</v>
       </c>
-      <c r="D69" s="19" t="s">
-        <v>311</v>
+      <c r="D69" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="24.75" customHeight="1">
@@ -3838,13 +3530,13 @@
         <v>163</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="C70" s="17">
         <v>1</v>
       </c>
-      <c r="D70" s="19" t="s">
-        <v>118</v>
+      <c r="D70" s="17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="24.75" customHeight="1">
@@ -3852,82 +3544,112 @@
         <v>164</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>383</v>
+        <v>55</v>
       </c>
       <c r="C71" s="17">
         <v>1</v>
       </c>
-      <c r="D71" s="19" t="s">
-        <v>118</v>
+      <c r="D71" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="24.75" customHeight="1">
       <c r="A72" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="B72" s="19" t="s">
-        <v>381</v>
+      <c r="B72" s="17" t="s">
+        <v>307</v>
       </c>
       <c r="C72" s="17">
         <v>1</v>
       </c>
-      <c r="D72" s="19" t="s">
-        <v>312</v>
+      <c r="D72" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="24.75" customHeight="1">
       <c r="A73" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="B73" s="19" t="s">
-        <v>324</v>
+      <c r="B73" s="17" t="s">
+        <v>308</v>
       </c>
       <c r="C73" s="17">
         <v>1</v>
       </c>
-      <c r="D73" s="19" t="s">
-        <v>360</v>
+      <c r="D73" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="24.75" customHeight="1">
       <c r="A74" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
+      <c r="B74" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="C74" s="17">
+        <v>1</v>
+      </c>
+      <c r="D74" s="19" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="75" spans="1:4" ht="24.75" customHeight="1">
       <c r="A75" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
+      <c r="B75" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C75" s="17">
+        <v>1</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="76" spans="1:4" ht="24.75" customHeight="1">
       <c r="A76" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
+      <c r="B76" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="C76" s="17">
+        <v>1</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="77" spans="1:4" ht="24.75" customHeight="1">
       <c r="A77" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
+      <c r="B77" s="19" t="s">
+        <v>380</v>
+      </c>
+      <c r="C77" s="17">
+        <v>1</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="78" spans="1:4" ht="24.75" customHeight="1">
       <c r="A78" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
+      <c r="B78" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="C78" s="17">
+        <v>1</v>
+      </c>
+      <c r="D78" s="17" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="79" spans="1:4" ht="24.75" customHeight="1">
       <c r="A79" s="17" t="s">
@@ -5773,45 +5495,44 @@
     <row r="1008" ht="15.75" customHeight="1"/>
     <row r="1009" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A2:D208"/>
-  <sortState ref="B3:D73">
-    <sortCondition descending="1" ref="C3:C73"/>
+  <sortState ref="B3:D78">
+    <sortCondition descending="1" ref="C3:C78"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="A3:D208">
-    <cfRule type="expression" dxfId="24" priority="49">
+    <cfRule type="expression" dxfId="15" priority="49">
       <formula>$D3="Sporting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="50">
+    <cfRule type="expression" dxfId="14" priority="50">
       <formula>$D3="Real Madrid"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="51">
+    <cfRule type="expression" dxfId="13" priority="51">
       <formula>$D3="Manchester City"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="52">
+    <cfRule type="expression" dxfId="12" priority="52">
       <formula>$D3="Bayern Munique"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="53">
+    <cfRule type="expression" dxfId="11" priority="53">
       <formula>$D3="Bayer Leverkusen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="54">
+    <cfRule type="expression" dxfId="10" priority="54">
       <formula>$D3="Internazionale"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="55">
+    <cfRule type="expression" dxfId="9" priority="55">
       <formula>$D3="Arsenal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="56">
+    <cfRule type="expression" dxfId="8" priority="56">
       <formula>$D3="Barcelona"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="D3:D42 D58 D60 D62:D111">
+    <dataValidation type="list" allowBlank="1" sqref="D3:D42 D58 D60 D62:D111" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Internazionale,Arsenal,Barcelona,Manchester City,Sporting,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D59 D61 D43:D57 D112:D208">
+    <dataValidation type="list" allowBlank="1" sqref="D59 D61 D43:D57 D112:D208" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Ajax,Arsenal,Barcelona,Liverpool,Milan,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5821,11 +5542,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="L1:T88"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView topLeftCell="K1" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5837,12 +5558,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="12:15" ht="30" customHeight="1">
-      <c r="L1" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
+      <c r="L1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
     </row>
     <row r="2" spans="12:15" ht="30" customHeight="1">
       <c r="L2" s="16" t="s">
@@ -5877,13 +5598,13 @@
         <v>10</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>56</v>
+        <v>316</v>
       </c>
       <c r="N4" s="17">
-        <v>6</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>35</v>
+        <v>7</v>
+      </c>
+      <c r="O4" s="19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="12:15" ht="24" customHeight="1">
@@ -5891,41 +5612,41 @@
         <v>11</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="N5" s="17">
         <v>6</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>312</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="12:15" ht="24" customHeight="1">
       <c r="L6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="N6" s="18">
+      <c r="M6" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="N6" s="17">
         <v>6</v>
       </c>
-      <c r="O6" s="19" t="s">
-        <v>34</v>
+      <c r="O6" s="17" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="12:15" ht="24" customHeight="1">
       <c r="L7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="N7" s="17">
-        <v>5</v>
-      </c>
-      <c r="O7" s="17" t="s">
-        <v>35</v>
+      <c r="M7" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="18">
+        <v>6</v>
+      </c>
+      <c r="O7" s="19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="12:15" ht="24" customHeight="1">
@@ -5936,7 +5657,7 @@
         <v>116</v>
       </c>
       <c r="N8" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O8" s="17" t="s">
         <v>360</v>
@@ -5950,7 +5671,7 @@
         <v>173</v>
       </c>
       <c r="N9" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O9" s="17" t="s">
         <v>312</v>
@@ -5964,7 +5685,7 @@
         <v>115</v>
       </c>
       <c r="N10" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O10" s="17" t="s">
         <v>360</v>
@@ -5978,7 +5699,7 @@
         <v>64</v>
       </c>
       <c r="N11" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O11" s="17" t="s">
         <v>311</v>
@@ -5988,27 +5709,27 @@
       <c r="L12" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="M12" s="18" t="s">
-        <v>338</v>
-      </c>
-      <c r="N12" s="18">
-        <v>4</v>
+      <c r="M12" s="19" t="s">
+        <v>372</v>
+      </c>
+      <c r="N12" s="17">
+        <v>6</v>
       </c>
       <c r="O12" s="19" t="s">
-        <v>36</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="12:15" ht="24" customHeight="1">
       <c r="L13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="M13" s="17" t="s">
-        <v>171</v>
+      <c r="M13" s="19" t="s">
+        <v>358</v>
       </c>
       <c r="N13" s="17">
-        <v>4</v>
-      </c>
-      <c r="O13" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13" s="19" t="s">
         <v>311</v>
       </c>
     </row>
@@ -6017,13 +5738,13 @@
         <v>20</v>
       </c>
       <c r="M14" s="19" t="s">
-        <v>41</v>
+        <v>378</v>
       </c>
       <c r="N14" s="17">
-        <v>4</v>
-      </c>
-      <c r="O14" s="17" t="s">
-        <v>34</v>
+        <v>6</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="12:15" ht="24" customHeight="1">
@@ -6031,13 +5752,13 @@
         <v>21</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="N15" s="17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O15" s="17" t="s">
-        <v>312</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="12:15" ht="24" customHeight="1">
@@ -6045,13 +5766,13 @@
         <v>22</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>38</v>
+        <v>171</v>
       </c>
       <c r="N16" s="17">
-        <v>4</v>
-      </c>
-      <c r="O16" s="19" t="s">
-        <v>312</v>
+        <v>5</v>
+      </c>
+      <c r="O16" s="17" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="12:20" ht="24" customHeight="1">
@@ -6062,7 +5783,7 @@
         <v>61</v>
       </c>
       <c r="N17" s="17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O17" s="19" t="s">
         <v>312</v>
@@ -6072,14 +5793,14 @@
       <c r="L18" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="M18" s="19" t="s">
-        <v>372</v>
-      </c>
-      <c r="N18" s="17">
+      <c r="M18" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="N18" s="18">
         <v>4</v>
       </c>
       <c r="O18" s="19" t="s">
-        <v>312</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="12:20" ht="24" customHeight="1">
@@ -6087,13 +5808,13 @@
         <v>25</v>
       </c>
       <c r="M19" s="19" t="s">
-        <v>354</v>
+        <v>41</v>
       </c>
       <c r="N19" s="17">
         <v>4</v>
       </c>
-      <c r="O19" s="19" t="s">
-        <v>360</v>
+      <c r="O19" s="17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="12:20" ht="24" customHeight="1">
@@ -6101,13 +5822,13 @@
         <v>26</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
       <c r="N20" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O20" s="17" t="s">
-        <v>36</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="12:20" ht="24" customHeight="1">
@@ -6115,13 +5836,13 @@
         <v>27</v>
       </c>
       <c r="M21" s="17" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="N21" s="17">
-        <v>3</v>
-      </c>
-      <c r="O21" s="17" t="s">
-        <v>36</v>
+        <v>4</v>
+      </c>
+      <c r="O21" s="19" t="s">
+        <v>312</v>
       </c>
       <c r="T21" s="2"/>
     </row>
@@ -6130,13 +5851,13 @@
         <v>28</v>
       </c>
       <c r="M22" s="19" t="s">
-        <v>321</v>
+        <v>354</v>
       </c>
       <c r="N22" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O22" s="19" t="s">
-        <v>311</v>
+        <v>360</v>
       </c>
       <c r="T22" s="2"/>
     </row>
@@ -6145,13 +5866,13 @@
         <v>29</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="N23" s="17">
         <v>3</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>118</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="12:20" ht="24" customHeight="1">
@@ -6159,13 +5880,13 @@
         <v>30</v>
       </c>
       <c r="M24" s="17" t="s">
-        <v>169</v>
+        <v>59</v>
       </c>
       <c r="N24" s="17">
         <v>3</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="12:20" ht="24" customHeight="1">
@@ -6173,7 +5894,7 @@
         <v>31</v>
       </c>
       <c r="M25" s="19" t="s">
-        <v>358</v>
+        <v>321</v>
       </c>
       <c r="N25" s="17">
         <v>3</v>
@@ -6187,13 +5908,13 @@
         <v>32</v>
       </c>
       <c r="M26" s="17" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
       <c r="N26" s="17">
-        <v>2</v>
-      </c>
-      <c r="O26" s="19" t="s">
-        <v>34</v>
+        <v>3</v>
+      </c>
+      <c r="O26" s="17" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="12:20" ht="24" customHeight="1">
@@ -6201,13 +5922,13 @@
         <v>120</v>
       </c>
       <c r="M27" s="17" t="s">
-        <v>47</v>
+        <v>169</v>
       </c>
       <c r="N27" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O27" s="17" t="s">
-        <v>312</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="12:20" ht="24" customHeight="1">
@@ -6215,83 +5936,83 @@
         <v>121</v>
       </c>
       <c r="M28" s="17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="N28" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O28" s="17" t="s">
-        <v>312</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="12:20" ht="24" customHeight="1">
       <c r="L29" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="M29" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="N29" s="17">
-        <v>2</v>
-      </c>
-      <c r="O29" s="17" t="s">
-        <v>34</v>
+      <c r="M29" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="N29" s="18">
+        <v>3</v>
+      </c>
+      <c r="O29" s="19" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="30" spans="12:20" ht="24" customHeight="1">
       <c r="L30" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="M30" s="17" t="s">
-        <v>310</v>
+      <c r="M30" s="19" t="s">
+        <v>177</v>
       </c>
       <c r="N30" s="17">
-        <v>2</v>
-      </c>
-      <c r="O30" s="17" t="s">
-        <v>36</v>
+        <v>3</v>
+      </c>
+      <c r="O30" s="19" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="12:20" ht="24" customHeight="1">
       <c r="L31" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="M31" s="19" t="s">
-        <v>320</v>
+      <c r="M31" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="N31" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O31" s="17" t="s">
-        <v>34</v>
+        <v>311</v>
       </c>
     </row>
     <row r="32" spans="12:20" ht="24" customHeight="1">
       <c r="L32" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="M32" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="N32" s="18">
-        <v>2</v>
-      </c>
-      <c r="O32" s="19" t="s">
-        <v>360</v>
+      <c r="M32" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="N32" s="17">
+        <v>3</v>
+      </c>
+      <c r="O32" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="12:15" ht="24" customHeight="1">
       <c r="L33" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="M33" s="18" t="s">
-        <v>315</v>
-      </c>
-      <c r="N33" s="18">
-        <v>2</v>
-      </c>
-      <c r="O33" s="19" t="s">
-        <v>311</v>
+      <c r="M33" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="N33" s="17">
+        <v>3</v>
+      </c>
+      <c r="O33" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="12:15" ht="24" customHeight="1">
@@ -6299,12 +6020,12 @@
         <v>127</v>
       </c>
       <c r="M34" s="17" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="N34" s="17">
         <v>2</v>
       </c>
-      <c r="O34" s="17" t="s">
+      <c r="O34" s="19" t="s">
         <v>34</v>
       </c>
     </row>
@@ -6313,69 +6034,69 @@
         <v>128</v>
       </c>
       <c r="M35" s="17" t="s">
-        <v>329</v>
+        <v>47</v>
       </c>
       <c r="N35" s="17">
         <v>2</v>
       </c>
       <c r="O35" s="17" t="s">
-        <v>35</v>
+        <v>312</v>
       </c>
     </row>
     <row r="36" spans="12:15" ht="24" customHeight="1">
       <c r="L36" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="M36" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="N36" s="18">
+      <c r="M36" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="N36" s="17">
         <v>2</v>
       </c>
-      <c r="O36" s="19" t="s">
-        <v>311</v>
+      <c r="O36" s="17" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="37" spans="12:15" ht="24.75" customHeight="1">
       <c r="L37" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="M37" s="19" t="s">
-        <v>373</v>
+      <c r="M37" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="N37" s="17">
         <v>2</v>
       </c>
-      <c r="O37" s="19" t="s">
-        <v>118</v>
+      <c r="O37" s="17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="12:15" ht="24.75" customHeight="1">
       <c r="L38" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="M38" s="19" t="s">
-        <v>374</v>
+      <c r="M38" s="17" t="s">
+        <v>310</v>
       </c>
       <c r="N38" s="17">
         <v>2</v>
       </c>
-      <c r="O38" s="19" t="s">
-        <v>35</v>
+      <c r="O38" s="17" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="12:15" ht="24.75" customHeight="1">
       <c r="L39" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="M39" s="18" t="s">
-        <v>345</v>
-      </c>
-      <c r="N39" s="18">
-        <v>1</v>
-      </c>
-      <c r="O39" s="19" t="s">
-        <v>311</v>
+      <c r="M39" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="N39" s="17">
+        <v>2</v>
+      </c>
+      <c r="O39" s="17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="12:15" ht="24.75" customHeight="1">
@@ -6383,13 +6104,13 @@
         <v>133</v>
       </c>
       <c r="M40" s="18" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="N40" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O40" s="19" t="s">
-        <v>311</v>
+        <v>360</v>
       </c>
     </row>
     <row r="41" spans="12:15" ht="24.75" customHeight="1">
@@ -6397,55 +6118,55 @@
         <v>134</v>
       </c>
       <c r="M41" s="18" t="s">
-        <v>178</v>
+        <v>315</v>
       </c>
       <c r="N41" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O41" s="19" t="s">
-        <v>360</v>
+        <v>311</v>
       </c>
     </row>
     <row r="42" spans="12:15" ht="24.75" customHeight="1">
       <c r="L42" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="M42" s="18" t="s">
-        <v>342</v>
-      </c>
-      <c r="N42" s="18">
-        <v>1</v>
-      </c>
-      <c r="O42" s="19" t="s">
-        <v>360</v>
+      <c r="M42" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="N42" s="17">
+        <v>2</v>
+      </c>
+      <c r="O42" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="12:15" ht="24.75" customHeight="1">
       <c r="L43" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="M43" s="18" t="s">
-        <v>340</v>
-      </c>
-      <c r="N43" s="18">
-        <v>1</v>
+      <c r="M43" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="N43" s="17">
+        <v>2</v>
       </c>
       <c r="O43" s="19" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="12:15" ht="24.75" customHeight="1">
       <c r="L44" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="M44" s="18" t="s">
-        <v>339</v>
-      </c>
-      <c r="N44" s="18">
-        <v>1</v>
+      <c r="M44" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="N44" s="17">
+        <v>2</v>
       </c>
       <c r="O44" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="45" spans="12:15" ht="24.75" customHeight="1">
@@ -6453,40 +6174,40 @@
         <v>138</v>
       </c>
       <c r="M45" s="17" t="s">
-        <v>63</v>
+        <v>383</v>
       </c>
       <c r="N45" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O45" s="19" t="s">
-        <v>36</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46" spans="12:15" ht="24.75" customHeight="1">
       <c r="L46" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="M46" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="N46" s="17">
-        <v>1</v>
-      </c>
-      <c r="O46" s="17" t="s">
-        <v>34</v>
+      <c r="M46" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="N46" s="18">
+        <v>1</v>
+      </c>
+      <c r="O46" s="19" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="47" spans="12:15" ht="24.75" customHeight="1">
       <c r="L47" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="M47" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="N47" s="17">
-        <v>1</v>
-      </c>
-      <c r="O47" s="17" t="s">
+      <c r="M47" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="N47" s="18">
+        <v>1</v>
+      </c>
+      <c r="O47" s="19" t="s">
         <v>311</v>
       </c>
     </row>
@@ -6494,56 +6215,56 @@
       <c r="L48" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="M48" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="N48" s="17">
-        <v>1</v>
-      </c>
-      <c r="O48" s="17" t="s">
-        <v>36</v>
+      <c r="M48" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="N48" s="18">
+        <v>1</v>
+      </c>
+      <c r="O48" s="19" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="49" spans="12:15" ht="24.75" customHeight="1">
       <c r="L49" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="M49" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="N49" s="17">
-        <v>1</v>
-      </c>
-      <c r="O49" s="17" t="s">
-        <v>312</v>
+      <c r="M49" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="N49" s="18">
+        <v>1</v>
+      </c>
+      <c r="O49" s="19" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="50" spans="12:15" ht="24.75" customHeight="1">
       <c r="L50" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="M50" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="N50" s="17">
-        <v>1</v>
-      </c>
-      <c r="O50" s="17" t="s">
-        <v>360</v>
+      <c r="M50" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="N50" s="18">
+        <v>1</v>
+      </c>
+      <c r="O50" s="19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="12:15" ht="24.75" customHeight="1">
       <c r="L51" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="M51" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="N51" s="17">
-        <v>1</v>
-      </c>
-      <c r="O51" s="17" t="s">
-        <v>84</v>
+      <c r="M51" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="N51" s="18">
+        <v>1</v>
+      </c>
+      <c r="O51" s="19" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="52" spans="12:15" ht="24.75" customHeight="1">
@@ -6551,13 +6272,13 @@
         <v>145</v>
       </c>
       <c r="M52" s="17" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="N52" s="17">
         <v>1</v>
       </c>
-      <c r="O52" s="17" t="s">
-        <v>360</v>
+      <c r="O52" s="19" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="12:15" ht="24.75" customHeight="1">
@@ -6565,13 +6286,13 @@
         <v>146</v>
       </c>
       <c r="M53" s="17" t="s">
-        <v>172</v>
+        <v>65</v>
       </c>
       <c r="N53" s="17">
         <v>1</v>
       </c>
       <c r="O53" s="17" t="s">
-        <v>360</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="12:15" ht="24.75" customHeight="1">
@@ -6579,13 +6300,13 @@
         <v>147</v>
       </c>
       <c r="M54" s="17" t="s">
-        <v>174</v>
+        <v>67</v>
       </c>
       <c r="N54" s="17">
         <v>1</v>
       </c>
       <c r="O54" s="17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="12:15" ht="24.75" customHeight="1">
@@ -6593,13 +6314,13 @@
         <v>148</v>
       </c>
       <c r="M55" s="17" t="s">
-        <v>175</v>
+        <v>53</v>
       </c>
       <c r="N55" s="17">
         <v>1</v>
       </c>
       <c r="O55" s="17" t="s">
-        <v>36</v>
+        <v>312</v>
       </c>
     </row>
     <row r="56" spans="12:15" ht="24.75" customHeight="1">
@@ -6607,13 +6328,13 @@
         <v>149</v>
       </c>
       <c r="M56" s="17" t="s">
-        <v>176</v>
+        <v>68</v>
       </c>
       <c r="N56" s="17">
         <v>1</v>
       </c>
       <c r="O56" s="17" t="s">
-        <v>35</v>
+        <v>360</v>
       </c>
     </row>
     <row r="57" spans="12:15" ht="24.75" customHeight="1">
@@ -6621,13 +6342,13 @@
         <v>150</v>
       </c>
       <c r="M57" s="17" t="s">
-        <v>58</v>
+        <v>170</v>
       </c>
       <c r="N57" s="17">
         <v>1</v>
       </c>
       <c r="O57" s="17" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="12:15" ht="24.75" customHeight="1">
@@ -6635,111 +6356,111 @@
         <v>151</v>
       </c>
       <c r="M58" s="17" t="s">
-        <v>177</v>
+        <v>42</v>
       </c>
       <c r="N58" s="17">
         <v>1</v>
       </c>
       <c r="O58" s="17" t="s">
-        <v>35</v>
+        <v>360</v>
       </c>
     </row>
     <row r="59" spans="12:15" ht="24.75" customHeight="1">
       <c r="L59" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="M59" s="19" t="s">
-        <v>322</v>
+      <c r="M59" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="N59" s="17">
         <v>1</v>
       </c>
       <c r="O59" s="17" t="s">
-        <v>118</v>
+        <v>360</v>
       </c>
     </row>
     <row r="60" spans="12:15" ht="24.75" customHeight="1">
       <c r="L60" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="M60" s="19" t="s">
-        <v>323</v>
+      <c r="M60" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="N60" s="17">
         <v>1</v>
       </c>
       <c r="O60" s="17" t="s">
-        <v>118</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="12:15" ht="24.75" customHeight="1">
       <c r="L61" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="M61" s="19" t="s">
-        <v>324</v>
+      <c r="M61" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="N61" s="17">
         <v>1</v>
       </c>
-      <c r="O61" s="19" t="s">
-        <v>360</v>
+      <c r="O61" s="17" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="12:15" ht="24.75" customHeight="1">
       <c r="L62" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="M62" s="19" t="s">
-        <v>325</v>
+      <c r="M62" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="N62" s="17">
         <v>1</v>
       </c>
       <c r="O62" s="17" t="s">
-        <v>118</v>
+        <v>35</v>
       </c>
     </row>
     <row r="63" spans="12:15" ht="24.75" customHeight="1">
       <c r="L63" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="M63" s="17" t="s">
-        <v>348</v>
+      <c r="M63" s="19" t="s">
+        <v>322</v>
       </c>
       <c r="N63" s="17">
         <v>1</v>
       </c>
       <c r="O63" s="17" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="12:15" ht="24.75" customHeight="1">
       <c r="L64" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="M64" s="17" t="s">
-        <v>349</v>
+      <c r="M64" s="19" t="s">
+        <v>323</v>
       </c>
       <c r="N64" s="17">
         <v>1</v>
       </c>
       <c r="O64" s="17" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="12:15" ht="24.75" customHeight="1">
       <c r="L65" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="M65" s="17" t="s">
-        <v>350</v>
+      <c r="M65" s="19" t="s">
+        <v>324</v>
       </c>
       <c r="N65" s="17">
         <v>1</v>
       </c>
-      <c r="O65" s="17" t="s">
-        <v>84</v>
+      <c r="O65" s="19" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="66" spans="12:15" ht="24.75" customHeight="1">
@@ -6747,26 +6468,26 @@
         <v>160</v>
       </c>
       <c r="M66" s="19" t="s">
-        <v>355</v>
+        <v>325</v>
       </c>
       <c r="N66" s="17">
         <v>1</v>
       </c>
       <c r="O66" s="17" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="12:15" ht="24.75" customHeight="1">
       <c r="L67" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="M67" s="19" t="s">
-        <v>351</v>
+      <c r="M67" s="17" t="s">
+        <v>348</v>
       </c>
       <c r="N67" s="17">
         <v>1</v>
       </c>
-      <c r="O67" s="19" t="s">
+      <c r="O67" s="17" t="s">
         <v>84</v>
       </c>
     </row>
@@ -6774,27 +6495,27 @@
       <c r="L68" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="M68" s="19" t="s">
-        <v>356</v>
+      <c r="M68" s="17" t="s">
+        <v>349</v>
       </c>
       <c r="N68" s="17">
         <v>1</v>
       </c>
-      <c r="O68" s="19" t="s">
-        <v>360</v>
+      <c r="O68" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="69" spans="12:15" ht="24.75" customHeight="1">
       <c r="L69" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="M69" s="19" t="s">
-        <v>308</v>
+      <c r="M69" s="17" t="s">
+        <v>350</v>
       </c>
       <c r="N69" s="17">
         <v>1</v>
       </c>
-      <c r="O69" s="19" t="s">
+      <c r="O69" s="17" t="s">
         <v>84</v>
       </c>
     </row>
@@ -6803,13 +6524,13 @@
         <v>164</v>
       </c>
       <c r="M70" s="19" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="N70" s="17">
         <v>1</v>
       </c>
       <c r="O70" s="19" t="s">
-        <v>360</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="12:15" ht="24.75" customHeight="1">
@@ -6817,27 +6538,27 @@
         <v>165</v>
       </c>
       <c r="M71" s="19" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
       <c r="N71" s="17">
         <v>1</v>
       </c>
       <c r="O71" s="19" t="s">
-        <v>118</v>
+        <v>360</v>
       </c>
     </row>
     <row r="72" spans="12:15" ht="24.75" customHeight="1">
       <c r="L72" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="M72" s="17" t="s">
-        <v>376</v>
+      <c r="M72" s="19" t="s">
+        <v>308</v>
       </c>
       <c r="N72" s="17">
         <v>1</v>
       </c>
       <c r="O72" s="19" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
     </row>
     <row r="73" spans="12:15" ht="24.75" customHeight="1">
@@ -6845,13 +6566,13 @@
         <v>167</v>
       </c>
       <c r="M73" s="19" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
       <c r="N73" s="17">
         <v>1</v>
       </c>
       <c r="O73" s="19" t="s">
-        <v>35</v>
+        <v>360</v>
       </c>
     </row>
     <row r="74" spans="12:15" ht="24.75" customHeight="1">
@@ -6859,7 +6580,7 @@
         <v>168</v>
       </c>
       <c r="M74" s="19" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="N74" s="17">
         <v>1</v>
@@ -6872,14 +6593,14 @@
       <c r="L75" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="M75" s="19" t="s">
-        <v>379</v>
+      <c r="M75" s="17" t="s">
+        <v>375</v>
       </c>
       <c r="N75" s="17">
         <v>1</v>
       </c>
       <c r="O75" s="19" t="s">
-        <v>312</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="12:15" ht="24.75" customHeight="1">
@@ -6887,13 +6608,13 @@
         <v>180</v>
       </c>
       <c r="M76" s="19" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="N76" s="17">
         <v>1</v>
       </c>
       <c r="O76" s="19" t="s">
-        <v>312</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77" spans="12:15" ht="24.75" customHeight="1">
@@ -6901,7 +6622,7 @@
         <v>181</v>
       </c>
       <c r="M77" s="19" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="N77" s="17">
         <v>1</v>
@@ -6915,13 +6636,13 @@
         <v>182</v>
       </c>
       <c r="M78" s="19" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="N78" s="17">
         <v>1</v>
       </c>
       <c r="O78" s="19" t="s">
-        <v>312</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="12:15" ht="24.75" customHeight="1">
@@ -6929,54 +6650,75 @@
         <v>183</v>
       </c>
       <c r="M79" s="19" t="s">
-        <v>337</v>
+        <v>380</v>
       </c>
       <c r="N79" s="17">
         <v>1</v>
       </c>
       <c r="O79" s="19" t="s">
-        <v>34</v>
+        <v>312</v>
       </c>
     </row>
     <row r="80" spans="12:15" ht="24.75" customHeight="1">
       <c r="L80" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="M80" s="17"/>
-      <c r="N80" s="17"/>
-      <c r="O80" s="19"/>
+      <c r="M80" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="N80" s="17">
+        <v>1</v>
+      </c>
+      <c r="O80" s="19" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="81" spans="12:15" ht="24.95" customHeight="1">
       <c r="L81" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="19"/>
+      <c r="M81" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="N81" s="17">
+        <v>1</v>
+      </c>
+      <c r="O81" s="19" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="82" spans="12:15" ht="24.95" customHeight="1">
       <c r="L82" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="M82" s="17"/>
-      <c r="N82" s="17"/>
-      <c r="O82" s="19"/>
+      <c r="M82" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="N82" s="17">
+        <v>1</v>
+      </c>
+      <c r="O82" s="19" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="83" spans="12:15" ht="24.95" customHeight="1">
       <c r="L83" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="M83" s="17"/>
-      <c r="N83" s="17"/>
-      <c r="O83" s="19"/>
+      <c r="M83" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="N83" s="17">
+        <v>1</v>
+      </c>
+      <c r="O83" s="19" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="84" spans="12:15" ht="24.95" customHeight="1">
       <c r="L84" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="M84" s="17"/>
-      <c r="N84" s="17"/>
-      <c r="O84" s="19"/>
     </row>
     <row r="85" spans="12:15" ht="24.95" customHeight="1">
       <c r="L85" s="17" t="s">
@@ -7011,42 +6753,41 @@
       <c r="O88" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="L2:O88"/>
-  <sortState ref="M3:O79">
-    <sortCondition descending="1" ref="N3:N79"/>
+  <sortState ref="M3:O84">
+    <sortCondition descending="1" ref="N3:N84"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="L1:O1"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="L3:O88">
-    <cfRule type="expression" dxfId="26" priority="1">
+  <conditionalFormatting sqref="L3:O62 L85:O88 L63:L84 M63:O83">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$O3="Sporting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$O3="Real Madrid"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$O3="Manchester City"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>$O3="Bayern Munique"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$O3="Bayer Leverkusen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>$O3="Internazionale"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>$O3="Arsenal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>$O3="Barcelona"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="O3:O88">
+    <dataValidation type="list" allowBlank="1" sqref="O85:O88 O3:O83" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Internazionale,Arsenal,Barcelona,Manchester City,Juventus,Bayern Munique,Bayer Leverkusen,Real Madrid"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7056,11 +6797,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:S92"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O72" sqref="O72:R75"/>
+    <sheetView topLeftCell="A83" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O84" sqref="O84:R87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9579,6 +9320,297 @@
       </c>
       <c r="R80" s="43"/>
     </row>
+    <row r="84" spans="1:18" ht="30" customHeight="1">
+      <c r="A84" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H84" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="K84" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="L84" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="M84" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="O84" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="P84" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q84" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="R84" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" ht="30" customHeight="1">
+      <c r="A85" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="B85" s="11">
+        <v>4</v>
+      </c>
+      <c r="C85" s="11">
+        <v>3</v>
+      </c>
+      <c r="D85" s="11">
+        <v>1</v>
+      </c>
+      <c r="E85" s="11">
+        <v>0</v>
+      </c>
+      <c r="F85" s="11">
+        <v>10</v>
+      </c>
+      <c r="G85" s="11">
+        <v>4</v>
+      </c>
+      <c r="H85" s="11">
+        <v>10</v>
+      </c>
+      <c r="K85" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="L85" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="M85" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="O85" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="P85" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q85" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="R85" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" ht="30" customHeight="1">
+      <c r="A86" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="B86" s="11">
+        <v>4</v>
+      </c>
+      <c r="C86" s="11">
+        <v>3</v>
+      </c>
+      <c r="D86" s="11">
+        <v>0</v>
+      </c>
+      <c r="E86" s="11">
+        <v>1</v>
+      </c>
+      <c r="F86" s="11">
+        <v>10</v>
+      </c>
+      <c r="G86" s="11">
+        <v>8</v>
+      </c>
+      <c r="H86" s="11">
+        <v>9</v>
+      </c>
+      <c r="K86" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="L86" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="M86" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="O86" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="P86" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q86" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="R86" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" ht="30" customHeight="1">
+      <c r="A87" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B87" s="11">
+        <v>4</v>
+      </c>
+      <c r="C87" s="11">
+        <v>1</v>
+      </c>
+      <c r="D87" s="11">
+        <v>1</v>
+      </c>
+      <c r="E87" s="11">
+        <v>2</v>
+      </c>
+      <c r="F87" s="11">
+        <v>8</v>
+      </c>
+      <c r="G87" s="11">
+        <v>7</v>
+      </c>
+      <c r="H87" s="11">
+        <v>4</v>
+      </c>
+      <c r="K87" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L87" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="M87" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O87" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="P87" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q87" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="R87" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" ht="30" customHeight="1">
+      <c r="A88" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="B88" s="11">
+        <v>4</v>
+      </c>
+      <c r="C88" s="11">
+        <v>0</v>
+      </c>
+      <c r="D88" s="11">
+        <v>3</v>
+      </c>
+      <c r="E88" s="11">
+        <v>1</v>
+      </c>
+      <c r="F88" s="11">
+        <v>3</v>
+      </c>
+      <c r="G88" s="11">
+        <v>6</v>
+      </c>
+      <c r="H88" s="11">
+        <v>3</v>
+      </c>
+      <c r="K88" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L88" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="M88" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" ht="30" customHeight="1">
+      <c r="A89" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B89" s="15">
+        <v>4</v>
+      </c>
+      <c r="C89" s="15">
+        <v>0</v>
+      </c>
+      <c r="D89" s="15">
+        <v>1</v>
+      </c>
+      <c r="E89" s="15">
+        <v>3</v>
+      </c>
+      <c r="F89" s="15">
+        <v>5</v>
+      </c>
+      <c r="G89" s="15">
+        <v>11</v>
+      </c>
+      <c r="H89" s="15">
+        <v>1</v>
+      </c>
+      <c r="K89" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="L89" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="M89" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" ht="30" customHeight="1">
+      <c r="K90" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="L90" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="M90" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" ht="30" customHeight="1">
+      <c r="K91" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L91" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="M91" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" ht="30" customHeight="1">
+      <c r="K92" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L92" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="M92" s="10" t="s">
+        <v>360</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9586,11 +9618,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="69" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="69" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9616,34 +9648,34 @@
       <c r="E1" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="49"/>
+      <c r="G1" s="50"/>
       <c r="H1" s="34" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1">
       <c r="A2" s="35">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B2" s="35">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2" s="35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="35">
         <v>9</v>
       </c>
       <c r="E2" s="35">
-        <v>28</v>
-      </c>
-      <c r="F2" s="50">
-        <v>28</v>
-      </c>
-      <c r="G2" s="50"/>
+        <v>42</v>
+      </c>
+      <c r="F2" s="51">
+        <v>33</v>
+      </c>
+      <c r="G2" s="51"/>
       <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1">
@@ -9672,34 +9704,34 @@
       <c r="E4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="42" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="24" customHeight="1">
       <c r="A5" s="23">
+        <v>32</v>
+      </c>
+      <c r="B5" s="23">
+        <v>11</v>
+      </c>
+      <c r="C5" s="23">
+        <v>10</v>
+      </c>
+      <c r="D5" s="23">
+        <v>11</v>
+      </c>
+      <c r="E5" s="23">
+        <v>28</v>
+      </c>
+      <c r="F5" s="53">
         <v>26</v>
       </c>
-      <c r="B5" s="23">
-        <v>9</v>
-      </c>
-      <c r="C5" s="23">
-        <v>9</v>
-      </c>
-      <c r="D5" s="23">
-        <v>8</v>
-      </c>
-      <c r="E5" s="23">
-        <v>27</v>
-      </c>
-      <c r="F5" s="52">
-        <v>17</v>
-      </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="53"/>
       <c r="H5" s="45"/>
     </row>
     <row r="6" spans="1:8" ht="24" customHeight="1">
@@ -9728,34 +9760,34 @@
       <c r="E7" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="53"/>
+      <c r="G7" s="54"/>
       <c r="H7" s="38" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="24" customHeight="1">
       <c r="A8" s="39">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B8" s="39">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C8" s="39">
         <v>4</v>
       </c>
       <c r="D8" s="39">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E8" s="39">
-        <v>61</v>
-      </c>
-      <c r="F8" s="48">
-        <v>33</v>
-      </c>
-      <c r="G8" s="48"/>
+        <v>74</v>
+      </c>
+      <c r="F8" s="49">
+        <v>44</v>
+      </c>
+      <c r="G8" s="49"/>
       <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" ht="24" customHeight="1">
@@ -9784,10 +9816,10 @@
       <c r="E10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="54" t="s">
+      <c r="F10" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="54"/>
+      <c r="G10" s="55"/>
       <c r="H10" s="5" t="s">
         <v>36</v>
       </c>
@@ -9808,10 +9840,10 @@
       <c r="E11" s="24">
         <v>19</v>
       </c>
-      <c r="F11" s="55">
+      <c r="F11" s="56">
         <v>36</v>
       </c>
-      <c r="G11" s="55"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" ht="24" customHeight="1">
@@ -9825,49 +9857,49 @@
       <c r="H12" s="32"/>
     </row>
     <row r="13" spans="1:8" ht="24" customHeight="1">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="63" t="s">
+      <c r="E13" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="64" t="s">
+      <c r="F13" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="64"/>
-      <c r="H13" s="63" t="s">
+      <c r="G13" s="57"/>
+      <c r="H13" s="46" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="24" customHeight="1">
       <c r="A14" s="36">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B14" s="36">
         <v>9</v>
       </c>
       <c r="C14" s="36">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D14" s="36">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E14" s="36">
-        <v>29</v>
-      </c>
-      <c r="F14" s="56">
-        <v>35</v>
-      </c>
-      <c r="G14" s="56"/>
+        <v>34</v>
+      </c>
+      <c r="F14" s="58">
+        <v>46</v>
+      </c>
+      <c r="G14" s="58"/>
       <c r="H14" s="37"/>
     </row>
     <row r="15" spans="1:8" ht="24" customHeight="1">
@@ -9896,10 +9928,10 @@
       <c r="E16" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="57" t="s">
+      <c r="F16" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="57"/>
+      <c r="G16" s="59"/>
       <c r="H16" s="6" t="s">
         <v>103</v>
       </c>
@@ -9920,10 +9952,10 @@
       <c r="E17" s="25">
         <v>15</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="60">
         <v>21</v>
       </c>
-      <c r="G17" s="58"/>
+      <c r="G17" s="60"/>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:11" ht="24" customHeight="1">
@@ -9952,10 +9984,10 @@
       <c r="E19" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="59" t="s">
+      <c r="F19" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="59"/>
+      <c r="G19" s="61"/>
       <c r="H19" s="26" t="s">
         <v>104</v>
       </c>
@@ -9976,10 +10008,10 @@
       <c r="E20" s="27">
         <v>7</v>
       </c>
-      <c r="F20" s="60">
+      <c r="F20" s="62">
         <v>3</v>
       </c>
-      <c r="G20" s="60"/>
+      <c r="G20" s="62"/>
       <c r="H20" s="32"/>
     </row>
     <row r="21" spans="1:11" ht="24" customHeight="1">
@@ -10008,34 +10040,34 @@
       <c r="E22" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="61" t="s">
+      <c r="F22" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="61"/>
+      <c r="G22" s="63"/>
       <c r="H22" s="28" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="24" customHeight="1">
       <c r="A23" s="29">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B23" s="29">
         <v>10</v>
       </c>
       <c r="C23" s="29">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D23" s="29">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E23" s="29">
-        <v>29</v>
-      </c>
-      <c r="F23" s="62">
         <v>34</v>
       </c>
-      <c r="G23" s="62"/>
+      <c r="F23" s="64">
+        <v>45</v>
+      </c>
+      <c r="G23" s="64"/>
       <c r="H23" s="32"/>
     </row>
     <row r="24" spans="1:11">

</xml_diff>